<commit_message>
screened 200 out of 1000 predicted "excludes" input into Colandr - full text showed no matches
</commit_message>
<xml_diff>
--- a/_data/screened_fulltext/ft_consolidated_coding.xlsx
+++ b/_data/screened_fulltext/ft_consolidated_coding.xlsx
@@ -16,7 +16,7 @@
     <sheet name="lists" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">ft_consolidated_revisit!$A$1:$O$208</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">ft_consolidated_revisit!$A$1:$W$208</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
 </workbook>
@@ -3452,10 +3452,10 @@
   <dimension ref="A1:W208"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="G5" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="J186" sqref="J186"/>
+      <selection pane="bottomRight" activeCell="A195" sqref="A195:D195"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3607,64 +3607,58 @@
     </row>
     <row r="5" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>204</v>
+        <v>115</v>
       </c>
       <c r="B5" t="s">
-        <v>205</v>
+        <v>116</v>
       </c>
       <c r="C5">
-        <v>2020</v>
+        <v>1997</v>
       </c>
       <c r="D5" t="s">
-        <v>206</v>
+        <v>624</v>
       </c>
       <c r="E5" t="s">
-        <v>207</v>
+        <v>8</v>
       </c>
       <c r="F5">
-        <v>0.99784111842534284</v>
-      </c>
-      <c r="G5" t="s">
-        <v>606</v>
+        <v>0.95081877406880044</v>
       </c>
       <c r="H5" t="s">
-        <v>568</v>
+        <v>558</v>
       </c>
       <c r="J5" t="s">
-        <v>737</v>
+        <v>748</v>
       </c>
       <c r="K5" t="s">
-        <v>602</v>
+        <v>604</v>
       </c>
       <c r="M5" t="s">
-        <v>602</v>
+        <v>604</v>
       </c>
       <c r="O5" t="s">
-        <v>603</v>
-      </c>
-      <c r="P5" t="s">
-        <v>723</v>
+        <v>605</v>
       </c>
       <c r="Q5" t="s">
-        <v>721</v>
+        <v>740</v>
       </c>
       <c r="R5" t="s">
-        <v>722</v>
+        <v>747</v>
       </c>
       <c r="S5" t="s">
-        <v>729</v>
+        <v>750</v>
       </c>
       <c r="T5" t="s">
-        <v>724</v>
+        <v>749</v>
       </c>
       <c r="U5" t="s">
-        <v>728</v>
+        <v>745</v>
       </c>
       <c r="V5" t="s">
-        <v>727</v>
+        <v>751</v>
       </c>
       <c r="W5" t="s">
-        <v>726</v>
+        <v>7</v>
       </c>
     </row>
     <row r="6" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
@@ -3729,58 +3723,70 @@
     </row>
     <row r="9" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>226</v>
+        <v>19</v>
       </c>
       <c r="B9" t="s">
-        <v>227</v>
+        <v>20</v>
       </c>
       <c r="C9">
-        <v>2018</v>
+        <v>2009</v>
       </c>
       <c r="D9" t="s">
-        <v>228</v>
+        <v>627</v>
       </c>
       <c r="E9" t="s">
-        <v>229</v>
+        <v>8</v>
       </c>
       <c r="F9">
-        <v>0.99247800970533862</v>
+        <v>0.98913501268963322</v>
+      </c>
+      <c r="G9" t="s">
+        <v>607</v>
       </c>
       <c r="H9" t="s">
+        <v>558</v>
+      </c>
+      <c r="I9" t="s">
         <v>567</v>
       </c>
       <c r="J9" t="s">
-        <v>738</v>
+        <v>759</v>
       </c>
       <c r="K9" t="s">
-        <v>602</v>
+        <v>550</v>
+      </c>
+      <c r="L9" t="s">
+        <v>556</v>
       </c>
       <c r="M9" t="s">
-        <v>544</v>
+        <v>550</v>
+      </c>
+      <c r="N9" t="s">
+        <v>549</v>
       </c>
       <c r="P9" t="s">
-        <v>732</v>
+        <v>760</v>
       </c>
       <c r="Q9" t="s">
-        <v>730</v>
+        <v>756</v>
       </c>
       <c r="R9" t="s">
-        <v>731</v>
+        <v>757</v>
       </c>
       <c r="S9" t="s">
-        <v>736</v>
+        <v>758</v>
       </c>
       <c r="T9" t="s">
-        <v>733</v>
+        <v>717</v>
       </c>
       <c r="U9" t="s">
-        <v>761</v>
+        <v>745</v>
       </c>
       <c r="V9" t="s">
-        <v>735</v>
+        <v>762</v>
       </c>
       <c r="W9" t="s">
-        <v>734</v>
+        <v>763</v>
       </c>
     </row>
     <row r="10" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
@@ -3925,67 +3931,52 @@
     </row>
     <row r="17" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>236</v>
+        <v>327</v>
       </c>
       <c r="B17" t="s">
-        <v>237</v>
+        <v>328</v>
       </c>
       <c r="C17">
-        <v>2017</v>
+        <v>2022</v>
       </c>
       <c r="D17" t="s">
-        <v>238</v>
+        <v>329</v>
       </c>
       <c r="E17" t="s">
-        <v>229</v>
+        <v>326</v>
       </c>
       <c r="F17">
-        <v>0.91594384348707403</v>
-      </c>
-      <c r="G17" t="s">
-        <v>601</v>
+        <v>0.92724577416628151</v>
       </c>
       <c r="H17" t="s">
-        <v>559</v>
-      </c>
-      <c r="I17" t="s">
-        <v>600</v>
+        <v>560</v>
       </c>
       <c r="J17" t="s">
-        <v>739</v>
+        <v>752</v>
       </c>
       <c r="K17" t="s">
-        <v>550</v>
-      </c>
-      <c r="L17" t="s">
-        <v>554</v>
+        <v>604</v>
       </c>
       <c r="M17" t="s">
-        <v>550</v>
-      </c>
-      <c r="N17" t="s">
-        <v>548</v>
+        <v>604</v>
       </c>
       <c r="P17" t="s">
-        <v>743</v>
+        <v>753</v>
       </c>
       <c r="Q17" t="s">
-        <v>740</v>
-      </c>
-      <c r="R17" t="s">
-        <v>741</v>
+        <v>754</v>
       </c>
       <c r="S17" t="s">
-        <v>742</v>
+        <v>755</v>
       </c>
       <c r="T17" t="s">
-        <v>744</v>
+        <v>45</v>
       </c>
       <c r="U17" t="s">
         <v>745</v>
       </c>
       <c r="V17" t="s">
-        <v>746</v>
+        <v>45</v>
       </c>
       <c r="W17" t="s">
         <v>7</v>
@@ -4093,28 +4084,28 @@
     </row>
     <row r="23" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>115</v>
+        <v>131</v>
       </c>
       <c r="B23" t="s">
-        <v>116</v>
+        <v>132</v>
       </c>
       <c r="C23">
-        <v>1997</v>
+        <v>2004</v>
       </c>
       <c r="D23" t="s">
-        <v>624</v>
+        <v>653</v>
       </c>
       <c r="E23" t="s">
         <v>8</v>
       </c>
       <c r="F23">
-        <v>0.95081877406880044</v>
+        <v>0.97897668902420254</v>
       </c>
       <c r="H23" t="s">
-        <v>558</v>
+        <v>560</v>
       </c>
       <c r="J23" t="s">
-        <v>748</v>
+        <v>787</v>
       </c>
       <c r="K23" t="s">
         <v>604</v>
@@ -4123,25 +4114,25 @@
         <v>604</v>
       </c>
       <c r="O23" t="s">
-        <v>605</v>
+        <v>788</v>
+      </c>
+      <c r="P23" t="s">
+        <v>790</v>
       </c>
       <c r="Q23" t="s">
         <v>740</v>
       </c>
-      <c r="R23" t="s">
-        <v>747</v>
-      </c>
       <c r="S23" t="s">
-        <v>750</v>
+        <v>789</v>
       </c>
       <c r="T23" t="s">
-        <v>749</v>
+        <v>791</v>
       </c>
       <c r="U23" t="s">
         <v>745</v>
       </c>
       <c r="V23" t="s">
-        <v>751</v>
+        <v>792</v>
       </c>
       <c r="W23" t="s">
         <v>7</v>
@@ -4238,55 +4229,55 @@
     </row>
     <row r="28" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>327</v>
+        <v>308</v>
       </c>
       <c r="B28" t="s">
-        <v>328</v>
+        <v>309</v>
       </c>
       <c r="C28">
-        <v>2022</v>
+        <v>2015</v>
       </c>
       <c r="D28" t="s">
-        <v>329</v>
+        <v>310</v>
       </c>
       <c r="E28" t="s">
-        <v>326</v>
+        <v>229</v>
       </c>
       <c r="F28">
-        <v>0.92724577416628151</v>
+        <v>0.90633376228548657</v>
+      </c>
+      <c r="G28" t="s">
+        <v>613</v>
       </c>
       <c r="H28" t="s">
         <v>560</v>
       </c>
-      <c r="J28" t="s">
-        <v>752</v>
-      </c>
       <c r="K28" t="s">
-        <v>604</v>
+        <v>602</v>
       </c>
       <c r="M28" t="s">
-        <v>604</v>
+        <v>544</v>
       </c>
       <c r="P28" t="s">
-        <v>753</v>
+        <v>852</v>
       </c>
       <c r="Q28" t="s">
-        <v>754</v>
+        <v>855</v>
+      </c>
+      <c r="R28" t="s">
+        <v>853</v>
       </c>
       <c r="S28" t="s">
-        <v>755</v>
+        <v>854</v>
       </c>
       <c r="T28" t="s">
-        <v>45</v>
+        <v>856</v>
       </c>
       <c r="U28" t="s">
-        <v>745</v>
+        <v>857</v>
       </c>
       <c r="V28" t="s">
-        <v>45</v>
-      </c>
-      <c r="W28" t="s">
-        <v>7</v>
+        <v>858</v>
       </c>
     </row>
     <row r="29" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
@@ -4311,70 +4302,52 @@
     </row>
     <row r="30" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>19</v>
+        <v>192</v>
       </c>
       <c r="B30" t="s">
-        <v>20</v>
+        <v>193</v>
       </c>
       <c r="C30">
-        <v>2009</v>
+        <v>2020</v>
       </c>
       <c r="D30" t="s">
-        <v>627</v>
+        <v>685</v>
       </c>
       <c r="E30" t="s">
-        <v>8</v>
+        <v>179</v>
       </c>
       <c r="F30">
-        <v>0.98913501268963322</v>
-      </c>
-      <c r="G30" t="s">
-        <v>607</v>
+        <v>0.99350047019181054</v>
       </c>
       <c r="H30" t="s">
-        <v>558</v>
-      </c>
-      <c r="I30" t="s">
-        <v>567</v>
-      </c>
-      <c r="J30" t="s">
-        <v>759</v>
+        <v>581</v>
       </c>
       <c r="K30" t="s">
-        <v>550</v>
-      </c>
-      <c r="L30" t="s">
-        <v>556</v>
+        <v>604</v>
       </c>
       <c r="M30" t="s">
-        <v>550</v>
+        <v>544</v>
       </c>
       <c r="N30" t="s">
-        <v>549</v>
+        <v>604</v>
       </c>
       <c r="P30" t="s">
-        <v>760</v>
+        <v>837</v>
       </c>
       <c r="Q30" t="s">
-        <v>756</v>
+        <v>838</v>
       </c>
       <c r="R30" t="s">
-        <v>757</v>
-      </c>
-      <c r="S30" t="s">
-        <v>758</v>
+        <v>839</v>
       </c>
       <c r="T30" t="s">
-        <v>717</v>
+        <v>840</v>
       </c>
       <c r="U30" t="s">
-        <v>745</v>
+        <v>728</v>
       </c>
       <c r="V30" t="s">
-        <v>762</v>
-      </c>
-      <c r="W30" t="s">
-        <v>763</v>
+        <v>841</v>
       </c>
     </row>
     <row r="31" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
@@ -4539,58 +4512,64 @@
     </row>
     <row r="39" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>339</v>
+        <v>204</v>
       </c>
       <c r="B39" t="s">
-        <v>340</v>
+        <v>205</v>
       </c>
       <c r="C39">
         <v>2020</v>
       </c>
       <c r="D39" t="s">
-        <v>341</v>
+        <v>206</v>
       </c>
       <c r="E39" t="s">
-        <v>326</v>
+        <v>207</v>
       </c>
       <c r="F39">
-        <v>0.92473916763464115</v>
+        <v>0.99784111842534284</v>
       </c>
       <c r="G39" t="s">
-        <v>608</v>
+        <v>606</v>
       </c>
       <c r="H39" t="s">
-        <v>573</v>
+        <v>568</v>
       </c>
       <c r="J39" t="s">
-        <v>766</v>
+        <v>737</v>
       </c>
       <c r="K39" t="s">
         <v>602</v>
       </c>
       <c r="M39" t="s">
-        <v>544</v>
+        <v>602</v>
+      </c>
+      <c r="O39" t="s">
+        <v>603</v>
       </c>
       <c r="P39" t="s">
-        <v>764</v>
+        <v>723</v>
       </c>
       <c r="Q39" t="s">
-        <v>765</v>
+        <v>721</v>
+      </c>
+      <c r="R39" t="s">
+        <v>722</v>
       </c>
       <c r="S39" t="s">
-        <v>768</v>
+        <v>729</v>
       </c>
       <c r="T39" t="s">
-        <v>769</v>
+        <v>724</v>
       </c>
       <c r="U39" t="s">
-        <v>745</v>
+        <v>728</v>
       </c>
       <c r="V39" t="s">
-        <v>770</v>
+        <v>727</v>
       </c>
       <c r="W39" t="s">
-        <v>767</v>
+        <v>726</v>
       </c>
     </row>
     <row r="40" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
@@ -5155,55 +5134,58 @@
     </row>
     <row r="68" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>454</v>
+        <v>339</v>
       </c>
       <c r="B68" t="s">
-        <v>455</v>
+        <v>340</v>
       </c>
       <c r="C68">
-        <v>2009</v>
+        <v>2020</v>
       </c>
       <c r="D68" t="s">
-        <v>456</v>
+        <v>341</v>
       </c>
       <c r="E68" t="s">
-        <v>423</v>
+        <v>326</v>
       </c>
       <c r="F68">
-        <v>0.98052761532990129</v>
+        <v>0.92473916763464115</v>
+      </c>
+      <c r="G68" t="s">
+        <v>608</v>
       </c>
       <c r="H68" t="s">
-        <v>559</v>
+        <v>573</v>
       </c>
       <c r="J68" t="s">
-        <v>780</v>
+        <v>766</v>
       </c>
       <c r="K68" t="s">
-        <v>550</v>
+        <v>602</v>
       </c>
       <c r="M68" t="s">
-        <v>550</v>
+        <v>544</v>
       </c>
       <c r="P68" t="s">
-        <v>775</v>
+        <v>764</v>
       </c>
       <c r="Q68" t="s">
-        <v>772</v>
-      </c>
-      <c r="R68" t="s">
-        <v>773</v>
+        <v>765</v>
       </c>
       <c r="S68" t="s">
-        <v>774</v>
+        <v>768</v>
       </c>
       <c r="T68" t="s">
-        <v>776</v>
+        <v>769</v>
       </c>
       <c r="U68" t="s">
         <v>745</v>
       </c>
       <c r="V68" t="s">
-        <v>771</v>
+        <v>770</v>
+      </c>
+      <c r="W68" t="s">
+        <v>767</v>
       </c>
     </row>
     <row r="69" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
@@ -5388,64 +5370,67 @@
     </row>
     <row r="78" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>175</v>
+        <v>393</v>
       </c>
       <c r="B78" t="s">
-        <v>176</v>
+        <v>394</v>
       </c>
       <c r="C78">
-        <v>1977</v>
+        <v>2023</v>
       </c>
       <c r="D78" t="s">
-        <v>651</v>
+        <v>395</v>
       </c>
       <c r="E78" t="s">
-        <v>8</v>
+        <v>326</v>
       </c>
       <c r="F78">
-        <v>0.98990510535464893</v>
+        <v>0.97458912963154121</v>
       </c>
       <c r="G78" t="s">
-        <v>609</v>
+        <v>611</v>
       </c>
       <c r="H78" t="s">
-        <v>567</v>
+        <v>573</v>
       </c>
       <c r="I78" t="s">
-        <v>559</v>
-      </c>
-      <c r="J78" t="s">
-        <v>785</v>
+        <v>577</v>
       </c>
       <c r="K78" t="s">
         <v>550</v>
       </c>
+      <c r="L78" t="s">
+        <v>557</v>
+      </c>
       <c r="M78" t="s">
         <v>550</v>
       </c>
+      <c r="N78" t="s">
+        <v>544</v>
+      </c>
       <c r="P78" t="s">
-        <v>779</v>
+        <v>831</v>
       </c>
       <c r="Q78" t="s">
-        <v>777</v>
+        <v>834</v>
       </c>
       <c r="R78" t="s">
-        <v>778</v>
+        <v>835</v>
       </c>
       <c r="S78" t="s">
-        <v>781</v>
+        <v>832</v>
       </c>
       <c r="T78" t="s">
-        <v>783</v>
+        <v>45</v>
       </c>
       <c r="U78" t="s">
-        <v>782</v>
+        <v>745</v>
       </c>
       <c r="V78" t="s">
-        <v>784</v>
+        <v>836</v>
       </c>
       <c r="W78" t="s">
-        <v>786</v>
+        <v>833</v>
       </c>
     </row>
     <row r="79" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
@@ -5530,28 +5515,28 @@
     </row>
     <row r="83" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>131</v>
+        <v>52</v>
       </c>
       <c r="B83" t="s">
-        <v>132</v>
+        <v>53</v>
       </c>
       <c r="C83">
-        <v>2004</v>
+        <v>2015</v>
       </c>
       <c r="D83" t="s">
-        <v>653</v>
+        <v>671</v>
       </c>
       <c r="E83" t="s">
         <v>8</v>
       </c>
       <c r="F83">
-        <v>0.97897668902420254</v>
+        <v>0.95050734852012941</v>
+      </c>
+      <c r="G83" t="s">
+        <v>112</v>
       </c>
       <c r="H83" t="s">
-        <v>560</v>
-      </c>
-      <c r="J83" t="s">
-        <v>787</v>
+        <v>594</v>
       </c>
       <c r="K83" t="s">
         <v>604</v>
@@ -5559,29 +5544,29 @@
       <c r="M83" t="s">
         <v>604</v>
       </c>
-      <c r="O83" t="s">
-        <v>788</v>
-      </c>
       <c r="P83" t="s">
-        <v>790</v>
+        <v>820</v>
       </c>
       <c r="Q83" t="s">
-        <v>740</v>
+        <v>826</v>
+      </c>
+      <c r="R83" t="s">
+        <v>827</v>
       </c>
       <c r="S83" t="s">
-        <v>789</v>
+        <v>821</v>
       </c>
       <c r="T83" t="s">
-        <v>791</v>
+        <v>822</v>
       </c>
       <c r="U83" t="s">
         <v>745</v>
       </c>
       <c r="V83" t="s">
-        <v>792</v>
+        <v>45</v>
       </c>
       <c r="W83" t="s">
-        <v>7</v>
+        <v>823</v>
       </c>
     </row>
     <row r="84" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
@@ -5966,55 +5951,58 @@
     </row>
     <row r="103" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>475</v>
+        <v>226</v>
       </c>
       <c r="B103" t="s">
-        <v>476</v>
+        <v>227</v>
       </c>
       <c r="C103">
-        <v>2003</v>
+        <v>2018</v>
       </c>
       <c r="D103" t="s">
-        <v>477</v>
+        <v>228</v>
       </c>
       <c r="E103" t="s">
-        <v>423</v>
+        <v>229</v>
       </c>
       <c r="F103">
-        <v>0.92120915300430206</v>
+        <v>0.99247800970533862</v>
       </c>
       <c r="H103" t="s">
         <v>567</v>
       </c>
+      <c r="J103" t="s">
+        <v>738</v>
+      </c>
       <c r="K103" t="s">
-        <v>555</v>
+        <v>602</v>
       </c>
       <c r="M103" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="P103" t="s">
-        <v>793</v>
+        <v>732</v>
       </c>
       <c r="Q103" t="s">
-        <v>772</v>
+        <v>730</v>
       </c>
       <c r="R103" t="s">
-        <v>794</v>
+        <v>731</v>
       </c>
       <c r="S103" t="s">
-        <v>795</v>
+        <v>736</v>
       </c>
       <c r="T103" t="s">
-        <v>796</v>
+        <v>733</v>
       </c>
       <c r="U103" t="s">
-        <v>745</v>
+        <v>761</v>
       </c>
       <c r="V103" t="s">
-        <v>797</v>
+        <v>735</v>
       </c>
       <c r="W103" t="s">
-        <v>7</v>
+        <v>734</v>
       </c>
     </row>
     <row r="104" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
@@ -6039,55 +6027,64 @@
     </row>
     <row r="105" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>50</v>
+        <v>175</v>
       </c>
       <c r="B105" t="s">
-        <v>51</v>
+        <v>176</v>
       </c>
       <c r="C105">
-        <v>2008</v>
+        <v>1977</v>
       </c>
       <c r="D105" t="s">
-        <v>664</v>
+        <v>651</v>
       </c>
       <c r="E105" t="s">
         <v>8</v>
       </c>
       <c r="F105">
-        <v>0.9377232202339163</v>
+        <v>0.98990510535464893</v>
+      </c>
+      <c r="G105" t="s">
+        <v>609</v>
       </c>
       <c r="H105" t="s">
+        <v>567</v>
+      </c>
+      <c r="I105" t="s">
         <v>559</v>
       </c>
+      <c r="J105" t="s">
+        <v>785</v>
+      </c>
       <c r="K105" t="s">
-        <v>546</v>
+        <v>550</v>
       </c>
       <c r="M105" t="s">
-        <v>543</v>
+        <v>550</v>
       </c>
       <c r="P105" t="s">
-        <v>798</v>
+        <v>779</v>
       </c>
       <c r="Q105" t="s">
-        <v>799</v>
+        <v>777</v>
       </c>
       <c r="R105" t="s">
-        <v>800</v>
+        <v>778</v>
       </c>
       <c r="S105" t="s">
-        <v>801</v>
+        <v>781</v>
       </c>
       <c r="T105" t="s">
-        <v>802</v>
+        <v>783</v>
       </c>
       <c r="U105" t="s">
-        <v>745</v>
+        <v>782</v>
       </c>
       <c r="V105" t="s">
-        <v>803</v>
+        <v>784</v>
       </c>
       <c r="W105" t="s">
-        <v>7</v>
+        <v>786</v>
       </c>
     </row>
     <row r="106" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
@@ -6152,58 +6149,52 @@
     </row>
     <row r="109" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
-        <v>372</v>
+        <v>475</v>
       </c>
       <c r="B109" t="s">
-        <v>373</v>
+        <v>476</v>
       </c>
       <c r="C109">
-        <v>2014</v>
+        <v>2003</v>
       </c>
       <c r="D109" t="s">
-        <v>374</v>
+        <v>477</v>
       </c>
       <c r="E109" t="s">
-        <v>326</v>
+        <v>423</v>
       </c>
       <c r="F109">
-        <v>0.94589893918682422</v>
+        <v>0.92120915300430206</v>
       </c>
       <c r="H109" t="s">
-        <v>559</v>
+        <v>567</v>
       </c>
       <c r="K109" t="s">
-        <v>550</v>
-      </c>
-      <c r="L109" t="s">
-        <v>554</v>
+        <v>555</v>
       </c>
       <c r="M109" t="s">
-        <v>550</v>
-      </c>
-      <c r="N109" t="s">
-        <v>548</v>
+        <v>545</v>
       </c>
       <c r="P109" t="s">
-        <v>804</v>
+        <v>793</v>
       </c>
       <c r="Q109" t="s">
-        <v>740</v>
+        <v>772</v>
       </c>
       <c r="R109" t="s">
-        <v>805</v>
+        <v>794</v>
       </c>
       <c r="S109" t="s">
-        <v>806</v>
+        <v>795</v>
       </c>
       <c r="T109" t="s">
-        <v>807</v>
+        <v>796</v>
       </c>
       <c r="U109" t="s">
         <v>745</v>
       </c>
       <c r="V109" t="s">
-        <v>808</v>
+        <v>797</v>
       </c>
       <c r="W109" t="s">
         <v>7</v>
@@ -6251,55 +6242,67 @@
     </row>
     <row r="112" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
-        <v>375</v>
+        <v>236</v>
       </c>
       <c r="B112" t="s">
-        <v>376</v>
+        <v>237</v>
       </c>
       <c r="C112">
-        <v>2021</v>
+        <v>2017</v>
       </c>
       <c r="D112" t="s">
-        <v>377</v>
+        <v>238</v>
       </c>
       <c r="E112" t="s">
-        <v>326</v>
+        <v>229</v>
       </c>
       <c r="F112">
-        <v>0.91646497939055904</v>
+        <v>0.91594384348707403</v>
+      </c>
+      <c r="G112" t="s">
+        <v>601</v>
       </c>
       <c r="H112" t="s">
         <v>559</v>
       </c>
       <c r="I112" t="s">
-        <v>567</v>
+        <v>600</v>
+      </c>
+      <c r="J112" t="s">
+        <v>739</v>
       </c>
       <c r="K112" t="s">
-        <v>553</v>
+        <v>550</v>
       </c>
       <c r="L112" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="M112" t="s">
-        <v>545</v>
+        <v>550</v>
+      </c>
+      <c r="N112" t="s">
+        <v>548</v>
       </c>
       <c r="P112" t="s">
-        <v>809</v>
+        <v>743</v>
       </c>
       <c r="Q112" t="s">
         <v>740</v>
       </c>
+      <c r="R112" t="s">
+        <v>741</v>
+      </c>
       <c r="S112" t="s">
-        <v>810</v>
+        <v>742</v>
       </c>
       <c r="T112" t="s">
-        <v>811</v>
+        <v>744</v>
       </c>
       <c r="U112" t="s">
         <v>745</v>
       </c>
       <c r="V112" t="s">
-        <v>812</v>
+        <v>746</v>
       </c>
       <c r="W112" t="s">
         <v>7</v>
@@ -6427,120 +6430,108 @@
     </row>
     <row r="119" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
-        <v>96</v>
+        <v>454</v>
       </c>
       <c r="B119" t="s">
-        <v>97</v>
+        <v>455</v>
       </c>
       <c r="C119">
-        <v>2018</v>
+        <v>2009</v>
       </c>
       <c r="D119" t="s">
-        <v>670</v>
+        <v>456</v>
       </c>
       <c r="E119" t="s">
-        <v>8</v>
+        <v>423</v>
       </c>
       <c r="F119">
-        <v>0.98671295859140085</v>
-      </c>
-      <c r="G119" t="s">
-        <v>817</v>
+        <v>0.98052761532990129</v>
       </c>
       <c r="H119" t="s">
         <v>559</v>
       </c>
-      <c r="I119" t="s">
-        <v>561</v>
+      <c r="J119" t="s">
+        <v>780</v>
       </c>
       <c r="K119" t="s">
         <v>550</v>
       </c>
-      <c r="L119" t="s">
-        <v>554</v>
-      </c>
       <c r="M119" t="s">
         <v>550</v>
       </c>
-      <c r="N119" t="s">
-        <v>548</v>
-      </c>
       <c r="P119" t="s">
-        <v>813</v>
+        <v>775</v>
       </c>
       <c r="Q119" t="s">
-        <v>814</v>
+        <v>772</v>
       </c>
       <c r="R119" t="s">
-        <v>815</v>
+        <v>773</v>
       </c>
       <c r="S119" t="s">
-        <v>816</v>
+        <v>774</v>
       </c>
       <c r="T119" t="s">
-        <v>818</v>
+        <v>776</v>
       </c>
       <c r="U119" t="s">
         <v>745</v>
       </c>
       <c r="V119" t="s">
-        <v>819</v>
+        <v>771</v>
       </c>
     </row>
     <row r="120" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B120" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C120">
-        <v>2015</v>
+        <v>2008</v>
       </c>
       <c r="D120" t="s">
-        <v>671</v>
+        <v>664</v>
       </c>
       <c r="E120" t="s">
         <v>8</v>
       </c>
       <c r="F120">
-        <v>0.95050734852012941</v>
-      </c>
-      <c r="G120" t="s">
-        <v>112</v>
+        <v>0.9377232202339163</v>
       </c>
       <c r="H120" t="s">
-        <v>594</v>
+        <v>559</v>
       </c>
       <c r="K120" t="s">
-        <v>604</v>
+        <v>546</v>
       </c>
       <c r="M120" t="s">
-        <v>604</v>
+        <v>543</v>
       </c>
       <c r="P120" t="s">
-        <v>820</v>
+        <v>798</v>
       </c>
       <c r="Q120" t="s">
-        <v>826</v>
+        <v>799</v>
       </c>
       <c r="R120" t="s">
-        <v>827</v>
+        <v>800</v>
       </c>
       <c r="S120" t="s">
-        <v>821</v>
+        <v>801</v>
       </c>
       <c r="T120" t="s">
-        <v>822</v>
+        <v>802</v>
       </c>
       <c r="U120" t="s">
         <v>745</v>
       </c>
       <c r="V120" t="s">
-        <v>45</v>
+        <v>803</v>
       </c>
       <c r="W120" t="s">
-        <v>823</v>
+        <v>7</v>
       </c>
     </row>
     <row r="121" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
@@ -6645,25 +6636,22 @@
     </row>
     <row r="126" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
-        <v>384</v>
+        <v>372</v>
       </c>
       <c r="B126" t="s">
-        <v>385</v>
+        <v>373</v>
       </c>
       <c r="C126">
-        <v>2005</v>
+        <v>2014</v>
       </c>
       <c r="D126" t="s">
-        <v>386</v>
+        <v>374</v>
       </c>
       <c r="E126" t="s">
         <v>326</v>
       </c>
       <c r="F126">
-        <v>0.909473415779947</v>
-      </c>
-      <c r="G126" t="s">
-        <v>610</v>
+        <v>0.94589893918682422</v>
       </c>
       <c r="H126" t="s">
         <v>559</v>
@@ -6671,29 +6659,35 @@
       <c r="K126" t="s">
         <v>550</v>
       </c>
+      <c r="L126" t="s">
+        <v>554</v>
+      </c>
       <c r="M126" t="s">
         <v>550</v>
       </c>
+      <c r="N126" t="s">
+        <v>548</v>
+      </c>
       <c r="P126" t="s">
-        <v>824</v>
+        <v>804</v>
       </c>
       <c r="Q126" t="s">
         <v>740</v>
       </c>
       <c r="R126" t="s">
-        <v>825</v>
+        <v>805</v>
       </c>
       <c r="S126" t="s">
-        <v>828</v>
+        <v>806</v>
       </c>
       <c r="T126" t="s">
-        <v>829</v>
+        <v>807</v>
       </c>
       <c r="U126" t="s">
         <v>745</v>
       </c>
       <c r="V126" t="s">
-        <v>830</v>
+        <v>808</v>
       </c>
       <c r="W126" t="s">
         <v>7</v>
@@ -7141,67 +7135,58 @@
     </row>
     <row r="149" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
-        <v>393</v>
+        <v>375</v>
       </c>
       <c r="B149" t="s">
-        <v>394</v>
+        <v>376</v>
       </c>
       <c r="C149">
-        <v>2023</v>
+        <v>2021</v>
       </c>
       <c r="D149" t="s">
-        <v>395</v>
+        <v>377</v>
       </c>
       <c r="E149" t="s">
         <v>326</v>
       </c>
       <c r="F149">
-        <v>0.97458912963154121</v>
-      </c>
-      <c r="G149" t="s">
-        <v>611</v>
+        <v>0.91646497939055904</v>
       </c>
       <c r="H149" t="s">
-        <v>573</v>
+        <v>559</v>
       </c>
       <c r="I149" t="s">
-        <v>577</v>
+        <v>567</v>
       </c>
       <c r="K149" t="s">
-        <v>550</v>
+        <v>553</v>
       </c>
       <c r="L149" t="s">
-        <v>557</v>
+        <v>555</v>
       </c>
       <c r="M149" t="s">
-        <v>550</v>
-      </c>
-      <c r="N149" t="s">
-        <v>544</v>
+        <v>545</v>
       </c>
       <c r="P149" t="s">
-        <v>831</v>
+        <v>809</v>
       </c>
       <c r="Q149" t="s">
-        <v>834</v>
-      </c>
-      <c r="R149" t="s">
-        <v>835</v>
+        <v>740</v>
       </c>
       <c r="S149" t="s">
-        <v>832</v>
+        <v>810</v>
       </c>
       <c r="T149" t="s">
-        <v>45</v>
+        <v>811</v>
       </c>
       <c r="U149" t="s">
         <v>745</v>
       </c>
       <c r="V149" t="s">
-        <v>836</v>
+        <v>812</v>
       </c>
       <c r="W149" t="s">
-        <v>833</v>
+        <v>7</v>
       </c>
     </row>
     <row r="150" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
@@ -7226,52 +7211,64 @@
     </row>
     <row r="151" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
-        <v>192</v>
+        <v>96</v>
       </c>
       <c r="B151" t="s">
-        <v>193</v>
+        <v>97</v>
       </c>
       <c r="C151">
-        <v>2020</v>
+        <v>2018</v>
       </c>
       <c r="D151" t="s">
-        <v>685</v>
+        <v>670</v>
       </c>
       <c r="E151" t="s">
-        <v>179</v>
+        <v>8</v>
       </c>
       <c r="F151">
-        <v>0.99350047019181054</v>
+        <v>0.98671295859140085</v>
+      </c>
+      <c r="G151" t="s">
+        <v>817</v>
       </c>
       <c r="H151" t="s">
-        <v>581</v>
+        <v>559</v>
+      </c>
+      <c r="I151" t="s">
+        <v>561</v>
       </c>
       <c r="K151" t="s">
-        <v>604</v>
+        <v>550</v>
+      </c>
+      <c r="L151" t="s">
+        <v>554</v>
       </c>
       <c r="M151" t="s">
-        <v>544</v>
+        <v>550</v>
       </c>
       <c r="N151" t="s">
-        <v>604</v>
+        <v>548</v>
       </c>
       <c r="P151" t="s">
-        <v>837</v>
+        <v>813</v>
       </c>
       <c r="Q151" t="s">
-        <v>838</v>
+        <v>814</v>
       </c>
       <c r="R151" t="s">
-        <v>839</v>
+        <v>815</v>
+      </c>
+      <c r="S151" t="s">
+        <v>816</v>
       </c>
       <c r="T151" t="s">
-        <v>840</v>
+        <v>818</v>
       </c>
       <c r="U151" t="s">
-        <v>728</v>
+        <v>745</v>
       </c>
       <c r="V151" t="s">
-        <v>841</v>
+        <v>819</v>
       </c>
     </row>
     <row r="152" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
@@ -7454,7 +7451,7 @@
         <v>0.4582988328042289</v>
       </c>
     </row>
-    <row r="161" spans="1:22" hidden="1" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
         <v>153</v>
       </c>
@@ -7474,7 +7471,7 @@
         <v>0.23920195213180984</v>
       </c>
     </row>
-    <row r="162" spans="1:22" hidden="1" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
         <v>290</v>
       </c>
@@ -7494,7 +7491,7 @@
         <v>0.30269949039670829</v>
       </c>
     </row>
-    <row r="163" spans="1:22" hidden="1" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
         <v>68</v>
       </c>
@@ -7514,7 +7511,7 @@
         <v>0.26186022556174315</v>
       </c>
     </row>
-    <row r="164" spans="1:22" hidden="1" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
         <v>511</v>
       </c>
@@ -7534,7 +7531,7 @@
         <v>7.9207072315683691E-2</v>
       </c>
     </row>
-    <row r="165" spans="1:22" hidden="1" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
         <v>293</v>
       </c>
@@ -7554,7 +7551,7 @@
         <v>0.50583927644494631</v>
       </c>
     </row>
-    <row r="166" spans="1:22" hidden="1" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
         <v>70</v>
       </c>
@@ -7574,7 +7571,7 @@
         <v>0.89472865765298393</v>
       </c>
     </row>
-    <row r="167" spans="1:22" hidden="1" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
         <v>217</v>
       </c>
@@ -7594,7 +7591,7 @@
         <v>0.85781123435434148</v>
       </c>
     </row>
-    <row r="168" spans="1:22" hidden="1" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
         <v>514</v>
       </c>
@@ -7614,7 +7611,7 @@
         <v>0.63167371710375375</v>
       </c>
     </row>
-    <row r="169" spans="1:22" hidden="1" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
         <v>296</v>
       </c>
@@ -7634,7 +7631,7 @@
         <v>0.14109683217325797</v>
       </c>
     </row>
-    <row r="170" spans="1:22" hidden="1" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
         <v>402</v>
       </c>
@@ -7654,7 +7651,7 @@
         <v>0.32684380856723494</v>
       </c>
     </row>
-    <row r="171" spans="1:22" hidden="1" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
         <v>299</v>
       </c>
@@ -7674,7 +7671,7 @@
         <v>0.52131912295853855</v>
       </c>
     </row>
-    <row r="172" spans="1:22" hidden="1" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
         <v>405</v>
       </c>
@@ -7694,34 +7691,31 @@
         <v>0.2474266587890579</v>
       </c>
     </row>
-    <row r="173" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
-        <v>302</v>
+        <v>384</v>
       </c>
       <c r="B173" t="s">
-        <v>303</v>
+        <v>385</v>
       </c>
       <c r="C173">
-        <v>2002</v>
+        <v>2005</v>
       </c>
       <c r="D173" t="s">
-        <v>304</v>
+        <v>386</v>
       </c>
       <c r="E173" t="s">
-        <v>229</v>
+        <v>326</v>
       </c>
       <c r="F173">
-        <v>0.96001626119540306</v>
-      </c>
-      <c r="G173" s="6" t="s">
-        <v>612</v>
+        <v>0.909473415779947</v>
+      </c>
+      <c r="G173" t="s">
+        <v>610</v>
       </c>
       <c r="H173" t="s">
         <v>559</v>
       </c>
-      <c r="I173" t="s">
-        <v>580</v>
-      </c>
       <c r="K173" t="s">
         <v>550</v>
       </c>
@@ -7729,28 +7723,31 @@
         <v>550</v>
       </c>
       <c r="P173" t="s">
-        <v>842</v>
+        <v>824</v>
       </c>
       <c r="Q173" t="s">
         <v>740</v>
       </c>
       <c r="R173" t="s">
-        <v>843</v>
+        <v>825</v>
       </c>
       <c r="S173" t="s">
-        <v>844</v>
+        <v>828</v>
       </c>
       <c r="T173" t="s">
-        <v>845</v>
+        <v>829</v>
       </c>
       <c r="U173" t="s">
         <v>745</v>
       </c>
       <c r="V173" t="s">
-        <v>846</v>
-      </c>
-    </row>
-    <row r="174" spans="1:22" hidden="1" x14ac:dyDescent="0.25">
+        <v>830</v>
+      </c>
+      <c r="W173" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="174" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
         <v>220</v>
       </c>
@@ -7770,7 +7767,7 @@
         <v>0.8478060590412958</v>
       </c>
     </row>
-    <row r="175" spans="1:22" hidden="1" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
       <c r="A175" t="s">
         <v>305</v>
       </c>
@@ -7790,7 +7787,7 @@
         <v>0.82259738157325779</v>
       </c>
     </row>
-    <row r="176" spans="1:22" hidden="1" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
         <v>155</v>
       </c>
@@ -7810,7 +7807,7 @@
         <v>0.82406871839071871</v>
       </c>
     </row>
-    <row r="177" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:22" hidden="1" x14ac:dyDescent="0.25">
       <c r="A177" t="s">
         <v>408</v>
       </c>
@@ -7830,7 +7827,7 @@
         <v>0.16830327699084247</v>
       </c>
     </row>
-    <row r="178" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:22" hidden="1" x14ac:dyDescent="0.25">
       <c r="A178" t="s">
         <v>72</v>
       </c>
@@ -7850,7 +7847,7 @@
         <v>0.64336201972799223</v>
       </c>
     </row>
-    <row r="179" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:22" hidden="1" x14ac:dyDescent="0.25">
       <c r="A179" t="s">
         <v>157</v>
       </c>
@@ -7870,7 +7867,7 @@
         <v>0.52290166213799183</v>
       </c>
     </row>
-    <row r="180" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:22" hidden="1" x14ac:dyDescent="0.25">
       <c r="A180" t="s">
         <v>411</v>
       </c>
@@ -7890,7 +7887,7 @@
         <v>0.77489464756864379</v>
       </c>
     </row>
-    <row r="181" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:22" hidden="1" x14ac:dyDescent="0.25">
       <c r="A181" t="s">
         <v>517</v>
       </c>
@@ -7910,7 +7907,7 @@
         <v>0.38552152104531323</v>
       </c>
     </row>
-    <row r="182" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:22" hidden="1" x14ac:dyDescent="0.25">
       <c r="A182" t="s">
         <v>196</v>
       </c>
@@ -7930,7 +7927,7 @@
         <v>0.68195928298704322</v>
       </c>
     </row>
-    <row r="183" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:22" hidden="1" x14ac:dyDescent="0.25">
       <c r="A183" t="s">
         <v>74</v>
       </c>
@@ -7950,7 +7947,7 @@
         <v>0.67328120425693738</v>
       </c>
     </row>
-    <row r="184" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:22" hidden="1" x14ac:dyDescent="0.25">
       <c r="A184" t="s">
         <v>104</v>
       </c>
@@ -7970,7 +7967,7 @@
         <v>0.76967267011478835</v>
       </c>
     </row>
-    <row r="185" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:22" hidden="1" x14ac:dyDescent="0.25">
       <c r="A185" t="s">
         <v>520</v>
       </c>
@@ -7990,60 +7987,63 @@
         <v>0.4283608544625106</v>
       </c>
     </row>
-    <row r="186" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A186" t="s">
-        <v>76</v>
+        <v>302</v>
       </c>
       <c r="B186" t="s">
-        <v>77</v>
-      </c>
-      <c r="C186" t="s">
-        <v>7</v>
+        <v>303</v>
+      </c>
+      <c r="C186">
+        <v>2002</v>
       </c>
       <c r="D186" t="s">
-        <v>700</v>
+        <v>304</v>
       </c>
       <c r="E186" t="s">
-        <v>8</v>
+        <v>229</v>
       </c>
       <c r="F186">
-        <v>0.95593579028494435</v>
+        <v>0.96001626119540306</v>
+      </c>
+      <c r="G186" s="6" t="s">
+        <v>612</v>
       </c>
       <c r="H186" t="s">
         <v>559</v>
       </c>
       <c r="I186" t="s">
-        <v>600</v>
+        <v>580</v>
       </c>
       <c r="K186" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
       <c r="M186" t="s">
-        <v>547</v>
+        <v>550</v>
       </c>
       <c r="P186" t="s">
-        <v>847</v>
+        <v>842</v>
       </c>
       <c r="Q186" t="s">
         <v>740</v>
       </c>
+      <c r="R186" t="s">
+        <v>843</v>
+      </c>
       <c r="S186" t="s">
-        <v>848</v>
+        <v>844</v>
       </c>
       <c r="T186" t="s">
-        <v>849</v>
+        <v>845</v>
       </c>
       <c r="U186" t="s">
-        <v>850</v>
+        <v>745</v>
       </c>
       <c r="V186" t="s">
-        <v>851</v>
-      </c>
-      <c r="W186" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="187" spans="1:23" x14ac:dyDescent="0.25">
+        <v>846</v>
+      </c>
+    </row>
+    <row r="187" spans="1:22" hidden="1" x14ac:dyDescent="0.25">
       <c r="A187" s="5" t="s">
         <v>523</v>
       </c>
@@ -8072,7 +8072,7 @@
       <c r="N187" s="5"/>
       <c r="O187" s="5"/>
     </row>
-    <row r="188" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:22" hidden="1" x14ac:dyDescent="0.25">
       <c r="A188" t="s">
         <v>414</v>
       </c>
@@ -8092,7 +8092,7 @@
         <v>0.62284863857130934</v>
       </c>
     </row>
-    <row r="189" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:22" hidden="1" x14ac:dyDescent="0.25">
       <c r="A189" t="s">
         <v>198</v>
       </c>
@@ -8112,7 +8112,7 @@
         <v>0.35332348050141593</v>
       </c>
     </row>
-    <row r="190" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:22" hidden="1" x14ac:dyDescent="0.25">
       <c r="A190" t="s">
         <v>526</v>
       </c>
@@ -8132,7 +8132,7 @@
         <v>0.86625883364667722</v>
       </c>
     </row>
-    <row r="191" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:22" hidden="1" x14ac:dyDescent="0.25">
       <c r="A191" t="s">
         <v>78</v>
       </c>
@@ -8152,7 +8152,7 @@
         <v>0.10404090788447473</v>
       </c>
     </row>
-    <row r="192" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:22" hidden="1" x14ac:dyDescent="0.25">
       <c r="A192" t="s">
         <v>80</v>
       </c>
@@ -8172,7 +8172,7 @@
         <v>0.3739980983272112</v>
       </c>
     </row>
-    <row r="193" spans="1:22" hidden="1" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
       <c r="A193" t="s">
         <v>200</v>
       </c>
@@ -8192,7 +8192,7 @@
         <v>0.43770015968354758</v>
       </c>
     </row>
-    <row r="194" spans="1:22" hidden="1" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
       <c r="A194" t="s">
         <v>529</v>
       </c>
@@ -8212,60 +8212,60 @@
         <v>0.40977105268787617</v>
       </c>
     </row>
-    <row r="195" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A195" t="s">
-        <v>308</v>
+        <v>76</v>
       </c>
       <c r="B195" t="s">
-        <v>309</v>
-      </c>
-      <c r="C195">
-        <v>2015</v>
+        <v>77</v>
+      </c>
+      <c r="C195" t="s">
+        <v>7</v>
       </c>
       <c r="D195" t="s">
-        <v>310</v>
+        <v>700</v>
       </c>
       <c r="E195" t="s">
-        <v>229</v>
+        <v>8</v>
       </c>
       <c r="F195">
-        <v>0.90633376228548657</v>
-      </c>
-      <c r="G195" t="s">
-        <v>613</v>
+        <v>0.95593579028494435</v>
       </c>
       <c r="H195" t="s">
-        <v>560</v>
+        <v>559</v>
+      </c>
+      <c r="I195" t="s">
+        <v>600</v>
       </c>
       <c r="K195" t="s">
-        <v>602</v>
+        <v>551</v>
       </c>
       <c r="M195" t="s">
-        <v>544</v>
+        <v>547</v>
       </c>
       <c r="P195" t="s">
-        <v>852</v>
+        <v>847</v>
       </c>
       <c r="Q195" t="s">
-        <v>855</v>
-      </c>
-      <c r="R195" t="s">
-        <v>853</v>
+        <v>740</v>
       </c>
       <c r="S195" t="s">
-        <v>854</v>
+        <v>848</v>
       </c>
       <c r="T195" t="s">
-        <v>856</v>
+        <v>849</v>
       </c>
       <c r="U195" t="s">
-        <v>857</v>
+        <v>850</v>
       </c>
       <c r="V195" t="s">
-        <v>858</v>
-      </c>
-    </row>
-    <row r="196" spans="1:22" hidden="1" x14ac:dyDescent="0.25">
+        <v>851</v>
+      </c>
+      <c r="W195" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="196" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
       <c r="A196" t="s">
         <v>223</v>
       </c>
@@ -8285,7 +8285,7 @@
         <v>0.49874744263805126</v>
       </c>
     </row>
-    <row r="197" spans="1:22" hidden="1" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
       <c r="A197" t="s">
         <v>532</v>
       </c>
@@ -8305,7 +8305,7 @@
         <v>0.46222181946868313</v>
       </c>
     </row>
-    <row r="198" spans="1:22" hidden="1" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
       <c r="A198" t="s">
         <v>82</v>
       </c>
@@ -8325,7 +8325,7 @@
         <v>7.3971468220319303E-2</v>
       </c>
     </row>
-    <row r="199" spans="1:22" hidden="1" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
       <c r="A199" t="s">
         <v>159</v>
       </c>
@@ -8345,7 +8345,7 @@
         <v>0.25122784488383565</v>
       </c>
     </row>
-    <row r="200" spans="1:22" hidden="1" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
       <c r="A200" t="s">
         <v>314</v>
       </c>
@@ -8365,7 +8365,7 @@
         <v>0.33212404034706278</v>
       </c>
     </row>
-    <row r="201" spans="1:22" hidden="1" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
       <c r="A201" t="s">
         <v>161</v>
       </c>
@@ -8385,7 +8385,7 @@
         <v>2.4867554476732945E-2</v>
       </c>
     </row>
-    <row r="202" spans="1:22" hidden="1" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
       <c r="A202" t="s">
         <v>535</v>
       </c>
@@ -8405,7 +8405,7 @@
         <v>0.72179019754562168</v>
       </c>
     </row>
-    <row r="203" spans="1:22" hidden="1" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
       <c r="A203" t="s">
         <v>317</v>
       </c>
@@ -8425,7 +8425,7 @@
         <v>5.4698861004331745E-2</v>
       </c>
     </row>
-    <row r="204" spans="1:22" hidden="1" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
       <c r="A204" t="s">
         <v>202</v>
       </c>
@@ -8445,7 +8445,7 @@
         <v>0.47047041171008219</v>
       </c>
     </row>
-    <row r="205" spans="1:22" hidden="1" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
       <c r="A205" t="s">
         <v>417</v>
       </c>
@@ -8465,7 +8465,7 @@
         <v>9.2272756155660773E-2</v>
       </c>
     </row>
-    <row r="206" spans="1:22" hidden="1" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
       <c r="A206" t="s">
         <v>320</v>
       </c>
@@ -8485,7 +8485,7 @@
         <v>0.47589895850307629</v>
       </c>
     </row>
-    <row r="207" spans="1:22" hidden="1" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
       <c r="A207" t="s">
         <v>84</v>
       </c>
@@ -8505,7 +8505,7 @@
         <v>0.49876287852409595</v>
       </c>
     </row>
-    <row r="208" spans="1:22" hidden="1" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
       <c r="A208" t="s">
         <v>163</v>
       </c>
@@ -8526,14 +8526,14 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:O208">
-    <filterColumn colId="5">
+  <autoFilter ref="A1:W208">
+    <filterColumn colId="7">
       <customFilters>
-        <customFilter operator="greaterThan" val="0.9"/>
+        <customFilter operator="notEqual" val=" "/>
       </customFilters>
     </filterColumn>
-    <sortState ref="A5:O196">
-      <sortCondition ref="B1:B209"/>
+    <sortState ref="A5:W195">
+      <sortCondition ref="H1:H208"/>
     </sortState>
   </autoFilter>
   <sortState ref="A2:Q209">

</xml_diff>

<commit_message>
setting up plots for manuscript... leaving off on getting author-title disambiguation reasonably complete
</commit_message>
<xml_diff>
--- a/_data/screened_fulltext/ft_consolidated_coding.xlsx
+++ b/_data/screened_fulltext/ft_consolidated_coding.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2788" uniqueCount="1561">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2796" uniqueCount="1562">
   <si>
     <t>title</t>
   </si>
@@ -2693,9 +2693,6 @@
   </si>
   <si>
     <t>The role of Earth observation (EO) data in addressing societal problems from environmental through to humanitarian should not be understated. Recent innovation in EO means provision of analysis ready data and data cubes, which allows for rapid use of EO data. This in combination with processing technologies, such as Google Earth Engine and open source algorithms/ software for EO data integration and analyses, has afforded an explosion of information to answer research questions and/or inform policy making. However, there is still a need for both training and validation data within EO projects – often this can be challenging to obtain. It has been suggested that citizen science can help here to provide these data, yet there is some perceived hesitancy in using citizen science within EO projects.</t>
-  </si>
-  <si>
-    <t>various;eudaimonistic</t>
   </si>
   <si>
     <t>Space systems play an important role in today’s society by generating or transmitting information from source to sink(s). The acquisition of the space system is often justified by the type, quantity and quality of information provided or transmitted. This work posits that the value of a class of space systems derives from and can be assessed through the value of information these systems provide.</t>
@@ -4709,6 +4706,12 @@
   </si>
   <si>
     <t>improved crop profitability and avoided losses</t>
+  </si>
+  <si>
+    <t>instrumental;fundamental</t>
+  </si>
+  <si>
+    <t>instrumental;fundamental;eudaimonistic</t>
   </si>
 </sst>
 </file>
@@ -5563,10 +5566,10 @@
   <dimension ref="A1:V171"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="D128" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="D53" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="G134" sqref="G134"/>
+      <selection pane="bottomRight" activeCell="M64" sqref="M64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6191,6 +6194,12 @@
       <c r="I11" s="5" t="s">
         <v>795</v>
       </c>
+      <c r="J11" s="5" t="s">
+        <v>457</v>
+      </c>
+      <c r="L11" s="5" t="s">
+        <v>457</v>
+      </c>
       <c r="O11" s="8" t="s">
         <v>792</v>
       </c>
@@ -6836,6 +6845,15 @@
       <c r="I23" t="s">
         <v>859</v>
       </c>
+      <c r="J23" s="5" t="s">
+        <v>458</v>
+      </c>
+      <c r="L23" s="5" t="s">
+        <v>454</v>
+      </c>
+      <c r="M23" s="5" t="s">
+        <v>451</v>
+      </c>
       <c r="O23" s="8" t="s">
         <v>855</v>
       </c>
@@ -7244,7 +7262,7 @@
         <v>887</v>
       </c>
       <c r="T30" t="s">
-        <v>890</v>
+        <v>1561</v>
       </c>
       <c r="U30" t="s">
         <v>888</v>
@@ -7279,25 +7297,25 @@
         <v>452</v>
       </c>
       <c r="O31" s="8" t="s">
-        <v>891</v>
+        <v>890</v>
       </c>
       <c r="P31" t="s">
         <v>626</v>
       </c>
       <c r="Q31" t="s">
+        <v>891</v>
+      </c>
+      <c r="R31" t="s">
         <v>892</v>
       </c>
-      <c r="R31" t="s">
+      <c r="S31" t="s">
         <v>893</v>
-      </c>
-      <c r="S31" t="s">
-        <v>894</v>
       </c>
       <c r="T31" t="s">
         <v>631</v>
       </c>
       <c r="U31" t="s">
-        <v>895</v>
+        <v>894</v>
       </c>
       <c r="V31" t="s">
         <v>7</v>
@@ -7323,7 +7341,7 @@
         <v>507</v>
       </c>
       <c r="I32" t="s">
-        <v>901</v>
+        <v>900</v>
       </c>
       <c r="J32" t="s">
         <v>458</v>
@@ -7332,16 +7350,16 @@
         <v>454</v>
       </c>
       <c r="O32" s="8" t="s">
+        <v>895</v>
+      </c>
+      <c r="P32" t="s">
         <v>896</v>
       </c>
-      <c r="P32" t="s">
+      <c r="Q32" t="s">
         <v>897</v>
       </c>
-      <c r="Q32" t="s">
+      <c r="R32" t="s">
         <v>898</v>
-      </c>
-      <c r="R32" t="s">
-        <v>899</v>
       </c>
       <c r="S32" t="s">
         <v>726</v>
@@ -7350,7 +7368,7 @@
         <v>736</v>
       </c>
       <c r="U32" s="5" t="s">
-        <v>900</v>
+        <v>899</v>
       </c>
       <c r="V32" s="5" t="s">
         <v>7</v>
@@ -7379,7 +7397,7 @@
         <v>480</v>
       </c>
       <c r="I33" t="s">
-        <v>908</v>
+        <v>907</v>
       </c>
       <c r="J33" t="s">
         <v>457</v>
@@ -7388,28 +7406,28 @@
         <v>457</v>
       </c>
       <c r="O33" s="8" t="s">
-        <v>903</v>
+        <v>902</v>
       </c>
       <c r="P33" t="s">
         <v>886</v>
       </c>
       <c r="Q33" t="s">
-        <v>904</v>
+        <v>903</v>
       </c>
       <c r="R33" t="s">
-        <v>906</v>
+        <v>905</v>
       </c>
       <c r="S33" t="s">
-        <v>902</v>
+        <v>901</v>
       </c>
       <c r="T33" s="5" t="s">
         <v>631</v>
       </c>
       <c r="U33" s="5" t="s">
-        <v>907</v>
+        <v>906</v>
       </c>
       <c r="V33" t="s">
-        <v>905</v>
+        <v>904</v>
       </c>
     </row>
     <row r="34" spans="1:22" x14ac:dyDescent="0.25">
@@ -7485,7 +7503,7 @@
         <v>466</v>
       </c>
       <c r="I35" t="s">
-        <v>913</v>
+        <v>912</v>
       </c>
       <c r="J35" t="s">
         <v>457</v>
@@ -7494,25 +7512,25 @@
         <v>457</v>
       </c>
       <c r="O35" s="8" t="s">
-        <v>909</v>
+        <v>908</v>
       </c>
       <c r="P35" t="s">
         <v>626</v>
       </c>
       <c r="Q35" t="s">
+        <v>909</v>
+      </c>
+      <c r="R35" t="s">
         <v>910</v>
       </c>
-      <c r="R35" t="s">
+      <c r="S35" t="s">
         <v>911</v>
-      </c>
-      <c r="S35" t="s">
-        <v>912</v>
       </c>
       <c r="T35" t="s">
         <v>631</v>
       </c>
       <c r="U35" t="s">
-        <v>914</v>
+        <v>913</v>
       </c>
       <c r="V35" t="s">
         <v>7</v>
@@ -7544,25 +7562,25 @@
         <v>457</v>
       </c>
       <c r="O36" s="8" t="s">
+        <v>914</v>
+      </c>
+      <c r="P36" t="s">
         <v>915</v>
       </c>
-      <c r="P36" t="s">
+      <c r="Q36" t="s">
         <v>916</v>
       </c>
-      <c r="Q36" t="s">
+      <c r="R36" t="s">
         <v>917</v>
       </c>
-      <c r="R36" t="s">
+      <c r="S36" t="s">
         <v>918</v>
-      </c>
-      <c r="S36" t="s">
-        <v>919</v>
       </c>
       <c r="T36" t="s">
         <v>631</v>
       </c>
       <c r="U36" t="s">
-        <v>920</v>
+        <v>919</v>
       </c>
       <c r="V36" t="s">
         <v>7</v>
@@ -7588,7 +7606,7 @@
         <v>480</v>
       </c>
       <c r="I37" t="s">
-        <v>928</v>
+        <v>927</v>
       </c>
       <c r="J37" t="s">
         <v>457</v>
@@ -7597,28 +7615,28 @@
         <v>457</v>
       </c>
       <c r="O37" s="8" t="s">
+        <v>920</v>
+      </c>
+      <c r="P37" t="s">
         <v>921</v>
       </c>
-      <c r="P37" t="s">
-        <v>922</v>
-      </c>
       <c r="Q37" t="s">
+        <v>923</v>
+      </c>
+      <c r="R37" t="s">
+        <v>925</v>
+      </c>
+      <c r="S37" t="s">
         <v>924</v>
-      </c>
-      <c r="R37" t="s">
-        <v>926</v>
-      </c>
-      <c r="S37" t="s">
-        <v>925</v>
       </c>
       <c r="T37" t="s">
         <v>668</v>
       </c>
       <c r="U37" t="s">
-        <v>927</v>
+        <v>926</v>
       </c>
       <c r="V37" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
     </row>
     <row r="38" spans="1:22" x14ac:dyDescent="0.25">
@@ -7641,7 +7659,7 @@
         <v>466</v>
       </c>
       <c r="I38" t="s">
-        <v>932</v>
+        <v>931</v>
       </c>
       <c r="J38" t="s">
         <v>457</v>
@@ -7656,25 +7674,25 @@
         <v>452</v>
       </c>
       <c r="O38" s="8" t="s">
-        <v>929</v>
+        <v>928</v>
       </c>
       <c r="P38" t="s">
         <v>626</v>
       </c>
       <c r="Q38" t="s">
-        <v>931</v>
+        <v>930</v>
       </c>
       <c r="R38" t="s">
-        <v>930</v>
+        <v>929</v>
       </c>
       <c r="S38" t="s">
-        <v>912</v>
+        <v>911</v>
       </c>
       <c r="T38" t="s">
         <v>631</v>
       </c>
       <c r="U38" t="s">
-        <v>933</v>
+        <v>932</v>
       </c>
     </row>
     <row r="39" spans="1:22" x14ac:dyDescent="0.25">
@@ -7700,7 +7718,7 @@
         <v>467</v>
       </c>
       <c r="I39" t="s">
-        <v>938</v>
+        <v>937</v>
       </c>
       <c r="J39" t="s">
         <v>453</v>
@@ -7709,25 +7727,25 @@
         <v>450</v>
       </c>
       <c r="O39" s="8" t="s">
+        <v>933</v>
+      </c>
+      <c r="P39" t="s">
+        <v>935</v>
+      </c>
+      <c r="R39" t="s">
         <v>934</v>
       </c>
-      <c r="P39" t="s">
-        <v>936</v>
-      </c>
-      <c r="R39" t="s">
-        <v>935</v>
-      </c>
       <c r="S39" t="s">
-        <v>925</v>
+        <v>924</v>
       </c>
       <c r="T39" t="s">
         <v>631</v>
       </c>
       <c r="U39" t="s">
-        <v>939</v>
+        <v>938</v>
       </c>
       <c r="V39" t="s">
-        <v>937</v>
+        <v>936</v>
       </c>
     </row>
     <row r="40" spans="1:22" x14ac:dyDescent="0.25">
@@ -7750,34 +7768,34 @@
         <v>466</v>
       </c>
       <c r="I40" t="s">
+        <v>943</v>
+      </c>
+      <c r="J40" t="s">
+        <v>457</v>
+      </c>
+      <c r="L40" t="s">
+        <v>457</v>
+      </c>
+      <c r="O40" s="8" t="s">
+        <v>939</v>
+      </c>
+      <c r="P40" t="s">
+        <v>941</v>
+      </c>
+      <c r="Q40" t="s">
+        <v>942</v>
+      </c>
+      <c r="R40" t="s">
+        <v>940</v>
+      </c>
+      <c r="S40" t="s">
         <v>944</v>
-      </c>
-      <c r="J40" t="s">
-        <v>457</v>
-      </c>
-      <c r="L40" t="s">
-        <v>457</v>
-      </c>
-      <c r="O40" s="8" t="s">
-        <v>940</v>
-      </c>
-      <c r="P40" t="s">
-        <v>942</v>
-      </c>
-      <c r="Q40" t="s">
-        <v>943</v>
-      </c>
-      <c r="R40" t="s">
-        <v>941</v>
-      </c>
-      <c r="S40" t="s">
-        <v>945</v>
       </c>
       <c r="T40" t="s">
         <v>631</v>
       </c>
       <c r="U40" t="s">
-        <v>946</v>
+        <v>945</v>
       </c>
       <c r="V40" t="s">
         <v>7</v>
@@ -7806,7 +7824,7 @@
         <v>475</v>
       </c>
       <c r="I41" t="s">
-        <v>953</v>
+        <v>952</v>
       </c>
       <c r="J41" t="s">
         <v>457</v>
@@ -7821,28 +7839,28 @@
         <v>456</v>
       </c>
       <c r="O41" s="8" t="s">
+        <v>946</v>
+      </c>
+      <c r="P41" t="s">
         <v>947</v>
       </c>
-      <c r="P41" t="s">
+      <c r="Q41" t="s">
         <v>948</v>
       </c>
-      <c r="Q41" t="s">
+      <c r="R41" t="s">
+        <v>953</v>
+      </c>
+      <c r="S41" t="s">
+        <v>924</v>
+      </c>
+      <c r="T41" t="s">
+        <v>950</v>
+      </c>
+      <c r="U41" t="s">
+        <v>951</v>
+      </c>
+      <c r="V41" t="s">
         <v>949</v>
-      </c>
-      <c r="R41" t="s">
-        <v>954</v>
-      </c>
-      <c r="S41" t="s">
-        <v>925</v>
-      </c>
-      <c r="T41" t="s">
-        <v>951</v>
-      </c>
-      <c r="U41" t="s">
-        <v>952</v>
-      </c>
-      <c r="V41" t="s">
-        <v>950</v>
       </c>
     </row>
     <row r="42" spans="1:22" x14ac:dyDescent="0.25">
@@ -7868,7 +7886,7 @@
         <v>468</v>
       </c>
       <c r="I42" t="s">
-        <v>957</v>
+        <v>956</v>
       </c>
       <c r="J42" t="s">
         <v>460</v>
@@ -7877,22 +7895,22 @@
         <v>452</v>
       </c>
       <c r="O42" s="8" t="s">
-        <v>955</v>
+        <v>954</v>
       </c>
       <c r="P42" t="s">
         <v>640</v>
       </c>
       <c r="R42" t="s">
-        <v>958</v>
+        <v>957</v>
       </c>
       <c r="S42" t="s">
-        <v>956</v>
+        <v>955</v>
       </c>
       <c r="T42" t="s">
         <v>631</v>
       </c>
       <c r="U42" t="s">
-        <v>959</v>
+        <v>958</v>
       </c>
       <c r="V42" t="s">
         <v>7</v>
@@ -7921,7 +7939,7 @@
         <v>466</v>
       </c>
       <c r="I43" t="s">
-        <v>963</v>
+        <v>962</v>
       </c>
       <c r="J43" t="s">
         <v>457</v>
@@ -7930,22 +7948,22 @@
         <v>457</v>
       </c>
       <c r="O43" s="8" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
       <c r="P43" t="s">
         <v>626</v>
       </c>
       <c r="R43" t="s">
-        <v>962</v>
+        <v>961</v>
       </c>
       <c r="S43" t="s">
-        <v>961</v>
+        <v>960</v>
       </c>
       <c r="T43" t="s">
         <v>631</v>
       </c>
       <c r="U43" t="s">
-        <v>964</v>
+        <v>963</v>
       </c>
       <c r="V43" t="s">
         <v>7</v>
@@ -7971,7 +7989,7 @@
         <v>466</v>
       </c>
       <c r="I44" t="s">
-        <v>967</v>
+        <v>966</v>
       </c>
       <c r="J44" t="s">
         <v>460</v>
@@ -7980,22 +7998,22 @@
         <v>452</v>
       </c>
       <c r="O44" s="8" t="s">
-        <v>965</v>
+        <v>964</v>
       </c>
       <c r="P44" t="s">
         <v>640</v>
       </c>
       <c r="R44" t="s">
-        <v>966</v>
+        <v>965</v>
       </c>
       <c r="S44" t="s">
-        <v>956</v>
+        <v>955</v>
       </c>
       <c r="T44" t="s">
         <v>631</v>
       </c>
       <c r="U44" t="s">
-        <v>959</v>
+        <v>958</v>
       </c>
       <c r="V44" t="s">
         <v>7</v>
@@ -8021,7 +8039,7 @@
         <v>466</v>
       </c>
       <c r="I45" t="s">
-        <v>972</v>
+        <v>971</v>
       </c>
       <c r="J45" t="s">
         <v>457</v>
@@ -8036,25 +8054,25 @@
         <v>456</v>
       </c>
       <c r="O45" s="8" t="s">
-        <v>969</v>
+        <v>968</v>
       </c>
       <c r="P45" t="s">
         <v>626</v>
       </c>
       <c r="Q45" t="s">
-        <v>970</v>
+        <v>969</v>
       </c>
       <c r="R45" t="s">
-        <v>968</v>
+        <v>967</v>
       </c>
       <c r="S45" t="s">
-        <v>912</v>
+        <v>911</v>
       </c>
       <c r="T45" t="s">
         <v>631</v>
       </c>
       <c r="U45" t="s">
-        <v>971</v>
+        <v>970</v>
       </c>
       <c r="V45" t="s">
         <v>7</v>
@@ -8092,25 +8110,25 @@
         <v>456</v>
       </c>
       <c r="O46" s="8" t="s">
-        <v>973</v>
+        <v>972</v>
       </c>
       <c r="P46" t="s">
         <v>720</v>
       </c>
       <c r="Q46" t="s">
+        <v>973</v>
+      </c>
+      <c r="R46" t="s">
         <v>974</v>
       </c>
-      <c r="R46" t="s">
+      <c r="S46" t="s">
         <v>975</v>
-      </c>
-      <c r="S46" t="s">
-        <v>976</v>
       </c>
       <c r="T46" t="s">
         <v>631</v>
       </c>
       <c r="U46" t="s">
-        <v>977</v>
+        <v>976</v>
       </c>
       <c r="V46" t="s">
         <v>7</v>
@@ -8148,25 +8166,25 @@
         <v>456</v>
       </c>
       <c r="O47" s="8" t="s">
+        <v>978</v>
+      </c>
+      <c r="P47" t="s">
         <v>979</v>
       </c>
-      <c r="P47" t="s">
+      <c r="Q47" t="s">
         <v>980</v>
       </c>
-      <c r="Q47" t="s">
+      <c r="R47" t="s">
+        <v>982</v>
+      </c>
+      <c r="S47" t="s">
         <v>981</v>
-      </c>
-      <c r="R47" t="s">
-        <v>983</v>
-      </c>
-      <c r="S47" t="s">
-        <v>982</v>
       </c>
       <c r="T47" t="s">
         <v>631</v>
       </c>
       <c r="U47" t="s">
-        <v>984</v>
+        <v>983</v>
       </c>
       <c r="V47" t="s">
         <v>7</v>
@@ -8204,22 +8222,22 @@
         <v>456</v>
       </c>
       <c r="O48" s="8" t="s">
-        <v>985</v>
+        <v>984</v>
       </c>
       <c r="P48" t="s">
         <v>780</v>
       </c>
       <c r="R48" t="s">
-        <v>986</v>
+        <v>985</v>
       </c>
       <c r="S48" t="s">
-        <v>982</v>
+        <v>981</v>
       </c>
       <c r="T48" t="s">
         <v>631</v>
       </c>
       <c r="U48" t="s">
-        <v>984</v>
+        <v>983</v>
       </c>
       <c r="V48" t="s">
         <v>7</v>
@@ -8260,22 +8278,22 @@
         <v>452</v>
       </c>
       <c r="O49" s="8" t="s">
+        <v>986</v>
+      </c>
+      <c r="P49" t="s">
         <v>987</v>
       </c>
-      <c r="P49" t="s">
+      <c r="R49" t="s">
+        <v>990</v>
+      </c>
+      <c r="S49" t="s">
         <v>988</v>
-      </c>
-      <c r="R49" t="s">
-        <v>991</v>
-      </c>
-      <c r="S49" t="s">
-        <v>989</v>
       </c>
       <c r="T49" t="s">
         <v>668</v>
       </c>
       <c r="U49" t="s">
-        <v>990</v>
+        <v>989</v>
       </c>
       <c r="V49" t="s">
         <v>7</v>
@@ -8301,7 +8319,7 @@
         <v>501</v>
       </c>
       <c r="I50" t="s">
-        <v>993</v>
+        <v>992</v>
       </c>
       <c r="J50" t="s">
         <v>457</v>
@@ -8316,25 +8334,25 @@
         <v>455</v>
       </c>
       <c r="O50" s="8" t="s">
-        <v>994</v>
+        <v>993</v>
       </c>
       <c r="P50" t="s">
         <v>720</v>
       </c>
       <c r="R50" t="s">
-        <v>996</v>
+        <v>995</v>
       </c>
       <c r="S50" t="s">
-        <v>992</v>
+        <v>991</v>
       </c>
       <c r="T50" t="s">
         <v>631</v>
       </c>
       <c r="U50" t="s">
-        <v>997</v>
+        <v>996</v>
       </c>
       <c r="V50" t="s">
-        <v>995</v>
+        <v>994</v>
       </c>
     </row>
     <row r="51" spans="1:22" x14ac:dyDescent="0.25">
@@ -8360,7 +8378,7 @@
         <v>480</v>
       </c>
       <c r="I51" t="s">
-        <v>999</v>
+        <v>998</v>
       </c>
       <c r="J51" t="s">
         <v>457</v>
@@ -8369,28 +8387,28 @@
         <v>457</v>
       </c>
       <c r="O51" s="8" t="s">
-        <v>998</v>
+        <v>997</v>
       </c>
       <c r="P51" t="s">
-        <v>916</v>
+        <v>915</v>
       </c>
       <c r="Q51" t="s">
+        <v>1000</v>
+      </c>
+      <c r="R51" t="s">
         <v>1001</v>
       </c>
-      <c r="R51" t="s">
-        <v>1002</v>
-      </c>
       <c r="S51" t="s">
-        <v>978</v>
+        <v>977</v>
       </c>
       <c r="T51" t="s">
         <v>615</v>
       </c>
       <c r="U51" t="s">
-        <v>1003</v>
+        <v>1002</v>
       </c>
       <c r="V51" t="s">
-        <v>1000</v>
+        <v>999</v>
       </c>
     </row>
     <row r="52" spans="1:22" x14ac:dyDescent="0.25">
@@ -8416,7 +8434,7 @@
         <v>480</v>
       </c>
       <c r="I52" t="s">
-        <v>1005</v>
+        <v>1004</v>
       </c>
       <c r="J52" t="s">
         <v>457</v>
@@ -8425,13 +8443,13 @@
         <v>457</v>
       </c>
       <c r="O52" s="8" t="s">
-        <v>1004</v>
+        <v>1003</v>
       </c>
       <c r="P52" t="s">
-        <v>916</v>
+        <v>915</v>
       </c>
       <c r="R52" t="s">
-        <v>1008</v>
+        <v>1007</v>
       </c>
       <c r="S52" t="s">
         <v>847</v>
@@ -8440,10 +8458,10 @@
         <v>668</v>
       </c>
       <c r="U52" t="s">
-        <v>1007</v>
+        <v>1006</v>
       </c>
       <c r="V52" t="s">
-        <v>1006</v>
+        <v>1005</v>
       </c>
     </row>
     <row r="53" spans="1:22" x14ac:dyDescent="0.25">
@@ -8466,7 +8484,7 @@
         <v>480</v>
       </c>
       <c r="I53" t="s">
-        <v>1011</v>
+        <v>1010</v>
       </c>
       <c r="J53" t="s">
         <v>457</v>
@@ -8475,16 +8493,16 @@
         <v>457</v>
       </c>
       <c r="O53" s="8" t="s">
-        <v>1009</v>
+        <v>1008</v>
       </c>
       <c r="T53" t="s">
         <v>668</v>
       </c>
       <c r="U53" t="s">
-        <v>1012</v>
+        <v>1011</v>
       </c>
       <c r="V53" t="s">
-        <v>1010</v>
+        <v>1009</v>
       </c>
     </row>
     <row r="54" spans="1:22" x14ac:dyDescent="0.25">
@@ -8513,25 +8531,25 @@
         <v>455</v>
       </c>
       <c r="O54" s="8" t="s">
+        <v>1012</v>
+      </c>
+      <c r="P54" t="s">
         <v>1013</v>
       </c>
-      <c r="P54" t="s">
+      <c r="Q54" t="s">
         <v>1014</v>
       </c>
-      <c r="Q54" t="s">
+      <c r="R54" t="s">
         <v>1015</v>
       </c>
-      <c r="R54" t="s">
+      <c r="S54" t="s">
         <v>1016</v>
-      </c>
-      <c r="S54" t="s">
-        <v>1017</v>
       </c>
       <c r="T54" t="s">
         <v>736</v>
       </c>
       <c r="U54" t="s">
-        <v>1018</v>
+        <v>1017</v>
       </c>
       <c r="V54" t="s">
         <v>7</v>
@@ -8569,28 +8587,28 @@
         <v>451</v>
       </c>
       <c r="O55" s="8" t="s">
+        <v>1018</v>
+      </c>
+      <c r="P55" t="s">
         <v>1019</v>
       </c>
-      <c r="P55" t="s">
+      <c r="Q55" t="s">
         <v>1020</v>
       </c>
-      <c r="Q55" t="s">
+      <c r="R55" t="s">
         <v>1021</v>
       </c>
-      <c r="R55" t="s">
+      <c r="S55" t="s">
         <v>1022</v>
-      </c>
-      <c r="S55" t="s">
-        <v>1023</v>
       </c>
       <c r="T55" t="s">
         <v>615</v>
       </c>
       <c r="U55" t="s">
+        <v>1023</v>
+      </c>
+      <c r="V55" t="s">
         <v>1024</v>
-      </c>
-      <c r="V55" t="s">
-        <v>1025</v>
       </c>
     </row>
     <row r="56" spans="1:22" x14ac:dyDescent="0.25">
@@ -8613,7 +8631,7 @@
         <v>501</v>
       </c>
       <c r="I56" t="s">
-        <v>1032</v>
+        <v>1031</v>
       </c>
       <c r="J56" t="s">
         <v>458</v>
@@ -8622,25 +8640,25 @@
         <v>454</v>
       </c>
       <c r="O56" s="8" t="s">
+        <v>1025</v>
+      </c>
+      <c r="P56" t="s">
+        <v>1027</v>
+      </c>
+      <c r="R56" t="s">
         <v>1026</v>
       </c>
-      <c r="P56" t="s">
+      <c r="S56" t="s">
         <v>1028</v>
-      </c>
-      <c r="R56" t="s">
-        <v>1027</v>
-      </c>
-      <c r="S56" t="s">
-        <v>1029</v>
       </c>
       <c r="T56" t="s">
         <v>668</v>
       </c>
       <c r="U56" t="s">
+        <v>1029</v>
+      </c>
+      <c r="V56" t="s">
         <v>1030</v>
-      </c>
-      <c r="V56" t="s">
-        <v>1031</v>
       </c>
     </row>
     <row r="57" spans="1:22" x14ac:dyDescent="0.25">
@@ -8669,25 +8687,25 @@
         <v>455</v>
       </c>
       <c r="O57" s="8" t="s">
+        <v>1032</v>
+      </c>
+      <c r="P57" t="s">
         <v>1033</v>
       </c>
-      <c r="P57" t="s">
+      <c r="Q57" t="s">
         <v>1034</v>
       </c>
-      <c r="Q57" t="s">
+      <c r="R57" t="s">
         <v>1035</v>
       </c>
-      <c r="R57" t="s">
+      <c r="S57" t="s">
         <v>1036</v>
-      </c>
-      <c r="S57" t="s">
-        <v>1037</v>
       </c>
       <c r="T57" t="s">
         <v>631</v>
       </c>
       <c r="U57" t="s">
-        <v>1038</v>
+        <v>1037</v>
       </c>
       <c r="V57" t="s">
         <v>7</v>
@@ -8766,7 +8784,7 @@
         <v>474</v>
       </c>
       <c r="I59" t="s">
-        <v>1044</v>
+        <v>1043</v>
       </c>
       <c r="J59" t="s">
         <v>462</v>
@@ -8781,19 +8799,19 @@
         <v>451</v>
       </c>
       <c r="O59" s="8" t="s">
+        <v>1038</v>
+      </c>
+      <c r="P59" t="s">
         <v>1039</v>
       </c>
-      <c r="P59" t="s">
+      <c r="Q59" t="s">
         <v>1040</v>
       </c>
-      <c r="Q59" t="s">
+      <c r="R59" t="s">
         <v>1041</v>
       </c>
-      <c r="R59" t="s">
+      <c r="S59" t="s">
         <v>1042</v>
-      </c>
-      <c r="S59" t="s">
-        <v>1043</v>
       </c>
       <c r="T59" t="s">
         <v>668</v>
@@ -8802,7 +8820,7 @@
         <v>41</v>
       </c>
       <c r="V59" t="s">
-        <v>1045</v>
+        <v>1044</v>
       </c>
     </row>
     <row r="60" spans="1:22" x14ac:dyDescent="0.25">
@@ -8831,16 +8849,16 @@
         <v>456</v>
       </c>
       <c r="O60" s="8" t="s">
-        <v>1046</v>
+        <v>1045</v>
       </c>
       <c r="P60" t="s">
         <v>720</v>
       </c>
       <c r="Q60" t="s">
-        <v>1048</v>
+        <v>1047</v>
       </c>
       <c r="R60" t="s">
-        <v>1047</v>
+        <v>1046</v>
       </c>
       <c r="S60" t="s">
         <v>726</v>
@@ -8849,7 +8867,7 @@
         <v>668</v>
       </c>
       <c r="U60" t="s">
-        <v>1049</v>
+        <v>1048</v>
       </c>
       <c r="V60" t="s">
         <v>7</v>
@@ -8875,7 +8893,7 @@
         <v>466</v>
       </c>
       <c r="I61" t="s">
-        <v>1053</v>
+        <v>1052</v>
       </c>
       <c r="J61" t="s">
         <v>461</v>
@@ -8890,16 +8908,16 @@
         <v>457</v>
       </c>
       <c r="O61" s="8" t="s">
-        <v>1050</v>
+        <v>1049</v>
       </c>
       <c r="P61" t="s">
         <v>626</v>
       </c>
       <c r="Q61" t="s">
+        <v>1050</v>
+      </c>
+      <c r="R61" t="s">
         <v>1051</v>
-      </c>
-      <c r="R61" t="s">
-        <v>1052</v>
       </c>
       <c r="S61" t="s">
         <v>812</v>
@@ -8908,7 +8926,7 @@
         <v>631</v>
       </c>
       <c r="U61" t="s">
-        <v>1054</v>
+        <v>1053</v>
       </c>
       <c r="V61" t="s">
         <v>7</v>
@@ -8934,7 +8952,7 @@
         <v>480</v>
       </c>
       <c r="I62" t="s">
-        <v>1057</v>
+        <v>1056</v>
       </c>
       <c r="J62" t="s">
         <v>457</v>
@@ -8949,28 +8967,28 @@
         <v>452</v>
       </c>
       <c r="O62" s="8" t="s">
-        <v>1055</v>
+        <v>1054</v>
       </c>
       <c r="P62" t="s">
         <v>651</v>
       </c>
       <c r="Q62" t="s">
-        <v>1060</v>
+        <v>1059</v>
       </c>
       <c r="R62" t="s">
-        <v>1059</v>
+        <v>1058</v>
       </c>
       <c r="S62" t="s">
-        <v>1056</v>
+        <v>1055</v>
       </c>
       <c r="T62" t="s">
         <v>736</v>
       </c>
       <c r="U62" t="s">
-        <v>1058</v>
+        <v>1057</v>
       </c>
       <c r="V62" t="s">
-        <v>1061</v>
+        <v>1060</v>
       </c>
     </row>
     <row r="63" spans="1:22" x14ac:dyDescent="0.25">
@@ -8993,7 +9011,7 @@
         <v>466</v>
       </c>
       <c r="I63" t="s">
-        <v>1067</v>
+        <v>1066</v>
       </c>
       <c r="J63" t="s">
         <v>457</v>
@@ -9008,25 +9026,25 @@
         <v>452</v>
       </c>
       <c r="O63" s="8" t="s">
-        <v>1062</v>
+        <v>1061</v>
       </c>
       <c r="P63" t="s">
         <v>626</v>
       </c>
       <c r="Q63" t="s">
+        <v>1062</v>
+      </c>
+      <c r="R63" t="s">
         <v>1063</v>
       </c>
-      <c r="R63" t="s">
+      <c r="S63" t="s">
         <v>1064</v>
-      </c>
-      <c r="S63" t="s">
-        <v>1065</v>
       </c>
       <c r="T63" t="s">
         <v>736</v>
       </c>
       <c r="U63" t="s">
-        <v>1066</v>
+        <v>1065</v>
       </c>
       <c r="V63" t="s">
         <v>7</v>
@@ -9055,10 +9073,19 @@
         <v>467</v>
       </c>
       <c r="I64" t="s">
-        <v>1069</v>
+        <v>1068</v>
+      </c>
+      <c r="J64" t="s">
+        <v>511</v>
+      </c>
+      <c r="L64" t="s">
+        <v>511</v>
       </c>
       <c r="O64" s="8" t="s">
-        <v>1068</v>
+        <v>1067</v>
+      </c>
+      <c r="T64" t="s">
+        <v>1560</v>
       </c>
     </row>
     <row r="65" spans="1:22" x14ac:dyDescent="0.25">
@@ -9081,7 +9108,7 @@
         <v>468</v>
       </c>
       <c r="I65" t="s">
-        <v>1073</v>
+        <v>1072</v>
       </c>
       <c r="J65" t="s">
         <v>453</v>
@@ -9090,13 +9117,13 @@
         <v>453</v>
       </c>
       <c r="O65" s="8" t="s">
-        <v>1070</v>
+        <v>1069</v>
       </c>
       <c r="P65" t="s">
         <v>780</v>
       </c>
       <c r="R65" t="s">
-        <v>1071</v>
+        <v>1070</v>
       </c>
       <c r="S65" t="s">
         <v>726</v>
@@ -9105,7 +9132,7 @@
         <v>631</v>
       </c>
       <c r="U65" t="s">
-        <v>1072</v>
+        <v>1071</v>
       </c>
       <c r="V65" t="s">
         <v>7</v>
@@ -9193,7 +9220,7 @@
         <v>480</v>
       </c>
       <c r="I67" t="s">
-        <v>1078</v>
+        <v>1077</v>
       </c>
       <c r="J67" t="s">
         <v>457</v>
@@ -9205,28 +9232,28 @@
         <v>457</v>
       </c>
       <c r="O67" s="8" t="s">
+        <v>1073</v>
+      </c>
+      <c r="P67" s="5" t="s">
         <v>1074</v>
       </c>
-      <c r="P67" s="5" t="s">
+      <c r="Q67" s="5" t="s">
         <v>1075</v>
       </c>
-      <c r="Q67" s="5" t="s">
+      <c r="R67" s="5" t="s">
         <v>1076</v>
       </c>
-      <c r="R67" s="5" t="s">
-        <v>1077</v>
-      </c>
       <c r="S67" s="5" t="s">
-        <v>1080</v>
+        <v>1079</v>
       </c>
       <c r="T67" s="5" t="s">
         <v>615</v>
       </c>
       <c r="U67" s="5" t="s">
-        <v>1081</v>
+        <v>1080</v>
       </c>
       <c r="V67" s="5" t="s">
-        <v>1079</v>
+        <v>1078</v>
       </c>
     </row>
     <row r="68" spans="1:22" x14ac:dyDescent="0.25">
@@ -9249,7 +9276,7 @@
         <v>466</v>
       </c>
       <c r="I68" t="s">
-        <v>1088</v>
+        <v>1087</v>
       </c>
       <c r="J68" t="s">
         <v>461</v>
@@ -9258,25 +9285,25 @@
         <v>455</v>
       </c>
       <c r="O68" s="8" t="s">
+        <v>1081</v>
+      </c>
+      <c r="P68" s="5" t="s">
         <v>1082</v>
       </c>
-      <c r="P68" s="5" t="s">
+      <c r="Q68" s="5" t="s">
         <v>1083</v>
       </c>
-      <c r="Q68" s="5" t="s">
+      <c r="R68" s="5" t="s">
         <v>1084</v>
       </c>
-      <c r="R68" s="5" t="s">
-        <v>1085</v>
-      </c>
       <c r="S68" s="5" t="s">
-        <v>1087</v>
+        <v>1086</v>
       </c>
       <c r="T68" s="5" t="s">
         <v>631</v>
       </c>
       <c r="U68" s="5" t="s">
-        <v>1086</v>
+        <v>1085</v>
       </c>
       <c r="V68" s="5" t="s">
         <v>7</v>
@@ -9302,34 +9329,34 @@
         <v>466</v>
       </c>
       <c r="I69" t="s">
+        <v>1091</v>
+      </c>
+      <c r="J69" t="s">
+        <v>457</v>
+      </c>
+      <c r="L69" t="s">
+        <v>457</v>
+      </c>
+      <c r="O69" s="8" t="s">
+        <v>1088</v>
+      </c>
+      <c r="P69" s="5" t="s">
+        <v>1089</v>
+      </c>
+      <c r="Q69" s="5" t="s">
+        <v>1090</v>
+      </c>
+      <c r="R69" t="s">
+        <v>1091</v>
+      </c>
+      <c r="S69" s="5" t="s">
         <v>1092</v>
-      </c>
-      <c r="J69" t="s">
-        <v>457</v>
-      </c>
-      <c r="L69" t="s">
-        <v>457</v>
-      </c>
-      <c r="O69" s="8" t="s">
-        <v>1089</v>
-      </c>
-      <c r="P69" s="5" t="s">
-        <v>1090</v>
-      </c>
-      <c r="Q69" s="5" t="s">
-        <v>1091</v>
-      </c>
-      <c r="R69" t="s">
-        <v>1092</v>
-      </c>
-      <c r="S69" s="5" t="s">
-        <v>1093</v>
       </c>
       <c r="T69" s="5" t="s">
         <v>631</v>
       </c>
       <c r="U69" s="5" t="s">
-        <v>1094</v>
+        <v>1093</v>
       </c>
       <c r="V69" s="5" t="s">
         <v>7</v>
@@ -9408,34 +9435,34 @@
         <v>466</v>
       </c>
       <c r="I71" t="s">
+        <v>1098</v>
+      </c>
+      <c r="J71" t="s">
+        <v>457</v>
+      </c>
+      <c r="L71" t="s">
+        <v>457</v>
+      </c>
+      <c r="O71" s="8" t="s">
+        <v>1094</v>
+      </c>
+      <c r="P71" t="s">
+        <v>1095</v>
+      </c>
+      <c r="Q71" t="s">
         <v>1099</v>
       </c>
-      <c r="J71" t="s">
-        <v>457</v>
-      </c>
-      <c r="L71" t="s">
-        <v>457</v>
-      </c>
-      <c r="O71" s="8" t="s">
-        <v>1095</v>
-      </c>
-      <c r="P71" t="s">
+      <c r="R71" t="s">
+        <v>1097</v>
+      </c>
+      <c r="S71" t="s">
         <v>1096</v>
-      </c>
-      <c r="Q71" t="s">
-        <v>1100</v>
-      </c>
-      <c r="R71" t="s">
-        <v>1098</v>
-      </c>
-      <c r="S71" t="s">
-        <v>1097</v>
       </c>
       <c r="T71" t="s">
         <v>631</v>
       </c>
       <c r="U71" t="s">
-        <v>1101</v>
+        <v>1100</v>
       </c>
       <c r="V71" t="s">
         <v>7</v>
@@ -9461,7 +9488,7 @@
         <v>469</v>
       </c>
       <c r="I72" t="s">
-        <v>1103</v>
+        <v>1102</v>
       </c>
       <c r="J72" t="s">
         <v>511</v>
@@ -9470,13 +9497,13 @@
         <v>511</v>
       </c>
       <c r="O72" s="8" t="s">
-        <v>1102</v>
+        <v>1101</v>
       </c>
       <c r="P72" t="s">
         <v>720</v>
       </c>
       <c r="R72" t="s">
-        <v>1104</v>
+        <v>1103</v>
       </c>
       <c r="S72" t="s">
         <v>41</v>
@@ -9485,7 +9512,7 @@
         <v>631</v>
       </c>
       <c r="U72" t="s">
-        <v>1105</v>
+        <v>1104</v>
       </c>
       <c r="V72" t="s">
         <v>7</v>
@@ -9517,25 +9544,25 @@
         <v>456</v>
       </c>
       <c r="O73" s="8" t="s">
-        <v>1106</v>
+        <v>1105</v>
       </c>
       <c r="P73" t="s">
         <v>626</v>
       </c>
       <c r="Q73" t="s">
+        <v>1106</v>
+      </c>
+      <c r="R73" t="s">
         <v>1107</v>
       </c>
-      <c r="R73" t="s">
-        <v>1108</v>
-      </c>
       <c r="S73" t="s">
-        <v>925</v>
+        <v>924</v>
       </c>
       <c r="T73" t="s">
         <v>668</v>
       </c>
       <c r="U73" t="s">
-        <v>1109</v>
+        <v>1108</v>
       </c>
       <c r="V73" t="s">
         <v>7</v>
@@ -9564,7 +9591,7 @@
         <v>469</v>
       </c>
       <c r="I74" t="s">
-        <v>1115</v>
+        <v>1114</v>
       </c>
       <c r="J74" t="s">
         <v>511</v>
@@ -9573,22 +9600,22 @@
         <v>511</v>
       </c>
       <c r="O74" s="8" t="s">
+        <v>1109</v>
+      </c>
+      <c r="P74" t="s">
         <v>1110</v>
       </c>
-      <c r="P74" t="s">
+      <c r="R74" t="s">
         <v>1111</v>
       </c>
-      <c r="R74" t="s">
+      <c r="S74" t="s">
         <v>1112</v>
-      </c>
-      <c r="S74" t="s">
-        <v>1113</v>
       </c>
       <c r="T74" t="s">
         <v>631</v>
       </c>
       <c r="U74" t="s">
-        <v>1114</v>
+        <v>1113</v>
       </c>
       <c r="V74" t="s">
         <v>7</v>
@@ -9614,7 +9641,7 @@
         <v>480</v>
       </c>
       <c r="I75" t="s">
-        <v>1119</v>
+        <v>1118</v>
       </c>
       <c r="J75" t="s">
         <v>463</v>
@@ -9626,25 +9653,25 @@
         <v>456</v>
       </c>
       <c r="O75" s="8" t="s">
-        <v>1116</v>
+        <v>1115</v>
       </c>
       <c r="P75" t="s">
         <v>640</v>
       </c>
       <c r="Q75" t="s">
+        <v>1116</v>
+      </c>
+      <c r="S75" t="s">
         <v>1117</v>
       </c>
-      <c r="S75" t="s">
+      <c r="T75" t="s">
+        <v>1119</v>
+      </c>
+      <c r="U75" t="s">
+        <v>1120</v>
+      </c>
+      <c r="V75" t="s">
         <v>1118</v>
-      </c>
-      <c r="T75" t="s">
-        <v>1120</v>
-      </c>
-      <c r="U75" t="s">
-        <v>1121</v>
-      </c>
-      <c r="V75" t="s">
-        <v>1119</v>
       </c>
     </row>
     <row r="76" spans="1:22" x14ac:dyDescent="0.25">
@@ -9667,7 +9694,7 @@
         <v>480</v>
       </c>
       <c r="I76" t="s">
-        <v>1124</v>
+        <v>1123</v>
       </c>
       <c r="J76" t="s">
         <v>457</v>
@@ -9676,28 +9703,28 @@
         <v>457</v>
       </c>
       <c r="O76" s="8" t="s">
-        <v>1122</v>
+        <v>1121</v>
       </c>
       <c r="P76" t="s">
         <v>712</v>
       </c>
       <c r="Q76" t="s">
+        <v>1125</v>
+      </c>
+      <c r="R76" t="s">
         <v>1126</v>
       </c>
-      <c r="R76" t="s">
-        <v>1127</v>
-      </c>
       <c r="S76" t="s">
-        <v>1129</v>
+        <v>1128</v>
       </c>
       <c r="T76" t="s">
         <v>736</v>
       </c>
       <c r="U76" t="s">
-        <v>1125</v>
+        <v>1124</v>
       </c>
       <c r="V76" t="s">
-        <v>1123</v>
+        <v>1122</v>
       </c>
     </row>
     <row r="77" spans="1:22" x14ac:dyDescent="0.25">
@@ -9726,16 +9753,16 @@
         <v>450</v>
       </c>
       <c r="O77" s="8" t="s">
-        <v>1128</v>
+        <v>1127</v>
       </c>
       <c r="P77" t="s">
         <v>626</v>
       </c>
       <c r="Q77" t="s">
+        <v>1129</v>
+      </c>
+      <c r="R77" t="s">
         <v>1130</v>
-      </c>
-      <c r="R77" t="s">
-        <v>1131</v>
       </c>
       <c r="S77" t="s">
         <v>854</v>
@@ -9744,7 +9771,7 @@
         <v>631</v>
       </c>
       <c r="U77" t="s">
-        <v>1132</v>
+        <v>1131</v>
       </c>
       <c r="V77" t="s">
         <v>7</v>
@@ -9773,7 +9800,7 @@
         <v>467</v>
       </c>
       <c r="I78" t="s">
-        <v>1135</v>
+        <v>1134</v>
       </c>
       <c r="J78" t="s">
         <v>457</v>
@@ -9782,19 +9809,19 @@
         <v>457</v>
       </c>
       <c r="O78" s="8" t="s">
+        <v>1132</v>
+      </c>
+      <c r="P78" t="s">
+        <v>1089</v>
+      </c>
+      <c r="Q78" t="s">
         <v>1133</v>
-      </c>
-      <c r="P78" t="s">
-        <v>1090</v>
-      </c>
-      <c r="Q78" t="s">
-        <v>1134</v>
       </c>
       <c r="T78" t="s">
         <v>631</v>
       </c>
       <c r="U78" t="s">
-        <v>1136</v>
+        <v>1135</v>
       </c>
       <c r="V78" t="s">
         <v>7</v>
@@ -9826,25 +9853,25 @@
         <v>456</v>
       </c>
       <c r="O79" s="8" t="s">
-        <v>1140</v>
+        <v>1139</v>
       </c>
       <c r="P79" t="s">
         <v>752</v>
       </c>
       <c r="Q79" t="s">
-        <v>1139</v>
+        <v>1138</v>
       </c>
       <c r="R79" t="s">
+        <v>1136</v>
+      </c>
+      <c r="S79" t="s">
         <v>1137</v>
-      </c>
-      <c r="S79" t="s">
-        <v>1138</v>
       </c>
       <c r="T79" t="s">
         <v>668</v>
       </c>
       <c r="U79" t="s">
-        <v>1141</v>
+        <v>1140</v>
       </c>
     </row>
     <row r="80" spans="1:22" x14ac:dyDescent="0.25">
@@ -9870,7 +9897,7 @@
         <v>468</v>
       </c>
       <c r="I80" t="s">
-        <v>1143</v>
+        <v>1142</v>
       </c>
       <c r="J80" t="s">
         <v>457</v>
@@ -9879,16 +9906,16 @@
         <v>457</v>
       </c>
       <c r="O80" s="8" t="s">
-        <v>1142</v>
+        <v>1141</v>
       </c>
       <c r="P80" t="s">
         <v>626</v>
       </c>
       <c r="Q80" t="s">
+        <v>1143</v>
+      </c>
+      <c r="R80" t="s">
         <v>1144</v>
-      </c>
-      <c r="R80" t="s">
-        <v>1145</v>
       </c>
       <c r="S80" t="s">
         <v>847</v>
@@ -9897,7 +9924,7 @@
         <v>631</v>
       </c>
       <c r="U80" t="s">
-        <v>1146</v>
+        <v>1145</v>
       </c>
       <c r="V80" t="s">
         <v>7</v>
@@ -9923,7 +9950,7 @@
         <v>501</v>
       </c>
       <c r="I81" t="s">
-        <v>1148</v>
+        <v>1147</v>
       </c>
       <c r="J81" t="s">
         <v>511</v>
@@ -9932,25 +9959,25 @@
         <v>511</v>
       </c>
       <c r="O81" s="8" t="s">
-        <v>1147</v>
+        <v>1146</v>
       </c>
       <c r="P81" t="s">
-        <v>980</v>
+        <v>979</v>
       </c>
       <c r="R81" t="s">
+        <v>1149</v>
+      </c>
+      <c r="S81" t="s">
         <v>1150</v>
-      </c>
-      <c r="S81" t="s">
-        <v>1151</v>
       </c>
       <c r="T81" t="s">
         <v>631</v>
       </c>
       <c r="U81" t="s">
-        <v>1152</v>
+        <v>1151</v>
       </c>
       <c r="V81" t="s">
-        <v>1149</v>
+        <v>1148</v>
       </c>
     </row>
     <row r="82" spans="1:22" ht="409.5" x14ac:dyDescent="0.25">
@@ -9976,7 +10003,7 @@
         <v>501</v>
       </c>
       <c r="I82" s="6" t="s">
-        <v>1157</v>
+        <v>1156</v>
       </c>
       <c r="J82" t="s">
         <v>457</v>
@@ -9985,28 +10012,28 @@
         <v>457</v>
       </c>
       <c r="O82" s="8" t="s">
+        <v>1152</v>
+      </c>
+      <c r="P82" t="s">
+        <v>979</v>
+      </c>
+      <c r="Q82" t="s">
+        <v>1154</v>
+      </c>
+      <c r="R82" t="s">
         <v>1153</v>
       </c>
-      <c r="P82" t="s">
-        <v>980</v>
-      </c>
-      <c r="Q82" t="s">
-        <v>1155</v>
-      </c>
-      <c r="R82" t="s">
-        <v>1154</v>
-      </c>
       <c r="S82" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="T82" t="s">
         <v>631</v>
       </c>
       <c r="U82" t="s">
-        <v>1158</v>
+        <v>1157</v>
       </c>
       <c r="V82" t="s">
-        <v>1156</v>
+        <v>1155</v>
       </c>
     </row>
     <row r="83" spans="1:22" x14ac:dyDescent="0.25">
@@ -10029,7 +10056,7 @@
         <v>467</v>
       </c>
       <c r="I83" t="s">
-        <v>1162</v>
+        <v>1161</v>
       </c>
       <c r="J83" t="s">
         <v>463</v>
@@ -10041,22 +10068,22 @@
         <v>456</v>
       </c>
       <c r="O83" s="8" t="s">
-        <v>1159</v>
+        <v>1158</v>
       </c>
       <c r="P83" t="s">
         <v>720</v>
       </c>
       <c r="Q83" t="s">
-        <v>1161</v>
+        <v>1160</v>
       </c>
       <c r="R83" t="s">
-        <v>1160</v>
+        <v>1159</v>
       </c>
       <c r="T83" t="s">
         <v>831</v>
       </c>
       <c r="U83" t="s">
-        <v>1163</v>
+        <v>1162</v>
       </c>
       <c r="V83" t="s">
         <v>7</v>
@@ -10088,25 +10115,25 @@
         <v>457</v>
       </c>
       <c r="O84" s="8" t="s">
-        <v>1164</v>
+        <v>1163</v>
       </c>
       <c r="P84" t="s">
         <v>626</v>
       </c>
       <c r="Q84" t="s">
+        <v>1164</v>
+      </c>
+      <c r="R84" t="s">
         <v>1165</v>
       </c>
-      <c r="R84" t="s">
+      <c r="S84" t="s">
         <v>1166</v>
-      </c>
-      <c r="S84" t="s">
-        <v>1167</v>
       </c>
       <c r="T84" t="s">
         <v>631</v>
       </c>
       <c r="U84" t="s">
-        <v>1168</v>
+        <v>1167</v>
       </c>
       <c r="V84" t="s">
         <v>7</v>
@@ -10132,7 +10159,7 @@
         <v>466</v>
       </c>
       <c r="I85" t="s">
-        <v>1172</v>
+        <v>1171</v>
       </c>
       <c r="J85" t="s">
         <v>457</v>
@@ -10141,25 +10168,25 @@
         <v>457</v>
       </c>
       <c r="O85" s="8" t="s">
-        <v>1170</v>
+        <v>1169</v>
       </c>
       <c r="P85" t="s">
         <v>626</v>
       </c>
       <c r="Q85" t="s">
-        <v>1171</v>
+        <v>1170</v>
       </c>
       <c r="R85" t="s">
-        <v>1169</v>
+        <v>1168</v>
       </c>
       <c r="S85" t="s">
-        <v>912</v>
+        <v>911</v>
       </c>
       <c r="T85" t="s">
         <v>631</v>
       </c>
       <c r="U85" t="s">
-        <v>1173</v>
+        <v>1172</v>
       </c>
     </row>
     <row r="86" spans="1:22" x14ac:dyDescent="0.25">
@@ -10182,7 +10209,7 @@
         <v>466</v>
       </c>
       <c r="I86" t="s">
-        <v>1178</v>
+        <v>1177</v>
       </c>
       <c r="J86" t="s">
         <v>511</v>
@@ -10191,25 +10218,25 @@
         <v>511</v>
       </c>
       <c r="O86" s="8" t="s">
-        <v>1174</v>
+        <v>1173</v>
       </c>
       <c r="P86" t="s">
         <v>626</v>
       </c>
       <c r="Q86" t="s">
-        <v>892</v>
+        <v>891</v>
       </c>
       <c r="R86" t="s">
+        <v>1174</v>
+      </c>
+      <c r="S86" t="s">
         <v>1175</v>
-      </c>
-      <c r="S86" t="s">
-        <v>1176</v>
       </c>
       <c r="T86" t="s">
         <v>631</v>
       </c>
       <c r="U86" t="s">
-        <v>1177</v>
+        <v>1176</v>
       </c>
     </row>
     <row r="87" spans="1:22" x14ac:dyDescent="0.25">
@@ -10232,7 +10259,7 @@
         <v>466</v>
       </c>
       <c r="I87" t="s">
-        <v>1184</v>
+        <v>1183</v>
       </c>
       <c r="J87" t="s">
         <v>457</v>
@@ -10241,25 +10268,25 @@
         <v>457</v>
       </c>
       <c r="O87" s="8" t="s">
-        <v>1179</v>
+        <v>1178</v>
       </c>
       <c r="P87" t="s">
         <v>806</v>
       </c>
       <c r="Q87" t="s">
+        <v>1179</v>
+      </c>
+      <c r="R87" t="s">
         <v>1180</v>
       </c>
-      <c r="R87" t="s">
+      <c r="S87" t="s">
         <v>1181</v>
-      </c>
-      <c r="S87" t="s">
-        <v>1182</v>
       </c>
       <c r="T87" t="s">
         <v>631</v>
       </c>
       <c r="U87" t="s">
-        <v>1183</v>
+        <v>1182</v>
       </c>
       <c r="V87" t="s">
         <v>7</v>
@@ -10335,7 +10362,7 @@
         <v>501</v>
       </c>
       <c r="I89" t="s">
-        <v>1190</v>
+        <v>1189</v>
       </c>
       <c r="J89" t="s">
         <v>457</v>
@@ -10344,28 +10371,28 @@
         <v>457</v>
       </c>
       <c r="O89" s="8" t="s">
-        <v>1185</v>
+        <v>1184</v>
       </c>
       <c r="P89" t="s">
         <v>626</v>
       </c>
       <c r="Q89" t="s">
+        <v>1185</v>
+      </c>
+      <c r="R89" t="s">
         <v>1186</v>
       </c>
-      <c r="R89" t="s">
+      <c r="S89" t="s">
         <v>1187</v>
-      </c>
-      <c r="S89" t="s">
-        <v>1188</v>
       </c>
       <c r="T89" t="s">
         <v>631</v>
       </c>
       <c r="U89" t="s">
-        <v>1191</v>
+        <v>1190</v>
       </c>
       <c r="V89" s="6" t="s">
-        <v>1189</v>
+        <v>1188</v>
       </c>
     </row>
     <row r="90" spans="1:22" x14ac:dyDescent="0.25">
@@ -10438,7 +10465,7 @@
         <v>501</v>
       </c>
       <c r="I91" t="s">
-        <v>1193</v>
+        <v>1192</v>
       </c>
       <c r="J91" t="s">
         <v>462</v>
@@ -10447,25 +10474,25 @@
         <v>509</v>
       </c>
       <c r="O91" s="8" t="s">
-        <v>1192</v>
+        <v>1191</v>
       </c>
       <c r="P91" t="s">
-        <v>1028</v>
+        <v>1027</v>
       </c>
       <c r="R91" t="s">
+        <v>1193</v>
+      </c>
+      <c r="S91" t="s">
         <v>1194</v>
-      </c>
-      <c r="S91" t="s">
-        <v>1195</v>
       </c>
       <c r="T91" t="s">
         <v>631</v>
       </c>
       <c r="U91" t="s">
+        <v>1195</v>
+      </c>
+      <c r="V91" t="s">
         <v>1196</v>
-      </c>
-      <c r="V91" t="s">
-        <v>1197</v>
       </c>
     </row>
     <row r="92" spans="1:22" x14ac:dyDescent="0.25">
@@ -10488,7 +10515,7 @@
         <v>466</v>
       </c>
       <c r="I92" t="s">
-        <v>1202</v>
+        <v>1201</v>
       </c>
       <c r="J92" t="s">
         <v>462</v>
@@ -10497,22 +10524,22 @@
         <v>509</v>
       </c>
       <c r="O92" s="8" t="s">
+        <v>1198</v>
+      </c>
+      <c r="P92" t="s">
         <v>1199</v>
       </c>
-      <c r="P92" t="s">
+      <c r="R92" t="s">
+        <v>1197</v>
+      </c>
+      <c r="S92" t="s">
         <v>1200</v>
-      </c>
-      <c r="R92" t="s">
-        <v>1198</v>
-      </c>
-      <c r="S92" t="s">
-        <v>1201</v>
       </c>
       <c r="T92" t="s">
         <v>631</v>
       </c>
       <c r="U92" t="s">
-        <v>1203</v>
+        <v>1202</v>
       </c>
       <c r="V92" t="s">
         <v>7</v>
@@ -10544,25 +10571,25 @@
         <v>455</v>
       </c>
       <c r="O93" s="8" t="s">
+        <v>1203</v>
+      </c>
+      <c r="P93" t="s">
+        <v>1205</v>
+      </c>
+      <c r="Q93" t="s">
+        <v>1206</v>
+      </c>
+      <c r="R93" t="s">
+        <v>1207</v>
+      </c>
+      <c r="S93" t="s">
         <v>1204</v>
-      </c>
-      <c r="P93" t="s">
-        <v>1206</v>
-      </c>
-      <c r="Q93" t="s">
-        <v>1207</v>
-      </c>
-      <c r="R93" t="s">
-        <v>1208</v>
-      </c>
-      <c r="S93" t="s">
-        <v>1205</v>
       </c>
       <c r="T93" t="s">
         <v>736</v>
       </c>
       <c r="U93" t="s">
-        <v>1209</v>
+        <v>1208</v>
       </c>
       <c r="V93" t="s">
         <v>7</v>
@@ -10644,7 +10671,7 @@
         <v>507</v>
       </c>
       <c r="I95" t="s">
-        <v>1213</v>
+        <v>1212</v>
       </c>
       <c r="J95" t="s">
         <v>457</v>
@@ -10653,13 +10680,13 @@
         <v>457</v>
       </c>
       <c r="O95" s="8" t="s">
-        <v>1210</v>
+        <v>1209</v>
       </c>
       <c r="P95" t="s">
         <v>626</v>
       </c>
       <c r="R95" t="s">
-        <v>1211</v>
+        <v>1210</v>
       </c>
       <c r="S95" t="s">
         <v>847</v>
@@ -10668,10 +10695,10 @@
         <v>631</v>
       </c>
       <c r="U95" t="s">
-        <v>1214</v>
+        <v>1213</v>
       </c>
       <c r="V95" t="s">
-        <v>1212</v>
+        <v>1211</v>
       </c>
     </row>
     <row r="96" spans="1:22" x14ac:dyDescent="0.25">
@@ -10694,7 +10721,7 @@
         <v>480</v>
       </c>
       <c r="I96" t="s">
-        <v>1218</v>
+        <v>1217</v>
       </c>
       <c r="J96" t="s">
         <v>457</v>
@@ -10706,25 +10733,25 @@
         <v>451</v>
       </c>
       <c r="O96" s="8" t="s">
-        <v>1215</v>
+        <v>1214</v>
       </c>
       <c r="P96" t="s">
         <v>784</v>
       </c>
       <c r="Q96" t="s">
-        <v>1216</v>
+        <v>1215</v>
       </c>
       <c r="S96" t="s">
-        <v>1219</v>
+        <v>1218</v>
       </c>
       <c r="T96" t="s">
         <v>631</v>
       </c>
       <c r="U96" t="s">
-        <v>1220</v>
+        <v>1219</v>
       </c>
       <c r="V96" t="s">
-        <v>1217</v>
+        <v>1216</v>
       </c>
     </row>
     <row r="97" spans="1:22" x14ac:dyDescent="0.25">
@@ -10803,7 +10830,7 @@
         <v>466</v>
       </c>
       <c r="I98" t="s">
-        <v>1225</v>
+        <v>1224</v>
       </c>
       <c r="J98" t="s">
         <v>462</v>
@@ -10818,25 +10845,25 @@
         <v>511</v>
       </c>
       <c r="O98" s="8" t="s">
-        <v>1222</v>
+        <v>1221</v>
       </c>
       <c r="P98" t="s">
         <v>626</v>
       </c>
       <c r="R98" t="s">
-        <v>1221</v>
+        <v>1220</v>
       </c>
       <c r="S98" t="s">
-        <v>1224</v>
+        <v>1223</v>
       </c>
       <c r="T98" t="s">
-        <v>951</v>
+        <v>950</v>
       </c>
       <c r="U98" t="s">
-        <v>1226</v>
+        <v>1225</v>
       </c>
       <c r="V98" t="s">
-        <v>1223</v>
+        <v>1222</v>
       </c>
     </row>
     <row r="99" spans="1:22" x14ac:dyDescent="0.25">
@@ -10859,34 +10886,34 @@
         <v>466</v>
       </c>
       <c r="I99" t="s">
+        <v>1228</v>
+      </c>
+      <c r="J99" t="s">
+        <v>457</v>
+      </c>
+      <c r="L99" t="s">
+        <v>457</v>
+      </c>
+      <c r="O99" s="8" t="s">
+        <v>1226</v>
+      </c>
+      <c r="P99" t="s">
         <v>1229</v>
       </c>
-      <c r="J99" t="s">
-        <v>457</v>
-      </c>
-      <c r="L99" t="s">
-        <v>457</v>
-      </c>
-      <c r="O99" s="8" t="s">
+      <c r="Q99" t="s">
+        <v>1230</v>
+      </c>
+      <c r="R99" t="s">
         <v>1227</v>
       </c>
-      <c r="P99" t="s">
-        <v>1230</v>
-      </c>
-      <c r="Q99" t="s">
-        <v>1231</v>
-      </c>
-      <c r="R99" t="s">
-        <v>1228</v>
-      </c>
       <c r="S99" t="s">
-        <v>912</v>
+        <v>911</v>
       </c>
       <c r="T99" t="s">
         <v>631</v>
       </c>
       <c r="U99" t="s">
-        <v>1232</v>
+        <v>1231</v>
       </c>
       <c r="V99" t="s">
         <v>7</v>
@@ -10918,25 +10945,25 @@
         <v>509</v>
       </c>
       <c r="O100" s="8" t="s">
-        <v>1233</v>
+        <v>1232</v>
       </c>
       <c r="P100" t="s">
         <v>626</v>
       </c>
       <c r="Q100" t="s">
+        <v>1233</v>
+      </c>
+      <c r="R100" t="s">
         <v>1234</v>
       </c>
-      <c r="R100" t="s">
+      <c r="S100" t="s">
         <v>1235</v>
-      </c>
-      <c r="S100" t="s">
-        <v>1236</v>
       </c>
       <c r="T100" t="s">
         <v>631</v>
       </c>
       <c r="U100" t="s">
-        <v>1237</v>
+        <v>1236</v>
       </c>
       <c r="V100" t="s">
         <v>7</v>
@@ -10965,7 +10992,7 @@
         <v>507</v>
       </c>
       <c r="I101" t="s">
-        <v>1243</v>
+        <v>1242</v>
       </c>
       <c r="J101" t="s">
         <v>461</v>
@@ -10974,25 +11001,25 @@
         <v>455</v>
       </c>
       <c r="O101" s="8" t="s">
+        <v>1237</v>
+      </c>
+      <c r="P101" t="s">
         <v>1238</v>
       </c>
-      <c r="P101" t="s">
+      <c r="Q101" t="s">
         <v>1239</v>
       </c>
-      <c r="Q101" t="s">
+      <c r="R101" t="s">
         <v>1240</v>
       </c>
-      <c r="R101" t="s">
-        <v>1241</v>
-      </c>
       <c r="S101" t="s">
-        <v>912</v>
+        <v>911</v>
       </c>
       <c r="T101" t="s">
         <v>668</v>
       </c>
       <c r="U101" t="s">
-        <v>1242</v>
+        <v>1241</v>
       </c>
       <c r="V101" t="s">
         <v>7</v>
@@ -11021,7 +11048,7 @@
         <v>507</v>
       </c>
       <c r="I102" s="6" t="s">
-        <v>1250</v>
+        <v>1249</v>
       </c>
       <c r="J102" t="s">
         <v>457</v>
@@ -11030,28 +11057,28 @@
         <v>457</v>
       </c>
       <c r="O102" s="8" t="s">
+        <v>1243</v>
+      </c>
+      <c r="P102" t="s">
         <v>1244</v>
       </c>
-      <c r="P102" t="s">
+      <c r="Q102" t="s">
         <v>1245</v>
       </c>
-      <c r="Q102" t="s">
+      <c r="R102" t="s">
         <v>1246</v>
       </c>
-      <c r="R102" t="s">
+      <c r="S102" t="s">
         <v>1247</v>
-      </c>
-      <c r="S102" t="s">
-        <v>1248</v>
       </c>
       <c r="T102" t="s">
         <v>631</v>
       </c>
       <c r="U102" t="s">
-        <v>1251</v>
+        <v>1250</v>
       </c>
       <c r="V102" t="s">
-        <v>1249</v>
+        <v>1248</v>
       </c>
     </row>
     <row r="103" spans="1:22" x14ac:dyDescent="0.25">
@@ -11189,7 +11216,7 @@
         <v>474</v>
       </c>
       <c r="I105" t="s">
-        <v>1257</v>
+        <v>1256</v>
       </c>
       <c r="J105" t="s">
         <v>457</v>
@@ -11198,28 +11225,28 @@
         <v>457</v>
       </c>
       <c r="O105" s="8" t="s">
+        <v>1251</v>
+      </c>
+      <c r="P105" t="s">
         <v>1252</v>
       </c>
-      <c r="P105" t="s">
+      <c r="Q105" t="s">
         <v>1253</v>
       </c>
-      <c r="Q105" t="s">
+      <c r="R105" t="s">
         <v>1254</v>
       </c>
-      <c r="R105" t="s">
+      <c r="S105" t="s">
         <v>1255</v>
-      </c>
-      <c r="S105" t="s">
-        <v>1256</v>
       </c>
       <c r="T105" t="s">
         <v>668</v>
       </c>
       <c r="U105" t="s">
+        <v>1257</v>
+      </c>
+      <c r="V105" t="s">
         <v>1258</v>
-      </c>
-      <c r="V105" t="s">
-        <v>1259</v>
       </c>
     </row>
     <row r="106" spans="1:22" x14ac:dyDescent="0.25">
@@ -11248,22 +11275,22 @@
         <v>511</v>
       </c>
       <c r="O106" s="8" t="s">
-        <v>1260</v>
+        <v>1259</v>
       </c>
       <c r="P106" t="s">
         <v>780</v>
       </c>
       <c r="R106" t="s">
+        <v>1260</v>
+      </c>
+      <c r="S106" t="s">
         <v>1261</v>
-      </c>
-      <c r="S106" t="s">
-        <v>1262</v>
       </c>
       <c r="T106" t="s">
         <v>631</v>
       </c>
       <c r="U106" t="s">
-        <v>1262</v>
+        <v>1261</v>
       </c>
       <c r="V106" t="s">
         <v>7</v>
@@ -11345,7 +11372,7 @@
         <v>467</v>
       </c>
       <c r="I108" t="s">
-        <v>1267</v>
+        <v>1266</v>
       </c>
       <c r="J108" t="s">
         <v>453</v>
@@ -11360,25 +11387,25 @@
         <v>455</v>
       </c>
       <c r="O108" s="8" t="s">
+        <v>1263</v>
+      </c>
+      <c r="P108" t="s">
+        <v>915</v>
+      </c>
+      <c r="Q108" t="s">
         <v>1264</v>
       </c>
-      <c r="P108" t="s">
-        <v>916</v>
-      </c>
-      <c r="Q108" t="s">
+      <c r="S108" t="s">
         <v>1265</v>
-      </c>
-      <c r="S108" t="s">
-        <v>1266</v>
       </c>
       <c r="T108" t="s">
         <v>631</v>
       </c>
       <c r="U108" t="s">
+        <v>1267</v>
+      </c>
+      <c r="V108" t="s">
         <v>1268</v>
-      </c>
-      <c r="V108" t="s">
-        <v>1269</v>
       </c>
     </row>
     <row r="109" spans="1:22" x14ac:dyDescent="0.25">
@@ -11401,7 +11428,7 @@
         <v>507</v>
       </c>
       <c r="I109" t="s">
-        <v>1272</v>
+        <v>1271</v>
       </c>
       <c r="J109" t="s">
         <v>462</v>
@@ -11410,16 +11437,16 @@
         <v>509</v>
       </c>
       <c r="O109" s="8" t="s">
+        <v>1269</v>
+      </c>
+      <c r="S109" t="s">
         <v>1270</v>
-      </c>
-      <c r="S109" t="s">
-        <v>1271</v>
       </c>
       <c r="T109" t="s">
         <v>668</v>
       </c>
       <c r="U109" t="s">
-        <v>1273</v>
+        <v>1272</v>
       </c>
       <c r="V109" t="s">
         <v>7</v>
@@ -11448,7 +11475,7 @@
         <v>501</v>
       </c>
       <c r="I110" t="s">
-        <v>1277</v>
+        <v>1276</v>
       </c>
       <c r="J110" t="s">
         <v>511</v>
@@ -11457,13 +11484,13 @@
         <v>511</v>
       </c>
       <c r="O110" s="8" t="s">
-        <v>1275</v>
+        <v>1274</v>
       </c>
       <c r="P110" t="s">
         <v>640</v>
       </c>
       <c r="Q110" t="s">
-        <v>1276</v>
+        <v>1275</v>
       </c>
       <c r="S110" t="s">
         <v>708</v>
@@ -11472,10 +11499,10 @@
         <v>631</v>
       </c>
       <c r="U110" t="s">
-        <v>1152</v>
+        <v>1151</v>
       </c>
       <c r="V110" t="s">
-        <v>1274</v>
+        <v>1273</v>
       </c>
     </row>
     <row r="111" spans="1:22" x14ac:dyDescent="0.25">
@@ -11498,7 +11525,7 @@
         <v>465</v>
       </c>
       <c r="I111" t="s">
-        <v>1279</v>
+        <v>1278</v>
       </c>
       <c r="J111" t="s">
         <v>462</v>
@@ -11507,22 +11534,22 @@
         <v>509</v>
       </c>
       <c r="O111" s="8" t="s">
-        <v>1278</v>
+        <v>1277</v>
       </c>
       <c r="P111" t="s">
         <v>780</v>
       </c>
       <c r="R111" t="s">
+        <v>1279</v>
+      </c>
+      <c r="S111" t="s">
         <v>1280</v>
-      </c>
-      <c r="S111" t="s">
-        <v>1281</v>
       </c>
       <c r="T111" t="s">
         <v>631</v>
       </c>
       <c r="U111" t="s">
-        <v>1282</v>
+        <v>1281</v>
       </c>
       <c r="V111" t="s">
         <v>7</v>
@@ -11554,25 +11581,25 @@
         <v>457</v>
       </c>
       <c r="O112" s="8" t="s">
+        <v>1282</v>
+      </c>
+      <c r="P112" t="s">
         <v>1283</v>
       </c>
-      <c r="P112" t="s">
+      <c r="Q112" t="s">
         <v>1284</v>
       </c>
-      <c r="Q112" t="s">
+      <c r="R112" t="s">
         <v>1285</v>
       </c>
-      <c r="R112" t="s">
+      <c r="S112" t="s">
         <v>1286</v>
-      </c>
-      <c r="S112" t="s">
-        <v>1287</v>
       </c>
       <c r="T112" t="s">
         <v>631</v>
       </c>
       <c r="U112" t="s">
-        <v>1288</v>
+        <v>1287</v>
       </c>
     </row>
     <row r="113" spans="1:22" x14ac:dyDescent="0.25">
@@ -11595,7 +11622,7 @@
         <v>480</v>
       </c>
       <c r="I113" t="s">
-        <v>1290</v>
+        <v>1289</v>
       </c>
       <c r="J113" t="s">
         <v>511</v>
@@ -11604,19 +11631,19 @@
         <v>511</v>
       </c>
       <c r="O113" s="8" t="s">
-        <v>1289</v>
+        <v>1288</v>
       </c>
       <c r="S113" t="s">
         <v>708</v>
       </c>
       <c r="T113" t="s">
-        <v>1120</v>
+        <v>1119</v>
       </c>
       <c r="U113" t="s">
-        <v>1292</v>
+        <v>1291</v>
       </c>
       <c r="V113" t="s">
-        <v>1291</v>
+        <v>1290</v>
       </c>
     </row>
     <row r="114" spans="1:22" x14ac:dyDescent="0.25">
@@ -11648,22 +11675,22 @@
         <v>453</v>
       </c>
       <c r="O114" s="8" t="s">
+        <v>1292</v>
+      </c>
+      <c r="P114" t="s">
         <v>1293</v>
       </c>
-      <c r="P114" t="s">
+      <c r="R114" t="s">
         <v>1294</v>
       </c>
-      <c r="R114" t="s">
+      <c r="S114" t="s">
         <v>1295</v>
-      </c>
-      <c r="S114" t="s">
-        <v>1296</v>
       </c>
       <c r="T114" t="s">
         <v>668</v>
       </c>
       <c r="U114" t="s">
-        <v>1297</v>
+        <v>1296</v>
       </c>
       <c r="V114" t="s">
         <v>7</v>
@@ -11695,25 +11722,25 @@
         <v>457</v>
       </c>
       <c r="O115" s="8" t="s">
-        <v>1298</v>
+        <v>1297</v>
       </c>
       <c r="P115" t="s">
-        <v>936</v>
+        <v>935</v>
       </c>
       <c r="R115" t="s">
+        <v>1299</v>
+      </c>
+      <c r="S115" t="s">
         <v>1300</v>
-      </c>
-      <c r="S115" t="s">
-        <v>1301</v>
       </c>
       <c r="T115" t="s">
         <v>631</v>
       </c>
       <c r="U115" t="s">
-        <v>1302</v>
+        <v>1301</v>
       </c>
       <c r="V115" t="s">
-        <v>1299</v>
+        <v>1298</v>
       </c>
     </row>
     <row r="116" spans="1:22" x14ac:dyDescent="0.25">
@@ -11742,19 +11769,19 @@
         <v>511</v>
       </c>
       <c r="O116" s="8" t="s">
-        <v>1303</v>
+        <v>1302</v>
       </c>
       <c r="P116" t="s">
         <v>780</v>
       </c>
       <c r="S116" t="s">
-        <v>1262</v>
+        <v>1261</v>
       </c>
       <c r="T116" t="s">
+        <v>1303</v>
+      </c>
+      <c r="U116" t="s">
         <v>1304</v>
-      </c>
-      <c r="U116" t="s">
-        <v>1305</v>
       </c>
       <c r="V116" t="s">
         <v>7</v>
@@ -11780,7 +11807,7 @@
         <v>467</v>
       </c>
       <c r="I117" t="s">
-        <v>1308</v>
+        <v>1307</v>
       </c>
       <c r="J117" t="s">
         <v>511</v>
@@ -11789,19 +11816,19 @@
         <v>511</v>
       </c>
       <c r="O117" s="8" t="s">
-        <v>1306</v>
+        <v>1305</v>
       </c>
       <c r="P117" t="s">
         <v>712</v>
       </c>
       <c r="S117" t="s">
-        <v>1307</v>
+        <v>1306</v>
       </c>
       <c r="T117" t="s">
         <v>647</v>
       </c>
       <c r="U117" t="s">
-        <v>1309</v>
+        <v>1308</v>
       </c>
       <c r="V117" t="s">
         <v>7</v>
@@ -11842,22 +11869,22 @@
         <v>511</v>
       </c>
       <c r="O118" s="8" t="s">
+        <v>1310</v>
+      </c>
+      <c r="P118" t="s">
+        <v>1309</v>
+      </c>
+      <c r="S118" t="s">
         <v>1311</v>
-      </c>
-      <c r="P118" t="s">
-        <v>1310</v>
-      </c>
-      <c r="S118" t="s">
-        <v>1312</v>
       </c>
       <c r="T118" t="s">
         <v>668</v>
       </c>
       <c r="U118" t="s">
-        <v>1314</v>
+        <v>1313</v>
       </c>
       <c r="V118" t="s">
-        <v>1313</v>
+        <v>1312</v>
       </c>
     </row>
     <row r="119" spans="1:22" x14ac:dyDescent="0.25">
@@ -11880,7 +11907,7 @@
         <v>466</v>
       </c>
       <c r="I119" t="s">
-        <v>1316</v>
+        <v>1315</v>
       </c>
       <c r="J119" t="s">
         <v>457</v>
@@ -11889,25 +11916,25 @@
         <v>457</v>
       </c>
       <c r="O119" s="8" t="s">
-        <v>1315</v>
+        <v>1314</v>
       </c>
       <c r="P119" t="s">
         <v>784</v>
       </c>
       <c r="Q119" t="s">
+        <v>1316</v>
+      </c>
+      <c r="R119" t="s">
         <v>1317</v>
       </c>
-      <c r="R119" t="s">
-        <v>1318</v>
-      </c>
       <c r="S119" t="s">
-        <v>925</v>
+        <v>924</v>
       </c>
       <c r="T119" t="s">
         <v>631</v>
       </c>
       <c r="U119" t="s">
-        <v>1319</v>
+        <v>1318</v>
       </c>
       <c r="V119" t="s">
         <v>7</v>
@@ -11936,7 +11963,7 @@
         <v>467</v>
       </c>
       <c r="I120" t="s">
-        <v>1325</v>
+        <v>1324</v>
       </c>
       <c r="J120" t="s">
         <v>457</v>
@@ -11945,25 +11972,25 @@
         <v>457</v>
       </c>
       <c r="O120" s="8" t="s">
-        <v>1320</v>
+        <v>1319</v>
       </c>
       <c r="P120" t="s">
         <v>806</v>
       </c>
       <c r="Q120" t="s">
+        <v>1320</v>
+      </c>
+      <c r="R120" t="s">
         <v>1321</v>
       </c>
-      <c r="R120" t="s">
+      <c r="S120" t="s">
         <v>1322</v>
-      </c>
-      <c r="S120" t="s">
-        <v>1323</v>
       </c>
       <c r="T120" t="s">
         <v>631</v>
       </c>
       <c r="U120" t="s">
-        <v>1324</v>
+        <v>1323</v>
       </c>
       <c r="V120" t="s">
         <v>7</v>
@@ -11989,7 +12016,7 @@
         <v>466</v>
       </c>
       <c r="I121" t="s">
-        <v>1330</v>
+        <v>1329</v>
       </c>
       <c r="J121" t="s">
         <v>457</v>
@@ -11998,16 +12025,16 @@
         <v>457</v>
       </c>
       <c r="O121" s="8" t="s">
-        <v>1326</v>
+        <v>1325</v>
       </c>
       <c r="P121" t="s">
         <v>784</v>
       </c>
       <c r="Q121" t="s">
+        <v>1326</v>
+      </c>
+      <c r="R121" t="s">
         <v>1327</v>
-      </c>
-      <c r="R121" t="s">
-        <v>1328</v>
       </c>
       <c r="S121" t="s">
         <v>787</v>
@@ -12016,7 +12043,7 @@
         <v>631</v>
       </c>
       <c r="U121" t="s">
-        <v>1329</v>
+        <v>1328</v>
       </c>
       <c r="V121" t="s">
         <v>7</v>
@@ -12045,7 +12072,7 @@
         <v>467</v>
       </c>
       <c r="I122" t="s">
-        <v>1331</v>
+        <v>1330</v>
       </c>
       <c r="J122" t="s">
         <v>511</v>
@@ -12054,19 +12081,19 @@
         <v>511</v>
       </c>
       <c r="O122" s="8" t="s">
-        <v>1332</v>
+        <v>1331</v>
       </c>
       <c r="P122" t="s">
         <v>712</v>
       </c>
       <c r="S122" t="s">
-        <v>1333</v>
+        <v>1332</v>
       </c>
       <c r="T122" t="s">
         <v>631</v>
       </c>
       <c r="U122" t="s">
-        <v>1334</v>
+        <v>1333</v>
       </c>
       <c r="V122" t="s">
         <v>7</v>
@@ -12098,13 +12125,13 @@
         <v>453</v>
       </c>
       <c r="O123" s="8" t="s">
+        <v>1334</v>
+      </c>
+      <c r="P123" t="s">
         <v>1335</v>
       </c>
-      <c r="P123" t="s">
+      <c r="Q123" t="s">
         <v>1336</v>
-      </c>
-      <c r="Q123" t="s">
-        <v>1337</v>
       </c>
       <c r="S123" t="s">
         <v>854</v>
@@ -12113,7 +12140,7 @@
         <v>631</v>
       </c>
       <c r="U123" t="s">
-        <v>1338</v>
+        <v>1337</v>
       </c>
       <c r="V123" t="s">
         <v>7</v>
@@ -12145,19 +12172,19 @@
         <v>454</v>
       </c>
       <c r="O124" s="8" t="s">
-        <v>1339</v>
+        <v>1338</v>
       </c>
       <c r="P124" t="s">
         <v>626</v>
       </c>
       <c r="S124" t="s">
-        <v>1341</v>
+        <v>1340</v>
       </c>
       <c r="T124" t="s">
         <v>668</v>
       </c>
       <c r="U124" t="s">
-        <v>1340</v>
+        <v>1339</v>
       </c>
       <c r="V124" t="s">
         <v>7</v>
@@ -12292,7 +12319,7 @@
         <v>501</v>
       </c>
       <c r="I127" t="s">
-        <v>1343</v>
+        <v>1342</v>
       </c>
       <c r="J127" t="s">
         <v>462</v>
@@ -12301,25 +12328,25 @@
         <v>509</v>
       </c>
       <c r="O127" s="8" t="s">
-        <v>1342</v>
+        <v>1341</v>
       </c>
       <c r="P127" t="s">
-        <v>1028</v>
+        <v>1027</v>
       </c>
       <c r="R127" t="s">
+        <v>1343</v>
+      </c>
+      <c r="S127" t="s">
         <v>1344</v>
-      </c>
-      <c r="S127" t="s">
-        <v>1345</v>
       </c>
       <c r="T127" t="s">
         <v>631</v>
       </c>
       <c r="U127" t="s">
-        <v>1347</v>
+        <v>1346</v>
       </c>
       <c r="V127" t="s">
-        <v>1346</v>
+        <v>1345</v>
       </c>
     </row>
     <row r="128" spans="1:22" x14ac:dyDescent="0.25">
@@ -12345,7 +12372,7 @@
         <v>467</v>
       </c>
       <c r="I128" t="s">
-        <v>1349</v>
+        <v>1348</v>
       </c>
       <c r="J128" t="s">
         <v>458</v>
@@ -12360,25 +12387,25 @@
         <v>457</v>
       </c>
       <c r="O128" s="8" t="s">
-        <v>1348</v>
+        <v>1347</v>
       </c>
       <c r="P128" t="s">
-        <v>1245</v>
+        <v>1244</v>
       </c>
       <c r="Q128" t="s">
-        <v>1352</v>
+        <v>1351</v>
       </c>
       <c r="R128" t="s">
+        <v>1349</v>
+      </c>
+      <c r="S128" t="s">
         <v>1350</v>
-      </c>
-      <c r="S128" t="s">
-        <v>1351</v>
       </c>
       <c r="T128" t="s">
         <v>631</v>
       </c>
       <c r="U128" t="s">
-        <v>1353</v>
+        <v>1352</v>
       </c>
       <c r="V128" t="s">
         <v>7</v>
@@ -12404,7 +12431,7 @@
         <v>466</v>
       </c>
       <c r="I129" t="s">
-        <v>1357</v>
+        <v>1356</v>
       </c>
       <c r="J129" t="s">
         <v>457</v>
@@ -12413,25 +12440,25 @@
         <v>457</v>
       </c>
       <c r="O129" s="8" t="s">
-        <v>1354</v>
+        <v>1353</v>
       </c>
       <c r="P129" t="s">
         <v>658</v>
       </c>
       <c r="Q129" t="s">
+        <v>1354</v>
+      </c>
+      <c r="R129" t="s">
         <v>1355</v>
       </c>
-      <c r="R129" t="s">
-        <v>1356</v>
-      </c>
       <c r="S129" t="s">
-        <v>1256</v>
+        <v>1255</v>
       </c>
       <c r="T129" t="s">
         <v>631</v>
       </c>
       <c r="U129" t="s">
-        <v>1358</v>
+        <v>1357</v>
       </c>
       <c r="V129" t="s">
         <v>7</v>
@@ -12463,25 +12490,25 @@
         <v>457</v>
       </c>
       <c r="O130" s="8" t="s">
-        <v>1359</v>
+        <v>1358</v>
       </c>
       <c r="P130" t="s">
         <v>700</v>
       </c>
       <c r="Q130" t="s">
+        <v>1359</v>
+      </c>
+      <c r="R130" t="s">
         <v>1360</v>
       </c>
-      <c r="R130" t="s">
+      <c r="S130" t="s">
         <v>1361</v>
-      </c>
-      <c r="S130" t="s">
-        <v>1362</v>
       </c>
       <c r="T130" t="s">
         <v>631</v>
       </c>
       <c r="U130" t="s">
-        <v>1363</v>
+        <v>1362</v>
       </c>
       <c r="V130" t="s">
         <v>7</v>
@@ -12513,22 +12540,22 @@
         <v>455</v>
       </c>
       <c r="O131" s="8" t="s">
-        <v>1364</v>
+        <v>1363</v>
       </c>
       <c r="P131" t="s">
         <v>626</v>
       </c>
       <c r="Q131" t="s">
+        <v>1364</v>
+      </c>
+      <c r="S131" t="s">
         <v>1365</v>
-      </c>
-      <c r="S131" t="s">
-        <v>1366</v>
       </c>
       <c r="T131" t="s">
         <v>631</v>
       </c>
       <c r="U131" t="s">
-        <v>1367</v>
+        <v>1366</v>
       </c>
       <c r="V131" t="s">
         <v>7</v>
@@ -12563,25 +12590,25 @@
         <v>509</v>
       </c>
       <c r="O132" s="8" t="s">
+        <v>1367</v>
+      </c>
+      <c r="P132" t="s">
         <v>1368</v>
       </c>
-      <c r="P132" t="s">
+      <c r="Q132" t="s">
         <v>1369</v>
       </c>
-      <c r="Q132" t="s">
+      <c r="R132" t="s">
         <v>1370</v>
       </c>
-      <c r="R132" t="s">
-        <v>1371</v>
-      </c>
       <c r="S132" t="s">
-        <v>1271</v>
+        <v>1270</v>
       </c>
       <c r="T132" t="s">
         <v>668</v>
       </c>
       <c r="U132" t="s">
-        <v>1372</v>
+        <v>1371</v>
       </c>
       <c r="V132" t="s">
         <v>7</v>
@@ -12616,22 +12643,22 @@
         <v>509</v>
       </c>
       <c r="O133" s="8" t="s">
+        <v>1372</v>
+      </c>
+      <c r="P133" t="s">
+        <v>1262</v>
+      </c>
+      <c r="Q133" t="s">
         <v>1373</v>
       </c>
-      <c r="P133" t="s">
-        <v>1263</v>
-      </c>
-      <c r="Q133" t="s">
-        <v>1374</v>
-      </c>
       <c r="S133" t="s">
-        <v>1345</v>
+        <v>1344</v>
       </c>
       <c r="T133" t="s">
         <v>631</v>
       </c>
       <c r="U133" t="s">
-        <v>1375</v>
+        <v>1374</v>
       </c>
     </row>
     <row r="134" spans="1:22" x14ac:dyDescent="0.25">
@@ -12654,7 +12681,7 @@
         <v>474</v>
       </c>
       <c r="I134" t="s">
-        <v>1379</v>
+        <v>1378</v>
       </c>
       <c r="J134" t="s">
         <v>509</v>
@@ -12663,19 +12690,19 @@
         <v>509</v>
       </c>
       <c r="O134" s="8" t="s">
-        <v>1376</v>
+        <v>1375</v>
       </c>
       <c r="S134" t="s">
-        <v>1378</v>
+        <v>1377</v>
       </c>
       <c r="T134" t="s">
         <v>631</v>
       </c>
       <c r="U134" t="s">
-        <v>1380</v>
+        <v>1379</v>
       </c>
       <c r="V134" t="s">
-        <v>1377</v>
+        <v>1376</v>
       </c>
     </row>
     <row r="135" spans="1:22" x14ac:dyDescent="0.25">
@@ -12704,19 +12731,19 @@
         <v>457</v>
       </c>
       <c r="O135" s="8" t="s">
-        <v>1381</v>
+        <v>1380</v>
       </c>
       <c r="P135" t="s">
         <v>780</v>
       </c>
       <c r="S135" t="s">
-        <v>1382</v>
+        <v>1381</v>
       </c>
       <c r="T135" t="s">
         <v>631</v>
       </c>
       <c r="U135" t="s">
-        <v>1383</v>
+        <v>1382</v>
       </c>
       <c r="V135" t="s">
         <v>7</v>
@@ -12742,7 +12769,7 @@
         <v>466</v>
       </c>
       <c r="I136" t="s">
-        <v>1391</v>
+        <v>1390</v>
       </c>
       <c r="J136" t="s">
         <v>463</v>
@@ -12754,25 +12781,25 @@
         <v>456</v>
       </c>
       <c r="O136" s="8" t="s">
+        <v>1383</v>
+      </c>
+      <c r="P136" t="s">
         <v>1384</v>
       </c>
-      <c r="P136" t="s">
+      <c r="Q136" t="s">
         <v>1385</v>
       </c>
-      <c r="Q136" t="s">
+      <c r="R136" t="s">
         <v>1386</v>
       </c>
-      <c r="R136" t="s">
+      <c r="S136" t="s">
         <v>1387</v>
       </c>
-      <c r="S136" t="s">
+      <c r="T136" t="s">
         <v>1388</v>
       </c>
-      <c r="T136" t="s">
+      <c r="U136" t="s">
         <v>1389</v>
-      </c>
-      <c r="U136" t="s">
-        <v>1390</v>
       </c>
       <c r="V136" t="s">
         <v>7</v>
@@ -12798,7 +12825,7 @@
         <v>466</v>
       </c>
       <c r="I137" t="s">
-        <v>1393</v>
+        <v>1392</v>
       </c>
       <c r="J137" t="s">
         <v>511</v>
@@ -12807,16 +12834,16 @@
         <v>511</v>
       </c>
       <c r="O137" s="8" t="s">
-        <v>1392</v>
+        <v>1391</v>
       </c>
       <c r="S137" t="s">
-        <v>1333</v>
+        <v>1332</v>
       </c>
       <c r="T137" t="s">
         <v>668</v>
       </c>
       <c r="U137" t="s">
-        <v>1394</v>
+        <v>1393</v>
       </c>
       <c r="V137" t="s">
         <v>7</v>
@@ -12842,7 +12869,7 @@
         <v>466</v>
       </c>
       <c r="I138" t="s">
-        <v>1400</v>
+        <v>1399</v>
       </c>
       <c r="J138" t="s">
         <v>460</v>
@@ -12857,25 +12884,25 @@
         <v>457</v>
       </c>
       <c r="O138" s="8" t="s">
+        <v>1394</v>
+      </c>
+      <c r="P138" t="s">
+        <v>1033</v>
+      </c>
+      <c r="Q138" t="s">
         <v>1395</v>
       </c>
-      <c r="P138" t="s">
-        <v>1034</v>
-      </c>
-      <c r="Q138" t="s">
+      <c r="R138" t="s">
         <v>1396</v>
       </c>
-      <c r="R138" t="s">
+      <c r="S138" t="s">
         <v>1397</v>
-      </c>
-      <c r="S138" t="s">
-        <v>1398</v>
       </c>
       <c r="T138" t="s">
         <v>668</v>
       </c>
       <c r="U138" t="s">
-        <v>1399</v>
+        <v>1398</v>
       </c>
       <c r="V138" t="s">
         <v>7</v>
@@ -12907,16 +12934,16 @@
         <v>454</v>
       </c>
       <c r="O139" s="8" t="s">
-        <v>1401</v>
+        <v>1400</v>
       </c>
       <c r="S139" t="s">
-        <v>1403</v>
+        <v>1402</v>
       </c>
       <c r="T139" t="s">
         <v>631</v>
       </c>
       <c r="U139" t="s">
-        <v>1402</v>
+        <v>1401</v>
       </c>
       <c r="V139" t="s">
         <v>7</v>
@@ -12948,7 +12975,7 @@
         <v>511</v>
       </c>
       <c r="O140" s="8" t="s">
-        <v>1404</v>
+        <v>1403</v>
       </c>
       <c r="R140" t="s">
         <v>41</v>
@@ -12957,10 +12984,10 @@
         <v>787</v>
       </c>
       <c r="T140" t="s">
-        <v>951</v>
+        <v>950</v>
       </c>
       <c r="U140" t="s">
-        <v>1408</v>
+        <v>1407</v>
       </c>
       <c r="V140" t="s">
         <v>7</v>
@@ -12989,7 +13016,7 @@
         <v>480</v>
       </c>
       <c r="I141" t="s">
-        <v>1406</v>
+        <v>1405</v>
       </c>
       <c r="J141" t="s">
         <v>511</v>
@@ -12998,25 +13025,25 @@
         <v>511</v>
       </c>
       <c r="O141" s="8" t="s">
-        <v>1405</v>
+        <v>1404</v>
       </c>
       <c r="P141" t="s">
+        <v>1409</v>
+      </c>
+      <c r="Q141" t="s">
         <v>1410</v>
       </c>
-      <c r="Q141" t="s">
+      <c r="R141" t="s">
         <v>1411</v>
-      </c>
-      <c r="R141" t="s">
-        <v>1412</v>
       </c>
       <c r="T141" t="s">
         <v>668</v>
       </c>
       <c r="U141" t="s">
-        <v>1409</v>
+        <v>1408</v>
       </c>
       <c r="V141" t="s">
-        <v>1407</v>
+        <v>1406</v>
       </c>
     </row>
     <row r="142" spans="1:22" x14ac:dyDescent="0.25">
@@ -13039,7 +13066,7 @@
         <v>467</v>
       </c>
       <c r="I142" t="s">
-        <v>1414</v>
+        <v>1413</v>
       </c>
       <c r="J142" t="s">
         <v>463</v>
@@ -13051,25 +13078,25 @@
         <v>456</v>
       </c>
       <c r="O142" s="8" t="s">
-        <v>1413</v>
+        <v>1412</v>
       </c>
       <c r="P142" t="s">
         <v>626</v>
       </c>
       <c r="Q142" t="s">
+        <v>1414</v>
+      </c>
+      <c r="R142" t="s">
         <v>1415</v>
       </c>
-      <c r="R142" t="s">
+      <c r="S142" t="s">
         <v>1416</v>
-      </c>
-      <c r="S142" t="s">
-        <v>1417</v>
       </c>
       <c r="T142" t="s">
         <v>736</v>
       </c>
       <c r="U142" t="s">
-        <v>1418</v>
+        <v>1417</v>
       </c>
       <c r="V142" t="s">
         <v>7</v>
@@ -13095,7 +13122,7 @@
         <v>487</v>
       </c>
       <c r="I143" t="s">
-        <v>1423</v>
+        <v>1422</v>
       </c>
       <c r="J143" t="s">
         <v>457</v>
@@ -13107,25 +13134,25 @@
         <v>451</v>
       </c>
       <c r="O143" s="8" t="s">
-        <v>1420</v>
+        <v>1419</v>
       </c>
       <c r="P143" t="s">
         <v>626</v>
       </c>
       <c r="Q143" t="s">
-        <v>1422</v>
+        <v>1421</v>
       </c>
       <c r="S143" t="s">
-        <v>1419</v>
+        <v>1418</v>
       </c>
       <c r="T143" t="s">
-        <v>951</v>
+        <v>950</v>
       </c>
       <c r="U143" t="s">
-        <v>1424</v>
+        <v>1423</v>
       </c>
       <c r="V143" t="s">
-        <v>1421</v>
+        <v>1420</v>
       </c>
     </row>
     <row r="144" spans="1:22" x14ac:dyDescent="0.25">
@@ -13204,7 +13231,7 @@
         <v>467</v>
       </c>
       <c r="I145" t="s">
-        <v>1430</v>
+        <v>1429</v>
       </c>
       <c r="J145" t="s">
         <v>463</v>
@@ -13213,25 +13240,25 @@
         <v>456</v>
       </c>
       <c r="O145" s="8" t="s">
+        <v>1424</v>
+      </c>
+      <c r="P145" t="s">
         <v>1425</v>
       </c>
-      <c r="P145" t="s">
+      <c r="Q145" t="s">
         <v>1426</v>
       </c>
-      <c r="Q145" t="s">
+      <c r="R145" t="s">
         <v>1427</v>
       </c>
-      <c r="R145" t="s">
+      <c r="S145" t="s">
         <v>1428</v>
-      </c>
-      <c r="S145" t="s">
-        <v>1429</v>
       </c>
       <c r="T145" t="s">
         <v>736</v>
       </c>
       <c r="U145" t="s">
-        <v>1431</v>
+        <v>1430</v>
       </c>
       <c r="V145" t="s">
         <v>7</v>
@@ -13257,7 +13284,7 @@
         <v>466</v>
       </c>
       <c r="I146" t="s">
-        <v>1435</v>
+        <v>1434</v>
       </c>
       <c r="J146" t="s">
         <v>461</v>
@@ -13266,25 +13293,25 @@
         <v>455</v>
       </c>
       <c r="O146" s="8" t="s">
-        <v>1432</v>
+        <v>1431</v>
       </c>
       <c r="P146" t="s">
         <v>626</v>
       </c>
       <c r="Q146" t="s">
-        <v>1434</v>
+        <v>1433</v>
       </c>
       <c r="R146" t="s">
-        <v>1433</v>
+        <v>1432</v>
       </c>
       <c r="S146" t="s">
-        <v>912</v>
+        <v>911</v>
       </c>
       <c r="T146" t="s">
         <v>668</v>
       </c>
       <c r="U146" t="s">
-        <v>1436</v>
+        <v>1435</v>
       </c>
       <c r="V146" t="s">
         <v>7</v>
@@ -13313,7 +13340,7 @@
         <v>474</v>
       </c>
       <c r="I147" t="s">
-        <v>1439</v>
+        <v>1438</v>
       </c>
       <c r="J147" t="s">
         <v>453</v>
@@ -13328,25 +13355,25 @@
         <v>455</v>
       </c>
       <c r="O147" s="8" t="s">
-        <v>1437</v>
+        <v>1436</v>
       </c>
       <c r="P147" t="s">
         <v>886</v>
       </c>
       <c r="Q147" t="s">
-        <v>1438</v>
+        <v>1437</v>
       </c>
       <c r="S147" t="s">
+        <v>1439</v>
+      </c>
+      <c r="T147" t="s">
+        <v>950</v>
+      </c>
+      <c r="U147" t="s">
+        <v>1441</v>
+      </c>
+      <c r="V147" t="s">
         <v>1440</v>
-      </c>
-      <c r="T147" t="s">
-        <v>951</v>
-      </c>
-      <c r="U147" t="s">
-        <v>1442</v>
-      </c>
-      <c r="V147" t="s">
-        <v>1441</v>
       </c>
     </row>
     <row r="148" spans="1:22" x14ac:dyDescent="0.25">
@@ -13369,7 +13396,7 @@
         <v>466</v>
       </c>
       <c r="I148" t="s">
-        <v>1447</v>
+        <v>1446</v>
       </c>
       <c r="J148" t="s">
         <v>509</v>
@@ -13381,22 +13408,22 @@
         <v>509</v>
       </c>
       <c r="O148" s="8" t="s">
-        <v>1443</v>
+        <v>1442</v>
       </c>
       <c r="P148" t="s">
         <v>617</v>
       </c>
       <c r="R148" t="s">
-        <v>1444</v>
+        <v>1443</v>
       </c>
       <c r="S148" t="s">
         <v>742</v>
       </c>
       <c r="T148" t="s">
+        <v>1444</v>
+      </c>
+      <c r="U148" t="s">
         <v>1445</v>
-      </c>
-      <c r="U148" t="s">
-        <v>1446</v>
       </c>
       <c r="V148" t="s">
         <v>7</v>
@@ -13422,7 +13449,7 @@
         <v>465</v>
       </c>
       <c r="I149" t="s">
-        <v>1451</v>
+        <v>1450</v>
       </c>
       <c r="J149" t="s">
         <v>457</v>
@@ -13431,22 +13458,22 @@
         <v>457</v>
       </c>
       <c r="O149" s="8" t="s">
-        <v>1448</v>
+        <v>1447</v>
       </c>
       <c r="P149" t="s">
         <v>626</v>
       </c>
       <c r="R149" t="s">
-        <v>1449</v>
+        <v>1448</v>
       </c>
       <c r="S149" t="s">
-        <v>912</v>
+        <v>911</v>
       </c>
       <c r="T149" t="s">
         <v>631</v>
       </c>
       <c r="U149" t="s">
-        <v>1450</v>
+        <v>1449</v>
       </c>
       <c r="V149" t="s">
         <v>7</v>
@@ -13475,7 +13502,7 @@
         <v>467</v>
       </c>
       <c r="I150" t="s">
-        <v>1454</v>
+        <v>1453</v>
       </c>
       <c r="J150" t="s">
         <v>457</v>
@@ -13484,22 +13511,22 @@
         <v>457</v>
       </c>
       <c r="O150" s="8" t="s">
-        <v>1452</v>
+        <v>1451</v>
       </c>
       <c r="P150" t="s">
         <v>784</v>
       </c>
       <c r="R150" t="s">
-        <v>1459</v>
+        <v>1458</v>
       </c>
       <c r="S150" t="s">
-        <v>1453</v>
+        <v>1452</v>
       </c>
       <c r="T150" t="s">
         <v>631</v>
       </c>
       <c r="U150" t="s">
-        <v>1455</v>
+        <v>1454</v>
       </c>
       <c r="V150" t="s">
         <v>7</v>
@@ -13528,7 +13555,7 @@
         <v>467</v>
       </c>
       <c r="I151" t="s">
-        <v>1461</v>
+        <v>1460</v>
       </c>
       <c r="J151" t="s">
         <v>457</v>
@@ -13537,22 +13564,22 @@
         <v>457</v>
       </c>
       <c r="O151" s="8" t="s">
+        <v>1455</v>
+      </c>
+      <c r="P151" t="s">
         <v>1456</v>
       </c>
-      <c r="P151" t="s">
+      <c r="R151" t="s">
         <v>1457</v>
       </c>
-      <c r="R151" t="s">
-        <v>1458</v>
-      </c>
       <c r="S151" t="s">
-        <v>1460</v>
+        <v>1459</v>
       </c>
       <c r="T151" t="s">
         <v>631</v>
       </c>
       <c r="U151" t="s">
-        <v>1462</v>
+        <v>1461</v>
       </c>
       <c r="V151" t="s">
         <v>7</v>
@@ -13578,7 +13605,7 @@
         <v>467</v>
       </c>
       <c r="I152" t="s">
-        <v>1467</v>
+        <v>1466</v>
       </c>
       <c r="J152" t="s">
         <v>511</v>
@@ -13587,19 +13614,19 @@
         <v>511</v>
       </c>
       <c r="O152" s="8" t="s">
+        <v>1462</v>
+      </c>
+      <c r="R152" t="s">
         <v>1463</v>
       </c>
-      <c r="R152" t="s">
+      <c r="S152" t="s">
         <v>1464</v>
-      </c>
-      <c r="S152" t="s">
-        <v>1465</v>
       </c>
       <c r="T152" t="s">
         <v>631</v>
       </c>
       <c r="U152" t="s">
-        <v>1466</v>
+        <v>1465</v>
       </c>
       <c r="V152" t="s">
         <v>7</v>
@@ -13625,7 +13652,7 @@
         <v>466</v>
       </c>
       <c r="I153" t="s">
-        <v>1473</v>
+        <v>1472</v>
       </c>
       <c r="J153" t="s">
         <v>461</v>
@@ -13640,25 +13667,25 @@
         <v>454</v>
       </c>
       <c r="O153" s="8" t="s">
-        <v>1469</v>
+        <v>1468</v>
       </c>
       <c r="P153" t="s">
         <v>626</v>
       </c>
       <c r="Q153" t="s">
-        <v>1468</v>
+        <v>1467</v>
       </c>
       <c r="R153" t="s">
+        <v>1469</v>
+      </c>
+      <c r="S153" t="s">
         <v>1470</v>
-      </c>
-      <c r="S153" t="s">
-        <v>1471</v>
       </c>
       <c r="T153" t="s">
         <v>668</v>
       </c>
       <c r="U153" t="s">
-        <v>1472</v>
+        <v>1471</v>
       </c>
       <c r="V153" t="s">
         <v>7</v>
@@ -13696,28 +13723,28 @@
         <v>509</v>
       </c>
       <c r="O154" s="8" t="s">
-        <v>1474</v>
+        <v>1473</v>
       </c>
       <c r="P154" t="s">
         <v>626</v>
       </c>
       <c r="Q154" t="s">
+        <v>1474</v>
+      </c>
+      <c r="R154" t="s">
         <v>1475</v>
       </c>
-      <c r="R154" t="s">
+      <c r="S154" t="s">
         <v>1476</v>
       </c>
-      <c r="S154" t="s">
+      <c r="T154" t="s">
         <v>1477</v>
       </c>
-      <c r="T154" t="s">
+      <c r="U154" t="s">
         <v>1478</v>
       </c>
-      <c r="U154" t="s">
+      <c r="V154" t="s">
         <v>1479</v>
-      </c>
-      <c r="V154" t="s">
-        <v>1480</v>
       </c>
     </row>
     <row r="155" spans="1:22" x14ac:dyDescent="0.25">
@@ -13792,7 +13819,7 @@
       </c>
       <c r="H156"/>
       <c r="I156" t="s">
-        <v>1485</v>
+        <v>1484</v>
       </c>
       <c r="J156" t="s">
         <v>457</v>
@@ -13808,16 +13835,16 @@
       </c>
       <c r="N156"/>
       <c r="O156" s="8" t="s">
+        <v>1480</v>
+      </c>
+      <c r="P156" t="s">
         <v>1481</v>
       </c>
-      <c r="P156" t="s">
+      <c r="Q156" t="s">
         <v>1482</v>
       </c>
-      <c r="Q156" t="s">
-        <v>1483</v>
-      </c>
       <c r="R156" t="s">
-        <v>1489</v>
+        <v>1488</v>
       </c>
       <c r="S156" t="s">
         <v>854</v>
@@ -13826,7 +13853,7 @@
         <v>668</v>
       </c>
       <c r="U156" t="s">
-        <v>1484</v>
+        <v>1483</v>
       </c>
       <c r="V156" t="s">
         <v>7</v>
@@ -13852,7 +13879,7 @@
         <v>466</v>
       </c>
       <c r="I157" t="s">
-        <v>1492</v>
+        <v>1491</v>
       </c>
       <c r="J157" t="s">
         <v>463</v>
@@ -13861,25 +13888,25 @@
         <v>456</v>
       </c>
       <c r="O157" s="8" t="s">
+        <v>1485</v>
+      </c>
+      <c r="P157" t="s">
+        <v>1089</v>
+      </c>
+      <c r="Q157" t="s">
         <v>1486</v>
       </c>
-      <c r="P157" t="s">
-        <v>1090</v>
-      </c>
-      <c r="Q157" t="s">
+      <c r="R157" t="s">
         <v>1487</v>
       </c>
-      <c r="R157" t="s">
-        <v>1488</v>
-      </c>
       <c r="S157" t="s">
-        <v>1490</v>
+        <v>1489</v>
       </c>
       <c r="T157" t="s">
         <v>736</v>
       </c>
       <c r="U157" t="s">
-        <v>1491</v>
+        <v>1490</v>
       </c>
       <c r="V157" t="s">
         <v>7</v>
@@ -13908,7 +13935,7 @@
         <v>478</v>
       </c>
       <c r="I158" t="s">
-        <v>1496</v>
+        <v>1495</v>
       </c>
       <c r="J158" t="s">
         <v>511</v>
@@ -13917,13 +13944,13 @@
         <v>511</v>
       </c>
       <c r="O158" s="8" t="s">
-        <v>1493</v>
+        <v>1492</v>
       </c>
       <c r="P158" t="s">
         <v>784</v>
       </c>
       <c r="R158" t="s">
-        <v>1494</v>
+        <v>1493</v>
       </c>
       <c r="S158" t="s">
         <v>787</v>
@@ -13932,10 +13959,10 @@
         <v>631</v>
       </c>
       <c r="U158" t="s">
-        <v>1497</v>
+        <v>1496</v>
       </c>
       <c r="V158" t="s">
-        <v>1495</v>
+        <v>1494</v>
       </c>
     </row>
     <row r="159" spans="1:22" x14ac:dyDescent="0.25">
@@ -13958,7 +13985,7 @@
         <v>466</v>
       </c>
       <c r="I159" t="s">
-        <v>1501</v>
+        <v>1500</v>
       </c>
       <c r="J159" t="s">
         <v>511</v>
@@ -13967,16 +13994,16 @@
         <v>511</v>
       </c>
       <c r="O159" s="8" t="s">
+        <v>1497</v>
+      </c>
+      <c r="S159" t="s">
         <v>1498</v>
-      </c>
-      <c r="S159" t="s">
-        <v>1499</v>
       </c>
       <c r="T159" t="s">
         <v>631</v>
       </c>
       <c r="U159" t="s">
-        <v>1500</v>
+        <v>1499</v>
       </c>
       <c r="V159" t="s">
         <v>7</v>
@@ -14008,25 +14035,25 @@
         <v>450</v>
       </c>
       <c r="O160" s="8" t="s">
-        <v>1502</v>
+        <v>1501</v>
       </c>
       <c r="P160" t="s">
         <v>626</v>
       </c>
       <c r="R160" t="s">
+        <v>1503</v>
+      </c>
+      <c r="S160" t="s">
         <v>1504</v>
-      </c>
-      <c r="S160" t="s">
-        <v>1505</v>
       </c>
       <c r="T160" t="s">
         <v>668</v>
       </c>
       <c r="U160" t="s">
-        <v>1506</v>
+        <v>1505</v>
       </c>
       <c r="V160" t="s">
-        <v>1503</v>
+        <v>1502</v>
       </c>
     </row>
     <row r="161" spans="1:22" x14ac:dyDescent="0.25">
@@ -14052,7 +14079,7 @@
         <v>480</v>
       </c>
       <c r="I161" t="s">
-        <v>1511</v>
+        <v>1510</v>
       </c>
       <c r="J161" t="s">
         <v>509</v>
@@ -14064,13 +14091,13 @@
         <v>451</v>
       </c>
       <c r="O161" s="8" t="s">
+        <v>1506</v>
+      </c>
+      <c r="P161" t="s">
         <v>1507</v>
       </c>
-      <c r="P161" t="s">
+      <c r="R161" t="s">
         <v>1508</v>
-      </c>
-      <c r="R161" t="s">
-        <v>1509</v>
       </c>
       <c r="S161" t="s">
         <v>854</v>
@@ -14079,10 +14106,10 @@
         <v>736</v>
       </c>
       <c r="U161" t="s">
-        <v>1510</v>
+        <v>1509</v>
       </c>
       <c r="V161" t="s">
-        <v>1512</v>
+        <v>1511</v>
       </c>
     </row>
     <row r="162" spans="1:22" x14ac:dyDescent="0.25">
@@ -14158,7 +14185,7 @@
         <v>480</v>
       </c>
       <c r="I163" t="s">
-        <v>1518</v>
+        <v>1517</v>
       </c>
       <c r="J163" t="s">
         <v>457</v>
@@ -14173,28 +14200,28 @@
         <v>455</v>
       </c>
       <c r="O163" s="8" t="s">
+        <v>1512</v>
+      </c>
+      <c r="P163" t="s">
         <v>1513</v>
       </c>
-      <c r="P163" t="s">
+      <c r="Q163" t="s">
         <v>1514</v>
       </c>
-      <c r="Q163" t="s">
+      <c r="R163" t="s">
         <v>1515</v>
       </c>
-      <c r="R163" t="s">
+      <c r="S163" t="s">
         <v>1516</v>
-      </c>
-      <c r="S163" t="s">
-        <v>1517</v>
       </c>
       <c r="T163" t="s">
         <v>631</v>
       </c>
       <c r="U163" t="s">
+        <v>1518</v>
+      </c>
+      <c r="V163" t="s">
         <v>1519</v>
-      </c>
-      <c r="V163" t="s">
-        <v>1520</v>
       </c>
     </row>
     <row r="164" spans="1:22" x14ac:dyDescent="0.25">
@@ -14223,25 +14250,25 @@
         <v>457</v>
       </c>
       <c r="O164" s="8" t="s">
+        <v>1520</v>
+      </c>
+      <c r="P164" t="s">
+        <v>1522</v>
+      </c>
+      <c r="Q164" t="s">
+        <v>1523</v>
+      </c>
+      <c r="R164" t="s">
         <v>1521</v>
       </c>
-      <c r="P164" t="s">
-        <v>1523</v>
-      </c>
-      <c r="Q164" t="s">
+      <c r="S164" t="s">
         <v>1524</v>
-      </c>
-      <c r="R164" t="s">
-        <v>1522</v>
-      </c>
-      <c r="S164" t="s">
-        <v>1525</v>
       </c>
       <c r="T164" t="s">
         <v>668</v>
       </c>
       <c r="U164" t="s">
-        <v>1526</v>
+        <v>1525</v>
       </c>
       <c r="V164" t="s">
         <v>7</v>
@@ -14273,25 +14300,25 @@
         <v>457</v>
       </c>
       <c r="O165" s="8" t="s">
-        <v>1527</v>
+        <v>1526</v>
       </c>
       <c r="P165" t="s">
         <v>626</v>
       </c>
       <c r="Q165" t="s">
+        <v>1527</v>
+      </c>
+      <c r="R165" t="s">
         <v>1528</v>
       </c>
-      <c r="R165" t="s">
+      <c r="S165" t="s">
         <v>1529</v>
-      </c>
-      <c r="S165" t="s">
-        <v>1530</v>
       </c>
       <c r="T165" t="s">
         <v>668</v>
       </c>
       <c r="U165" t="s">
-        <v>1531</v>
+        <v>1530</v>
       </c>
       <c r="V165" t="s">
         <v>7</v>
@@ -14323,25 +14350,25 @@
         <v>457</v>
       </c>
       <c r="O166" s="8" t="s">
-        <v>1532</v>
+        <v>1531</v>
       </c>
       <c r="P166" t="s">
         <v>626</v>
       </c>
       <c r="Q166" t="s">
-        <v>892</v>
+        <v>891</v>
       </c>
       <c r="R166" t="s">
+        <v>1532</v>
+      </c>
+      <c r="S166" t="s">
         <v>1533</v>
-      </c>
-      <c r="S166" t="s">
-        <v>1534</v>
       </c>
       <c r="T166" t="s">
         <v>647</v>
       </c>
       <c r="U166" t="s">
-        <v>1535</v>
+        <v>1534</v>
       </c>
       <c r="V166" t="s">
         <v>7</v>
@@ -14370,7 +14397,7 @@
         <v>466</v>
       </c>
       <c r="I167" t="s">
-        <v>1540</v>
+        <v>1539</v>
       </c>
       <c r="J167" t="s">
         <v>463</v>
@@ -14382,16 +14409,16 @@
         <v>456</v>
       </c>
       <c r="O167" s="8" t="s">
+        <v>1535</v>
+      </c>
+      <c r="P167" t="s">
         <v>1536</v>
       </c>
-      <c r="P167" t="s">
+      <c r="Q167" t="s">
         <v>1537</v>
       </c>
-      <c r="Q167" t="s">
+      <c r="R167" t="s">
         <v>1538</v>
-      </c>
-      <c r="R167" t="s">
-        <v>1539</v>
       </c>
       <c r="S167" t="s">
         <v>742</v>
@@ -14400,7 +14427,7 @@
         <v>631</v>
       </c>
       <c r="U167" t="s">
-        <v>1541</v>
+        <v>1540</v>
       </c>
       <c r="V167" t="s">
         <v>7</v>
@@ -14426,7 +14453,7 @@
         <v>466</v>
       </c>
       <c r="I168" t="s">
-        <v>1543</v>
+        <v>1542</v>
       </c>
       <c r="J168" t="s">
         <v>462</v>
@@ -14438,22 +14465,22 @@
         <v>452</v>
       </c>
       <c r="O168" s="8" t="s">
-        <v>1542</v>
+        <v>1541</v>
       </c>
       <c r="P168" t="s">
         <v>780</v>
       </c>
       <c r="R168" t="s">
-        <v>1544</v>
+        <v>1543</v>
       </c>
       <c r="S168" t="s">
-        <v>1281</v>
+        <v>1280</v>
       </c>
       <c r="T168" t="s">
         <v>631</v>
       </c>
       <c r="U168" t="s">
-        <v>1545</v>
+        <v>1544</v>
       </c>
       <c r="V168" t="s">
         <v>7</v>
@@ -14479,7 +14506,7 @@
         <v>466</v>
       </c>
       <c r="I169" t="s">
-        <v>1546</v>
+        <v>1545</v>
       </c>
       <c r="J169" t="s">
         <v>509</v>
@@ -14488,25 +14515,25 @@
         <v>451</v>
       </c>
       <c r="O169" s="8" t="s">
-        <v>1547</v>
+        <v>1546</v>
       </c>
       <c r="P169" t="s">
         <v>617</v>
       </c>
       <c r="Q169" t="s">
+        <v>1548</v>
+      </c>
+      <c r="R169" t="s">
+        <v>1547</v>
+      </c>
+      <c r="S169" t="s">
         <v>1549</v>
       </c>
-      <c r="R169" t="s">
-        <v>1548</v>
-      </c>
-      <c r="S169" t="s">
+      <c r="T169" t="s">
+        <v>1444</v>
+      </c>
+      <c r="U169" t="s">
         <v>1550</v>
-      </c>
-      <c r="T169" t="s">
-        <v>1445</v>
-      </c>
-      <c r="U169" t="s">
-        <v>1551</v>
       </c>
       <c r="V169" t="s">
         <v>7</v>
@@ -14538,28 +14565,28 @@
         <v>456</v>
       </c>
       <c r="O170" s="8" t="s">
-        <v>1552</v>
+        <v>1551</v>
       </c>
       <c r="P170" t="s">
         <v>658</v>
       </c>
       <c r="Q170" t="s">
+        <v>1552</v>
+      </c>
+      <c r="R170" t="s">
         <v>1553</v>
       </c>
-      <c r="R170" t="s">
+      <c r="S170" t="s">
         <v>1554</v>
-      </c>
-      <c r="S170" t="s">
-        <v>1555</v>
       </c>
       <c r="T170" t="s">
         <v>668</v>
       </c>
       <c r="U170" t="s">
-        <v>1557</v>
+        <v>1556</v>
       </c>
       <c r="V170" t="s">
-        <v>1556</v>
+        <v>1555</v>
       </c>
     </row>
     <row r="171" spans="1:22" x14ac:dyDescent="0.25">
@@ -14588,25 +14615,25 @@
         <v>457</v>
       </c>
       <c r="O171" s="8" t="s">
-        <v>1558</v>
+        <v>1557</v>
       </c>
       <c r="P171" t="s">
         <v>626</v>
       </c>
       <c r="Q171" t="s">
-        <v>1186</v>
+        <v>1185</v>
       </c>
       <c r="R171" t="s">
-        <v>1559</v>
+        <v>1558</v>
       </c>
       <c r="S171" t="s">
-        <v>1188</v>
+        <v>1187</v>
       </c>
       <c r="T171" t="s">
         <v>631</v>
       </c>
       <c r="U171" t="s">
-        <v>1560</v>
+        <v>1559</v>
       </c>
       <c r="V171" t="s">
         <v>7</v>

</xml_diff>

<commit_message>
cleaning up some coding in the data; tweaking plots
</commit_message>
<xml_diff>
--- a/_data/screened_fulltext/ft_consolidated_coding.xlsx
+++ b/_data/screened_fulltext/ft_consolidated_coding.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2806" uniqueCount="1562">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5548" uniqueCount="1563">
   <si>
     <t>title</t>
   </si>
@@ -4712,6 +4712,9 @@
   </si>
   <si>
     <t>Eastern Africa</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Whale conservation goals are due to legal protections - not intrinsic value, but legal value… </t>
   </si>
 </sst>
 </file>
@@ -5566,10 +5569,10 @@
   <dimension ref="A1:V171"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="D121" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="D7" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="O132" sqref="O132"/>
+      <selection pane="bottomRight" activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6571,6 +6574,9 @@
       <c r="E18" s="5" t="s">
         <v>8</v>
       </c>
+      <c r="F18" s="5" t="s">
+        <v>1562</v>
+      </c>
       <c r="G18" s="5" t="s">
         <v>466</v>
       </c>
@@ -6596,7 +6602,7 @@
         <v>827</v>
       </c>
       <c r="T18" s="5" t="s">
-        <v>828</v>
+        <v>665</v>
       </c>
       <c r="U18" s="5" t="s">
         <v>829</v>
@@ -8792,11 +8798,8 @@
       <c r="J59" t="s">
         <v>462</v>
       </c>
-      <c r="K59" t="s">
-        <v>511</v>
-      </c>
       <c r="L59" t="s">
-        <v>511</v>
+        <v>452</v>
       </c>
       <c r="M59" t="s">
         <v>451</v>
@@ -9671,7 +9674,7 @@
         <v>1111</v>
       </c>
       <c r="T75" t="s">
-        <v>1113</v>
+        <v>733</v>
       </c>
       <c r="U75" t="s">
         <v>1114</v>
@@ -10086,7 +10089,7 @@
         <v>1153</v>
       </c>
       <c r="T83" t="s">
-        <v>828</v>
+        <v>665</v>
       </c>
       <c r="U83" t="s">
         <v>1156</v>
@@ -11649,7 +11652,7 @@
         <v>705</v>
       </c>
       <c r="T113" t="s">
-        <v>1113</v>
+        <v>665</v>
       </c>
       <c r="U113" t="s">
         <v>1282</v>
@@ -12230,9 +12233,6 @@
       <c r="J125" t="s">
         <v>457</v>
       </c>
-      <c r="K125" t="s">
-        <v>464</v>
-      </c>
       <c r="L125" t="s">
         <v>457</v>
       </c>
@@ -12811,7 +12811,7 @@
         <v>1376</v>
       </c>
       <c r="T136" t="s">
-        <v>1377</v>
+        <v>1548</v>
       </c>
       <c r="U136" t="s">
         <v>1378</v>

</xml_diff>

<commit_message>
wrapping up most author comments/suggestions; next step, re-examine relational values esp with respect to justice
</commit_message>
<xml_diff>
--- a/_data/screened_fulltext/ft_consolidated_coding.xlsx
+++ b/_data/screened_fulltext/ft_consolidated_coding.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2978" uniqueCount="1564">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3022" uniqueCount="1596">
   <si>
     <t>title</t>
   </si>
@@ -4718,13 +4718,109 @@
   </si>
   <si>
     <t>value type arias arevalo</t>
+  </si>
+  <si>
+    <t>fundamental;instrumental; eudaimonistic</t>
+  </si>
+  <si>
+    <t>RG thoughts on relationality of values</t>
+  </si>
+  <si>
+    <t>Rachelle summary</t>
+  </si>
+  <si>
+    <t>Agree that relational is the best category for the items listed - they speak to the relationships people have with that place, or might want to have with it</t>
+  </si>
+  <si>
+    <t>Agree</t>
+  </si>
+  <si>
+    <t>I don't see the values mentioned in Table 3 as relational. Were you thinking of ones such as "better motivated workforce," maybe? I don't see anything that is about the relationship between people and nature.</t>
+  </si>
+  <si>
+    <t>disagree</t>
+  </si>
+  <si>
+    <t>Not sure I agree with the reasoning in "societal benefit description"; I also think "intrinsic" might be add-able. I think instrumental is clearly there, in the general purposes of EO in this study. But for relational, I don't think the slavery example is really about relational values; it's neither peoples' relationships with nature, nor even really the relationship between people. I do see relational, however, in Figure 3 - "Inspire interest in natural world" and maybe "raise awareness of issues". I might even say this could be coded as intrinsic; I think the slavery case study is about upholding the intrinsic value of humans. It's about rights of those possibly enslaved people.</t>
+  </si>
+  <si>
+    <t>Agree with categorization but for different reasons, and add intrinsic</t>
+  </si>
+  <si>
+    <t>From the abstract, it doesn't seem like the values listed at left are values that the EO are contributing to. The value the EO are providing here seems to be to get farmers paid for damages to their crops, via crop insurance. BUT, the way the paper is written, it claims that the EO did contribute to the values listed, and I agree that they're a combo of relational and instrumental. The main one that is relational is trust - trust among farmers and between farmers and the companies.</t>
+  </si>
+  <si>
+    <t>Agree but only think some values are relational</t>
+  </si>
+  <si>
+    <t>I agree with classfication, but I would add to the notes that to me, relationality is perhaps most evident in this finding: "we find that when interacting with orthomosaics created from UAV images of their farms, farmers’ responses reveal a greater focus on management strategies at larger spatial and temporal scales. UAV imagery thus supports studies of agricultural heritage not only by recording agricultural spaces but also by revealing agrarian knowledge and practices." ... and potentially by helping farmers see a type of interconnectedness and larger scale they hadn't seen before? (Maura might tell us if they found that or not; see email on July 13).</t>
+  </si>
+  <si>
+    <t>Agree and have added reasons</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Not sure I see relational values here. The "sentiment analysis" is less about sentiment per se, and more looks like they used automated coding of their data, to reveal what I see as instrumental benefits of EO -- more efficiency, makes work easier. People are positive about EO, but it seems like they are mostly positive about instrumental values. </t>
+  </si>
+  <si>
+    <t>I think the relational values are evident in this paragraph of the results (basically, increases relationality of the mapping process - more human-human relational values, but also a bit allowing people to express relationships with the land more fluidly): "Practitioners have observed that the remote sensing image enables participation of people who previously had limitations to participate in planning activities, such as elderly and disabled. With the image there is less need to GPS track land uses in order to map them, which is an activity where physically challenged people cannot participate. The image enables these people to visually examine their village landscape and subsequently express their knowledge using the analogue or digital remote sensing image as a visual aid. Practitioners also mention having seen how the remote sensing image is engaging to participants. According to them it is fun, captures participants’ attention and keeps them actively engaged during the mapping exercise. Interviewed practitioners have observed impact of use of remote sensing image on the quality of decision-making among participants in terms of better understanding of the planning issues and capture of wider participant views. Most practitioners (9) have noticed the increase of participants’ spatial understanding such as on environmental condition, relative size of areas, and magnitude of resources. 84% of the participants who answered the survey (n = 351) stated that they learned something new about their environment during the exercises with images (Fig. 3). The practitioners have observed the remote sensing image to create a room for discussion and help participants to express themselves. 89% of the surveyed participants (n = 351) think images helped them in the discussion (Fig. 3). "</t>
+  </si>
+  <si>
+    <t>I think maybe there is conflation between relational values and justice in a couple of these -- the modern slavery one is maybe another example. There is value above and beyond instrumental here, but I don't think it's really relational value -- it's better distribution of instrumental value, which is a justice thing.  Here is a sentence that I think best summarizes this paper's point (which I found difficult to fully grasp until I read this sentence): "By including height into the tree allocation strategy, fewer trees were allocated to blocks with higher quality pre-existing canopies and were instead redistributed to blocks with relatively lower quality tree canopies. " So, LiDAR and machine learning allow them to do that, which allows a more just response (but not necsesarily one with more relational value)</t>
+  </si>
+  <si>
+    <t>Disagree</t>
+  </si>
+  <si>
+    <t>Agree! Great example. I'd add something like the following: the use of EO in this case allows expression of relational values the Indigenous communities have, e.g., as expressed for instance in this quote from the authors' data collection: "The forest is our home, our market, our hospital: that's why we protect it. But foreigners, strangers who come, they think that the forest is like an object which can be sold, we don't allow this."</t>
+  </si>
+  <si>
+    <t>A bit less obvious, the relational value here …. But I see why you coded it. I guess the argument is that better weather forecasts allow people to better plan recreational activities and outdoor work, which both contribute to relational values -- so the EO contributes to relational values. There's a little bit of extrapolation involved in that, from the data provided, but I think it's reasonable.</t>
+  </si>
+  <si>
+    <t>Yes! I think the culturla benefits they mention certainly qualify, some of them, as relational (changing the way people see their relationship with the planet). In general, very interesting paper in general for our purposes, and I really like their discussion of cultural and leisure activities and foregrounding these.  Definitely one we should cite as motivation for the more "perceptual" work we're doing. They don't mention that specifically, but I think we could say that they have recognized the "cultural" implications and that we're taking it a step further to the perceptual aspects.</t>
+  </si>
+  <si>
+    <t>This is a very unique publication; it's offering a general way of calculating the social value of scientific publications in general, using EO as a model. It also comes up with a "social value of EO". I think the argument that it's realational comes from its calculation of SOCIAL value, and that includes elements such as links between people, for instance, how others are using a given publication (via citation). That is MAYBE relational, but more in the sense that it describes relationships, rather than it's about the relationships themselves being valued/valuable. So, it's a borderline case, but since there may be some of that more relational valuing, I'll land on overall a weak agree :)</t>
+  </si>
+  <si>
+    <t>Not sure how the description currently there depicts relational values! But I think here, the relational values are in the nature of knowledge-sharing: the value of the EO is that it allows bridging of relationships between experts and volunteer mappers, who have more local knowledge. So it allows more relationships between knowledge types, and it is those relationships (weaving of knowledge) that create value (this makes me think of, e.g., Tengo's work on weaving knowledge systems. Essentially, because EO in the form of Open Street Maps are very intuitive to use, they can be a tool that helps to bridge knowledge systems. That is relational): "Most importantly, it [their approach] helps to bring knowledge from different sources and experts in the volunteered contribution and allows them to corroborate each other. It also enables both researchers and local people to transfer technical knowledge, collect location-specific data, and use them for better decision-making. "</t>
+  </si>
+  <si>
+    <t>Agree but perhaps for different reasons</t>
+  </si>
+  <si>
+    <t>Yes, their "societal benefit" category is very interesting and has a couple of relational elements. The strongest is that one of their "societal benefit" [of EO] categories is "Community and quality of life", which they define as "Increased sense of community and the quality of life through enhanced perception of the country/region/town/etc as a place to live."  They also mention increased ability to, for example, swim in non-polluted lakes, but they talk about that more in an instrumental way (reducing human exposure to pollution, rather than about faciliating relationships with place).</t>
+  </si>
+  <si>
+    <t>maybe…. The relational bit is really just information-sharing; it lets farmers participate and be part of the research process. It's possible that creates relational values with their land, but the paper isn't studying that. It doesn't even really seem to be talking about links between farmers (though I'm not looking at the full paper -- only the abstract, so maybe the full paper expands on the "learning community" idea and talks more about person-to-person interactions). So I would call this relational values "light", if at all.</t>
+  </si>
+  <si>
+    <t>Mostly disagree, maybe a little RV</t>
+  </si>
+  <si>
+    <t>Relational values are related to peoples' understanding of their place; this study didn't collect data on values like sense of place, but it's mentioned in the intro that similar programs can create sense of place, and the data from this study suggest that people better understood "the relationship between [landscape] features and the impact of flooding." Data also suggest that people appreciated being able to engage with the landscape in this interactive way, which has relational elements.</t>
+  </si>
+  <si>
+    <t>This seems pretty clearly to be another example of the isntrumental values contributing to distributional justice -- or justice of some kind. I don't really see the sattelites as contributing to relational values.</t>
+  </si>
+  <si>
+    <t>Borderline case; it's not entirely clear that the values students are learning/receiving are necessarily relational in nature. This sentence from the abstract is the most clear indication that the values coming from this experience might be relational: "In their multiscalar analysis of environmental data, students are forced to acknowledge the different yet overlapping operational scales of various social and ecological processes that drive landscape changes affecting Earth's resources." This is a pretty good indicatation that the EO are being used to talk about human-nature (/social-ecological) relationships, so we can call that relational values I suppose!</t>
+  </si>
+  <si>
+    <t>Another example of where the outcome is justice -- not relational values. I considered whether the rural electrification bit was relational, because it is fundamentally about using EO to better map out networks and the topologies of energy systems -- but though that is technically about relationships between places, it's stretching too far to say that is relational values.</t>
+  </si>
+  <si>
+    <t>I can't access the full article so cannot be sure -- but it seems like they're talking about recreation in a more instrumental way. That is, the abstract doesn't imply that there is anything particularly relational about the information provided, or what that information makes possible. It's possible that the full paper has relational elements (e.g., that the information contributes to fishermen creating more nuanced or deep relationships with their places? Something like that),but I'm not seeing indications of that in the abstract</t>
+  </si>
+  <si>
+    <t>Another instance of the mapping creating an instrumental value (mapping poverty) that has justice implications</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="22" x14ac:knownFonts="1">
+  <fonts count="23" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -4886,8 +4982,15 @@
       <name val="DejaVu Sans"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="34">
+  <fills count="40">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -5073,6 +5176,42 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="10">
     <border>
@@ -5234,7 +5373,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -5260,6 +5399,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="22" fillId="35" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="36" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="22" fillId="36" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="37" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="22" fillId="37" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="22" fillId="38" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="22" fillId="39" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -5581,13 +5732,14 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:W171"/>
+  <sheetPr filterMode="1"/>
+  <dimension ref="A1:Y171"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="G2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="J5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="T2" sqref="T2"/>
+      <selection pane="bottomRight" activeCell="O140" sqref="O140"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5607,9 +5759,11 @@
     <col min="21" max="21" width="13.5703125" customWidth="1"/>
     <col min="22" max="22" width="12.28515625" customWidth="1"/>
     <col min="23" max="23" width="16.140625" customWidth="1"/>
+    <col min="24" max="24" width="28.5703125" customWidth="1"/>
+    <col min="25" max="25" width="16.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" s="6" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:25" s="6" customFormat="1" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
@@ -5679,8 +5833,14 @@
       <c r="W1" s="6" t="s">
         <v>609</v>
       </c>
-    </row>
-    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X1" s="14" t="s">
+        <v>1565</v>
+      </c>
+      <c r="Y1" s="14" t="s">
+        <v>1566</v>
+      </c>
+    </row>
+    <row r="2" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>266</v>
       </c>
@@ -5739,7 +5899,7 @@
         <v>737</v>
       </c>
     </row>
-    <row r="3" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>86</v>
       </c>
@@ -5798,7 +5958,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:25" ht="14.25" hidden="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>84</v>
       </c>
@@ -5857,69 +6017,75 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+    <row r="5" spans="1:25" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="13" t="s">
         <v>168</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="13" t="s">
         <v>169</v>
       </c>
-      <c r="C5">
+      <c r="C5" s="13">
         <v>2020</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D5" s="13" t="s">
         <v>170</v>
       </c>
-      <c r="E5" t="s">
+      <c r="E5" s="13" t="s">
         <v>171</v>
       </c>
-      <c r="F5" t="s">
+      <c r="F5" s="13" t="s">
         <v>781</v>
       </c>
-      <c r="G5" t="s">
+      <c r="G5" s="13" t="s">
         <v>475</v>
       </c>
-      <c r="I5" t="s">
+      <c r="I5" s="13" t="s">
         <v>619</v>
       </c>
-      <c r="J5" t="s">
+      <c r="J5" s="13" t="s">
         <v>509</v>
       </c>
-      <c r="L5" t="s">
+      <c r="L5" s="13" t="s">
         <v>509</v>
       </c>
       <c r="N5" t="s">
         <v>510</v>
       </c>
-      <c r="O5" s="8" t="s">
+      <c r="O5" s="13" t="s">
         <v>607</v>
       </c>
-      <c r="P5" t="s">
+      <c r="P5" s="13" t="s">
         <v>605</v>
       </c>
-      <c r="Q5" t="s">
+      <c r="Q5" s="13" t="s">
         <v>606</v>
       </c>
-      <c r="R5" t="s">
+      <c r="R5" s="13" t="s">
         <v>612</v>
       </c>
-      <c r="S5" t="s">
+      <c r="S5" s="13" t="s">
         <v>608</v>
       </c>
-      <c r="T5" s="10" t="s">
+      <c r="T5" s="13" t="s">
         <v>1553</v>
       </c>
-      <c r="U5" t="s">
+      <c r="U5" s="13" t="s">
         <v>1549</v>
       </c>
-      <c r="V5" t="s">
+      <c r="V5" s="13" t="s">
         <v>611</v>
       </c>
-      <c r="W5" t="s">
+      <c r="W5" s="13" t="s">
         <v>610</v>
       </c>
-    </row>
-    <row r="6" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X5" s="15" t="s">
+        <v>1567</v>
+      </c>
+      <c r="Y5" s="15" t="s">
+        <v>1568</v>
+      </c>
+    </row>
+    <row r="6" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>88</v>
       </c>
@@ -5975,63 +6141,70 @@
         <v>757</v>
       </c>
     </row>
-    <row r="7" spans="1:23" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="5" t="s">
+    <row r="7" spans="1:25" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="17" t="s">
         <v>190</v>
       </c>
-      <c r="B7" s="5" t="s">
+      <c r="B7" s="17" t="s">
         <v>191</v>
       </c>
-      <c r="C7" s="5">
+      <c r="C7" s="17">
         <v>2018</v>
       </c>
-      <c r="D7" s="5" t="s">
+      <c r="D7" s="17" t="s">
         <v>192</v>
       </c>
-      <c r="E7" s="5" t="s">
+      <c r="E7" s="17" t="s">
         <v>193</v>
       </c>
-      <c r="G7" s="5" t="s">
+      <c r="G7" s="17" t="s">
         <v>474</v>
       </c>
-      <c r="I7" s="5" t="s">
+      <c r="I7" s="17" t="s">
         <v>620</v>
       </c>
-      <c r="J7" s="5" t="s">
+      <c r="J7" s="17" t="s">
         <v>509</v>
       </c>
-      <c r="L7" s="5" t="s">
+      <c r="L7" s="17" t="s">
         <v>451</v>
       </c>
-      <c r="O7" s="8" t="s">
+      <c r="N7" s="5"/>
+      <c r="O7" s="17" t="s">
         <v>615</v>
       </c>
-      <c r="P7" s="5" t="s">
+      <c r="P7" s="17" t="s">
         <v>613</v>
       </c>
-      <c r="Q7" s="5" t="s">
+      <c r="Q7" s="17" t="s">
         <v>614</v>
       </c>
-      <c r="R7" s="5" t="s">
+      <c r="R7" s="17" t="s">
         <v>618</v>
       </c>
-      <c r="S7" s="5" t="s">
+      <c r="S7" s="17" t="s">
         <v>765</v>
       </c>
-      <c r="T7" s="11" t="s">
+      <c r="T7" s="17" t="s">
         <v>1554</v>
       </c>
-      <c r="U7" s="5" t="s">
+      <c r="U7" s="17" t="s">
         <v>1550</v>
       </c>
-      <c r="V7" s="5" t="s">
+      <c r="V7" s="17" t="s">
         <v>617</v>
       </c>
-      <c r="W7" s="5" t="s">
+      <c r="W7" s="17" t="s">
         <v>616</v>
       </c>
-    </row>
-    <row r="8" spans="1:23" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="X7" s="18" t="s">
+        <v>1569</v>
+      </c>
+      <c r="Y7" s="18" t="s">
+        <v>1570</v>
+      </c>
+    </row>
+    <row r="8" spans="1:25" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
         <v>352</v>
       </c>
@@ -6093,7 +6266,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:23" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:25" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
         <v>91</v>
       </c>
@@ -6152,7 +6325,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:23" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:25" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
         <v>194</v>
       </c>
@@ -6217,7 +6390,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="11" spans="1:23" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:25" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
         <v>355</v>
       </c>
@@ -6270,7 +6443,7 @@
         <v>786</v>
       </c>
     </row>
-    <row r="12" spans="1:23" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:25" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
         <v>5</v>
       </c>
@@ -6326,7 +6499,7 @@
         <v>794</v>
       </c>
     </row>
-    <row r="13" spans="1:23" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:25" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
         <v>358</v>
       </c>
@@ -6382,7 +6555,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="14" spans="1:23" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:25" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
         <v>200</v>
       </c>
@@ -6450,7 +6623,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="15" spans="1:23" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:25" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
         <v>197</v>
       </c>
@@ -6512,7 +6685,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="16" spans="1:23" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:25" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
         <v>11</v>
       </c>
@@ -6568,7 +6741,7 @@
         <v>809</v>
       </c>
     </row>
-    <row r="17" spans="1:23" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:25" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
         <v>9</v>
       </c>
@@ -6624,7 +6797,7 @@
         <v>806</v>
       </c>
     </row>
-    <row r="18" spans="1:23" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:25" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
         <v>13</v>
       </c>
@@ -6680,7 +6853,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="19" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>93</v>
       </c>
@@ -6739,7 +6912,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="20" spans="1:23" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:25" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A20" s="5" t="s">
         <v>151</v>
       </c>
@@ -6795,7 +6968,7 @@
         <v>828</v>
       </c>
     </row>
-    <row r="21" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>361</v>
       </c>
@@ -6851,7 +7024,7 @@
         <v>832</v>
       </c>
     </row>
-    <row r="22" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>172</v>
       </c>
@@ -6910,7 +7083,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="23" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>275</v>
       </c>
@@ -6969,7 +7142,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="24" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>279</v>
       </c>
@@ -7022,7 +7195,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="25" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>15</v>
       </c>
@@ -7087,7 +7260,7 @@
         <v>854</v>
       </c>
     </row>
-    <row r="26" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>17</v>
       </c>
@@ -7155,7 +7328,7 @@
         <v>642</v>
       </c>
     </row>
-    <row r="27" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>19</v>
       </c>
@@ -7214,7 +7387,7 @@
         <v>864</v>
       </c>
     </row>
-    <row r="28" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>21</v>
       </c>
@@ -7273,7 +7446,7 @@
         <v>866</v>
       </c>
     </row>
-    <row r="29" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>282</v>
       </c>
@@ -7326,63 +7499,70 @@
         <v>7</v>
       </c>
     </row>
-    <row r="30" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
+    <row r="30" spans="1:25" s="19" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="19" t="s">
         <v>364</v>
       </c>
-      <c r="B30" t="s">
+      <c r="B30" s="19" t="s">
         <v>365</v>
       </c>
-      <c r="C30">
+      <c r="C30" s="19">
         <v>2022</v>
       </c>
-      <c r="D30" t="s">
+      <c r="D30" s="19" t="s">
         <v>366</v>
       </c>
-      <c r="E30" t="s">
+      <c r="E30" s="19" t="s">
         <v>351</v>
       </c>
-      <c r="G30" t="s">
+      <c r="G30" s="19" t="s">
         <v>480</v>
       </c>
-      <c r="H30" t="s">
+      <c r="H30" s="19" t="s">
         <v>474</v>
       </c>
-      <c r="J30" t="s">
+      <c r="J30" s="19" t="s">
         <v>511</v>
       </c>
-      <c r="L30" t="s">
+      <c r="L30" s="19" t="s">
         <v>511</v>
       </c>
-      <c r="M30" t="s">
+      <c r="M30" s="19" t="s">
         <v>451</v>
       </c>
-      <c r="O30" s="8" t="s">
+      <c r="N30"/>
+      <c r="O30" s="19" t="s">
         <v>874</v>
       </c>
-      <c r="P30" t="s">
+      <c r="P30" s="19" t="s">
         <v>875</v>
       </c>
-      <c r="R30" t="s">
+      <c r="R30" s="19" t="s">
         <v>878</v>
       </c>
-      <c r="S30" t="s">
+      <c r="S30" s="19" t="s">
         <v>876</v>
       </c>
-      <c r="T30" s="10" t="s">
+      <c r="T30" s="19" t="s">
         <v>1556</v>
       </c>
-      <c r="U30" t="s">
+      <c r="U30" s="19" t="s">
         <v>1551</v>
       </c>
-      <c r="V30" t="s">
+      <c r="V30" s="19" t="s">
         <v>877</v>
       </c>
-      <c r="W30" t="s">
+      <c r="W30" s="19" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="31" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X30" s="20" t="s">
+        <v>1571</v>
+      </c>
+      <c r="Y30" s="20" t="s">
+        <v>1572</v>
+      </c>
+    </row>
+    <row r="31" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>23</v>
       </c>
@@ -7435,7 +7615,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="32" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>285</v>
       </c>
@@ -7491,7 +7671,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="33" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>95</v>
       </c>
@@ -7550,7 +7730,7 @@
         <v>893</v>
       </c>
     </row>
-    <row r="34" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>288</v>
       </c>
@@ -7606,7 +7786,7 @@
         <v>646</v>
       </c>
     </row>
-    <row r="35" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>97</v>
       </c>
@@ -7662,7 +7842,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="36" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>25</v>
       </c>
@@ -7715,63 +7895,69 @@
         <v>7</v>
       </c>
     </row>
-    <row r="37" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
+    <row r="37" spans="1:25" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="13" t="s">
         <v>291</v>
       </c>
-      <c r="B37" t="s">
+      <c r="B37" s="13" t="s">
         <v>292</v>
       </c>
-      <c r="C37">
+      <c r="C37" s="13">
         <v>2020</v>
       </c>
-      <c r="D37" t="s">
+      <c r="D37" s="13" t="s">
         <v>293</v>
       </c>
-      <c r="E37" t="s">
+      <c r="E37" s="13" t="s">
         <v>278</v>
       </c>
-      <c r="G37" t="s">
+      <c r="G37" s="13" t="s">
         <v>480</v>
       </c>
-      <c r="I37" t="s">
+      <c r="I37" s="13" t="s">
         <v>916</v>
       </c>
-      <c r="J37" t="s">
+      <c r="J37" s="13" t="s">
         <v>457</v>
       </c>
-      <c r="L37" t="s">
+      <c r="L37" s="13" t="s">
         <v>457</v>
       </c>
-      <c r="O37" s="8" t="s">
+      <c r="O37" s="13" t="s">
         <v>909</v>
       </c>
-      <c r="P37" t="s">
+      <c r="P37" s="13" t="s">
         <v>910</v>
       </c>
-      <c r="Q37" t="s">
+      <c r="Q37" s="13" t="s">
         <v>912</v>
       </c>
-      <c r="R37" t="s">
+      <c r="R37" s="13" t="s">
         <v>914</v>
       </c>
-      <c r="S37" t="s">
+      <c r="S37" s="13" t="s">
         <v>913</v>
       </c>
-      <c r="T37" s="10" t="s">
-        <v>1555</v>
-      </c>
-      <c r="U37" t="s">
+      <c r="T37" s="13" t="s">
+        <v>1564</v>
+      </c>
+      <c r="U37" s="13" t="s">
         <v>1550</v>
       </c>
-      <c r="V37" t="s">
+      <c r="V37" s="13" t="s">
         <v>915</v>
       </c>
-      <c r="W37" t="s">
+      <c r="W37" s="13" t="s">
         <v>911</v>
       </c>
-    </row>
-    <row r="38" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X37" s="15" t="s">
+        <v>1573</v>
+      </c>
+      <c r="Y37" s="15" t="s">
+        <v>1574</v>
+      </c>
+    </row>
+    <row r="38" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>99</v>
       </c>
@@ -7830,7 +8016,7 @@
         <v>921</v>
       </c>
     </row>
-    <row r="39" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>203</v>
       </c>
@@ -7886,7 +8072,7 @@
         <v>925</v>
       </c>
     </row>
-    <row r="40" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>367</v>
       </c>
@@ -7942,72 +8128,79 @@
         <v>7</v>
       </c>
     </row>
-    <row r="41" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A41" t="s">
+    <row r="41" spans="1:25" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="13" t="s">
         <v>370</v>
       </c>
-      <c r="B41" t="s">
+      <c r="B41" s="13" t="s">
         <v>371</v>
       </c>
-      <c r="C41">
+      <c r="C41" s="13">
         <v>2020</v>
       </c>
-      <c r="D41" t="s">
+      <c r="D41" s="13" t="s">
         <v>372</v>
       </c>
-      <c r="E41" t="s">
+      <c r="E41" s="13" t="s">
         <v>351</v>
       </c>
-      <c r="G41" t="s">
+      <c r="G41" s="13" t="s">
         <v>480</v>
       </c>
-      <c r="H41" t="s">
+      <c r="H41" s="13" t="s">
         <v>475</v>
       </c>
-      <c r="I41" t="s">
+      <c r="I41" s="13" t="s">
         <v>940</v>
       </c>
-      <c r="J41" t="s">
+      <c r="J41" s="13" t="s">
         <v>457</v>
       </c>
-      <c r="K41" t="s">
+      <c r="K41" s="13" t="s">
         <v>464</v>
       </c>
-      <c r="L41" t="s">
+      <c r="L41" s="13" t="s">
         <v>457</v>
       </c>
-      <c r="M41" t="s">
+      <c r="M41" s="13" t="s">
         <v>456</v>
       </c>
-      <c r="O41" s="8" t="s">
+      <c r="N41"/>
+      <c r="O41" s="13" t="s">
         <v>935</v>
       </c>
-      <c r="P41" t="s">
+      <c r="P41" s="13" t="s">
         <v>936</v>
       </c>
-      <c r="Q41" t="s">
+      <c r="Q41" s="13" t="s">
         <v>937</v>
       </c>
-      <c r="R41" t="s">
+      <c r="R41" s="13" t="s">
         <v>941</v>
       </c>
-      <c r="S41" t="s">
+      <c r="S41" s="13" t="s">
         <v>913</v>
       </c>
-      <c r="T41" s="10" t="s">
+      <c r="T41" s="13" t="s">
         <v>1558</v>
       </c>
-      <c r="U41" t="s">
+      <c r="U41" s="13" t="s">
         <v>1551</v>
       </c>
-      <c r="V41" t="s">
+      <c r="V41" s="13" t="s">
         <v>939</v>
       </c>
-      <c r="W41" t="s">
+      <c r="W41" s="13" t="s">
         <v>938</v>
       </c>
-    </row>
-    <row r="42" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X41" s="15" t="s">
+        <v>1575</v>
+      </c>
+      <c r="Y41" s="15" t="s">
+        <v>1576</v>
+      </c>
+    </row>
+    <row r="42" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>294</v>
       </c>
@@ -8063,7 +8256,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="43" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>29</v>
       </c>
@@ -8119,7 +8312,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="44" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>27</v>
       </c>
@@ -8172,7 +8365,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="45" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>101</v>
       </c>
@@ -8234,7 +8427,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="46" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>31</v>
       </c>
@@ -8293,7 +8486,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="47" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>33</v>
       </c>
@@ -8352,7 +8545,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="48" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>103</v>
       </c>
@@ -8408,7 +8601,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="49" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>373</v>
       </c>
@@ -8467,7 +8660,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="50" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>105</v>
       </c>
@@ -8526,66 +8719,73 @@
         <v>982</v>
       </c>
     </row>
-    <row r="51" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A51" t="s">
+    <row r="51" spans="1:25" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A51" s="17" t="s">
         <v>297</v>
       </c>
-      <c r="B51" t="s">
+      <c r="B51" s="17" t="s">
         <v>298</v>
       </c>
-      <c r="C51">
+      <c r="C51" s="17">
         <v>2023</v>
       </c>
-      <c r="D51" t="s">
+      <c r="D51" s="17" t="s">
         <v>299</v>
       </c>
-      <c r="E51" t="s">
+      <c r="E51" s="17" t="s">
         <v>278</v>
       </c>
-      <c r="G51" t="s">
+      <c r="G51" s="17" t="s">
         <v>484</v>
       </c>
-      <c r="H51" t="s">
+      <c r="H51" s="17" t="s">
         <v>480</v>
       </c>
-      <c r="I51" t="s">
+      <c r="I51" s="17" t="s">
         <v>986</v>
       </c>
-      <c r="J51" t="s">
+      <c r="J51" s="17" t="s">
         <v>457</v>
       </c>
-      <c r="L51" t="s">
+      <c r="L51" s="17" t="s">
         <v>457</v>
       </c>
-      <c r="O51" s="8" t="s">
+      <c r="N51"/>
+      <c r="O51" s="17" t="s">
         <v>985</v>
       </c>
-      <c r="P51" t="s">
+      <c r="P51" s="17" t="s">
         <v>904</v>
       </c>
-      <c r="Q51" t="s">
+      <c r="Q51" s="17" t="s">
         <v>988</v>
       </c>
-      <c r="R51" t="s">
+      <c r="R51" s="17" t="s">
         <v>989</v>
       </c>
-      <c r="S51" t="s">
+      <c r="S51" s="17" t="s">
         <v>965</v>
       </c>
-      <c r="T51" s="10" t="s">
+      <c r="T51" s="17" t="s">
         <v>1553</v>
       </c>
-      <c r="U51" t="s">
+      <c r="U51" s="17" t="s">
         <v>1551</v>
       </c>
-      <c r="V51" t="s">
+      <c r="V51" s="17" t="s">
         <v>990</v>
       </c>
-      <c r="W51" t="s">
+      <c r="W51" s="17" t="s">
         <v>987</v>
       </c>
-    </row>
-    <row r="52" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X51" s="18" t="s">
+        <v>1577</v>
+      </c>
+      <c r="Y51" s="18" t="s">
+        <v>1570</v>
+      </c>
+    </row>
+    <row r="52" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>35</v>
       </c>
@@ -8641,7 +8841,7 @@
         <v>993</v>
       </c>
     </row>
-    <row r="53" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>206</v>
       </c>
@@ -8688,7 +8888,7 @@
         <v>997</v>
       </c>
     </row>
-    <row r="54" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>156</v>
       </c>
@@ -8741,66 +8941,73 @@
         <v>7</v>
       </c>
     </row>
-    <row r="55" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A55" t="s">
+    <row r="55" spans="1:25" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A55" s="13" t="s">
         <v>175</v>
       </c>
-      <c r="B55" t="s">
+      <c r="B55" s="13" t="s">
         <v>176</v>
       </c>
-      <c r="C55">
+      <c r="C55" s="13">
         <v>2021</v>
       </c>
-      <c r="D55" t="s">
+      <c r="D55" s="13" t="s">
         <v>177</v>
       </c>
-      <c r="E55" t="s">
+      <c r="E55" s="13" t="s">
         <v>171</v>
       </c>
-      <c r="G55" t="s">
+      <c r="G55" s="13" t="s">
         <v>480</v>
       </c>
-      <c r="H55" t="s">
+      <c r="H55" s="13" t="s">
         <v>484</v>
       </c>
-      <c r="J55" t="s">
+      <c r="J55" s="13" t="s">
         <v>511</v>
       </c>
-      <c r="L55" t="s">
+      <c r="L55" s="13" t="s">
         <v>511</v>
       </c>
-      <c r="M55" t="s">
+      <c r="M55" s="13" t="s">
         <v>451</v>
       </c>
-      <c r="O55" s="8" t="s">
+      <c r="N55"/>
+      <c r="O55" s="13" t="s">
         <v>1006</v>
       </c>
-      <c r="P55" t="s">
+      <c r="P55" s="13" t="s">
         <v>1007</v>
       </c>
-      <c r="Q55" t="s">
+      <c r="Q55" s="13" t="s">
         <v>1008</v>
       </c>
-      <c r="R55" t="s">
+      <c r="R55" s="13" t="s">
         <v>1009</v>
       </c>
-      <c r="S55" t="s">
+      <c r="S55" s="13" t="s">
         <v>1010</v>
       </c>
-      <c r="T55" s="10" t="s">
+      <c r="T55" s="13" t="s">
         <v>1553</v>
       </c>
-      <c r="U55" t="s">
+      <c r="U55" s="13" t="s">
         <v>1551</v>
       </c>
-      <c r="V55" t="s">
+      <c r="V55" s="13" t="s">
         <v>1011</v>
       </c>
-      <c r="W55" t="s">
+      <c r="W55" s="13" t="s">
         <v>1012</v>
       </c>
-    </row>
-    <row r="56" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X55" s="16" t="s">
+        <v>1578</v>
+      </c>
+      <c r="Y55" s="16" t="s">
+        <v>1568</v>
+      </c>
+    </row>
+    <row r="56" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>209</v>
       </c>
@@ -8853,7 +9060,7 @@
         <v>1018</v>
       </c>
     </row>
-    <row r="57" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>212</v>
       </c>
@@ -8906,7 +9113,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="58" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>376</v>
       </c>
@@ -8962,7 +9169,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="59" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>379</v>
       </c>
@@ -9021,7 +9228,7 @@
         <v>1031</v>
       </c>
     </row>
-    <row r="60" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>300</v>
       </c>
@@ -9074,7 +9281,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="61" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>68</v>
       </c>
@@ -9136,7 +9343,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="62" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>303</v>
       </c>
@@ -9198,69 +9405,76 @@
         <v>1047</v>
       </c>
     </row>
-    <row r="63" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A63" t="s">
+    <row r="63" spans="1:25" s="19" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A63" s="19" t="s">
         <v>178</v>
       </c>
-      <c r="B63" t="s">
+      <c r="B63" s="19" t="s">
         <v>179</v>
       </c>
-      <c r="C63">
+      <c r="C63" s="19">
         <v>2023</v>
       </c>
-      <c r="D63" t="s">
+      <c r="D63" s="19" t="s">
         <v>180</v>
       </c>
-      <c r="E63" t="s">
+      <c r="E63" s="19" t="s">
         <v>171</v>
       </c>
-      <c r="G63" t="s">
+      <c r="G63" s="19" t="s">
         <v>466</v>
       </c>
-      <c r="I63" t="s">
+      <c r="I63" s="19" t="s">
         <v>1053</v>
       </c>
-      <c r="J63" t="s">
+      <c r="J63" s="19" t="s">
         <v>457</v>
       </c>
-      <c r="K63" t="s">
+      <c r="K63" s="19" t="s">
         <v>460</v>
       </c>
-      <c r="L63" t="s">
+      <c r="L63" s="19" t="s">
         <v>457</v>
       </c>
-      <c r="M63" t="s">
+      <c r="M63" s="19" t="s">
         <v>452</v>
       </c>
-      <c r="O63" s="8" t="s">
+      <c r="N63"/>
+      <c r="O63" s="19" t="s">
         <v>1048</v>
       </c>
-      <c r="P63" t="s">
+      <c r="P63" s="19" t="s">
         <v>622</v>
       </c>
-      <c r="Q63" t="s">
+      <c r="Q63" s="19" t="s">
         <v>1049</v>
       </c>
-      <c r="R63" t="s">
+      <c r="R63" s="19" t="s">
         <v>1050</v>
       </c>
-      <c r="S63" t="s">
+      <c r="S63" s="19" t="s">
         <v>1051</v>
       </c>
-      <c r="T63" s="10" t="s">
+      <c r="T63" s="19" t="s">
         <v>1557</v>
       </c>
-      <c r="U63" t="s">
+      <c r="U63" s="19" t="s">
         <v>1551</v>
       </c>
-      <c r="V63" t="s">
+      <c r="V63" s="19" t="s">
         <v>1052</v>
       </c>
-      <c r="W63" t="s">
+      <c r="W63" s="19" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="64" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X63" s="20" t="s">
+        <v>1579</v>
+      </c>
+      <c r="Y63" s="20" t="s">
+        <v>1580</v>
+      </c>
+    </row>
+    <row r="64" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>37</v>
       </c>
@@ -9304,7 +9518,7 @@
         <v>627</v>
       </c>
     </row>
-    <row r="65" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>215</v>
       </c>
@@ -9357,7 +9571,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="66" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>153</v>
       </c>
@@ -9419,69 +9633,76 @@
         <v>663</v>
       </c>
     </row>
-    <row r="67" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A67" t="s">
+    <row r="67" spans="1:25" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A67" s="13" t="s">
         <v>382</v>
       </c>
-      <c r="B67" t="s">
+      <c r="B67" s="13" t="s">
         <v>383</v>
       </c>
-      <c r="C67">
+      <c r="C67" s="13">
         <v>2023</v>
       </c>
-      <c r="D67" t="s">
+      <c r="D67" s="13" t="s">
         <v>384</v>
       </c>
-      <c r="E67" t="s">
+      <c r="E67" s="13" t="s">
         <v>351</v>
       </c>
-      <c r="G67" t="s">
+      <c r="G67" s="13" t="s">
         <v>484</v>
       </c>
-      <c r="H67" t="s">
+      <c r="H67" s="13" t="s">
         <v>480</v>
       </c>
-      <c r="I67" t="s">
+      <c r="I67" s="13" t="s">
         <v>1063</v>
       </c>
-      <c r="J67" t="s">
+      <c r="J67" s="13" t="s">
         <v>457</v>
       </c>
-      <c r="L67" t="s">
+      <c r="L67" s="13" t="s">
         <v>451</v>
       </c>
-      <c r="M67" t="s">
+      <c r="M67" s="13" t="s">
         <v>457</v>
       </c>
-      <c r="O67" s="8" t="s">
+      <c r="N67"/>
+      <c r="O67" s="13" t="s">
         <v>1060</v>
       </c>
-      <c r="P67" s="5" t="s">
+      <c r="P67" s="13" t="s">
         <v>1535</v>
       </c>
-      <c r="Q67" s="5" t="s">
+      <c r="Q67" s="13" t="s">
         <v>1061</v>
       </c>
-      <c r="R67" s="5" t="s">
+      <c r="R67" s="13" t="s">
         <v>1062</v>
       </c>
-      <c r="S67" s="5" t="s">
+      <c r="S67" s="13" t="s">
         <v>1065</v>
       </c>
-      <c r="T67" s="11" t="s">
+      <c r="T67" s="13" t="s">
         <v>1553</v>
       </c>
-      <c r="U67" s="5" t="s">
+      <c r="U67" s="13" t="s">
         <v>1551</v>
       </c>
-      <c r="V67" s="5" t="s">
+      <c r="V67" s="13" t="s">
         <v>1066</v>
       </c>
-      <c r="W67" s="5" t="s">
+      <c r="W67" s="13" t="s">
         <v>1064</v>
       </c>
-    </row>
-    <row r="68" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X67" s="16" t="s">
+        <v>1581</v>
+      </c>
+      <c r="Y67" s="16" t="s">
+        <v>1568</v>
+      </c>
+    </row>
+    <row r="68" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>107</v>
       </c>
@@ -9537,7 +9758,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="69" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>385</v>
       </c>
@@ -9593,7 +9814,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="70" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>109</v>
       </c>
@@ -9649,7 +9870,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="71" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>149</v>
       </c>
@@ -9705,7 +9926,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="72" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>39</v>
       </c>
@@ -9758,7 +9979,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="73" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>388</v>
       </c>
@@ -9811,7 +10032,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="74" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>143</v>
       </c>
@@ -9867,7 +10088,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="75" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>218</v>
       </c>
@@ -9923,7 +10144,7 @@
         <v>1103</v>
       </c>
     </row>
-    <row r="76" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>391</v>
       </c>
@@ -9979,7 +10200,7 @@
         <v>1106</v>
       </c>
     </row>
-    <row r="77" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>42</v>
       </c>
@@ -10032,7 +10253,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="78" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>394</v>
       </c>
@@ -10085,7 +10306,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="79" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>306</v>
       </c>
@@ -10135,7 +10356,7 @@
         <v>1124</v>
       </c>
     </row>
-    <row r="80" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>158</v>
       </c>
@@ -10194,7 +10415,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="81" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>221</v>
       </c>
@@ -10247,7 +10468,7 @@
         <v>1132</v>
       </c>
     </row>
-    <row r="82" spans="1:23" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:23" ht="409.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>309</v>
       </c>
@@ -10306,7 +10527,7 @@
         <v>1139</v>
       </c>
     </row>
-    <row r="83" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>224</v>
       </c>
@@ -10362,7 +10583,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="84" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>111</v>
       </c>
@@ -10415,7 +10636,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="85" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>147</v>
       </c>
@@ -10468,7 +10689,7 @@
         <v>1156</v>
       </c>
     </row>
-    <row r="86" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>70</v>
       </c>
@@ -10521,7 +10742,7 @@
         <v>1160</v>
       </c>
     </row>
-    <row r="87" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>227</v>
       </c>
@@ -10577,7 +10798,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="88" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>397</v>
       </c>
@@ -10630,7 +10851,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="89" spans="1:23" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:23" ht="409.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>44</v>
       </c>
@@ -10686,7 +10907,7 @@
         <v>1172</v>
       </c>
     </row>
-    <row r="90" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>46</v>
       </c>
@@ -10739,7 +10960,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="91" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>230</v>
       </c>
@@ -10792,7 +11013,7 @@
         <v>1180</v>
       </c>
     </row>
-    <row r="92" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>113</v>
       </c>
@@ -10845,7 +11066,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="93" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>72</v>
       </c>
@@ -10898,7 +11119,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="94" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:23" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>312</v>
       </c>
@@ -10957,7 +11178,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="95" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>233</v>
       </c>
@@ -11010,7 +11231,7 @@
         <v>1194</v>
       </c>
     </row>
-    <row r="96" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>400</v>
       </c>
@@ -11066,7 +11287,7 @@
         <v>1199</v>
       </c>
     </row>
-    <row r="97" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>315</v>
       </c>
@@ -11122,69 +11343,76 @@
         <v>7</v>
       </c>
     </row>
-    <row r="98" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A98" t="s">
+    <row r="98" spans="1:25" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A98" s="13" t="s">
         <v>145</v>
       </c>
-      <c r="B98" t="s">
+      <c r="B98" s="13" t="s">
         <v>146</v>
       </c>
-      <c r="C98">
+      <c r="C98" s="13">
         <v>2002</v>
       </c>
-      <c r="D98" t="s">
+      <c r="D98" s="13" t="s">
         <v>564</v>
       </c>
-      <c r="E98" t="s">
+      <c r="E98" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="G98" t="s">
+      <c r="G98" s="13" t="s">
         <v>501</v>
       </c>
-      <c r="H98" t="s">
+      <c r="H98" s="13" t="s">
         <v>466</v>
       </c>
-      <c r="I98" t="s">
+      <c r="I98" s="13" t="s">
         <v>1207</v>
       </c>
-      <c r="J98" t="s">
+      <c r="J98" s="13" t="s">
         <v>462</v>
       </c>
-      <c r="K98" t="s">
+      <c r="K98" s="13" t="s">
         <v>511</v>
       </c>
-      <c r="L98" t="s">
+      <c r="L98" s="13" t="s">
         <v>509</v>
       </c>
-      <c r="M98" t="s">
+      <c r="M98" s="13" t="s">
         <v>511</v>
       </c>
-      <c r="O98" s="8" t="s">
+      <c r="N98"/>
+      <c r="O98" s="13" t="s">
         <v>1204</v>
       </c>
-      <c r="P98" t="s">
+      <c r="P98" s="13" t="s">
         <v>622</v>
       </c>
-      <c r="R98" t="s">
+      <c r="R98" s="13" t="s">
         <v>1203</v>
       </c>
-      <c r="S98" t="s">
+      <c r="S98" s="13" t="s">
         <v>1206</v>
       </c>
-      <c r="T98" s="10" t="s">
+      <c r="T98" s="13" t="s">
         <v>1558</v>
       </c>
-      <c r="U98" t="s">
+      <c r="U98" s="13" t="s">
         <v>1551</v>
       </c>
-      <c r="V98" t="s">
+      <c r="V98" s="13" t="s">
         <v>1208</v>
       </c>
-      <c r="W98" t="s">
+      <c r="W98" s="13" t="s">
         <v>1205</v>
       </c>
-    </row>
-    <row r="99" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X98" s="16" t="s">
+        <v>1582</v>
+      </c>
+      <c r="Y98" s="16" t="s">
+        <v>1568</v>
+      </c>
+    </row>
+    <row r="99" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>115</v>
       </c>
@@ -11240,7 +11468,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="100" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:25" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>236</v>
       </c>
@@ -11293,7 +11521,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="101" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>117</v>
       </c>
@@ -11352,7 +11580,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="102" spans="1:23" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:25" ht="409.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>318</v>
       </c>
@@ -11411,7 +11639,7 @@
         <v>1230</v>
       </c>
     </row>
-    <row r="103" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>74</v>
       </c>
@@ -11473,7 +11701,7 @@
         <v>696</v>
       </c>
     </row>
-    <row r="104" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>48</v>
       </c>
@@ -11529,7 +11757,7 @@
         <v>700</v>
       </c>
     </row>
-    <row r="105" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
         <v>119</v>
       </c>
@@ -11588,7 +11816,7 @@
         <v>1239</v>
       </c>
     </row>
-    <row r="106" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
         <v>50</v>
       </c>
@@ -11638,7 +11866,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="107" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
         <v>321</v>
       </c>
@@ -11694,7 +11922,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="108" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
         <v>52</v>
       </c>
@@ -11756,7 +11984,7 @@
         <v>1249</v>
       </c>
     </row>
-    <row r="109" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
         <v>121</v>
       </c>
@@ -11806,7 +12034,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="110" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:25" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
         <v>76</v>
       </c>
@@ -11862,7 +12090,7 @@
         <v>1254</v>
       </c>
     </row>
-    <row r="111" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
         <v>123</v>
       </c>
@@ -11915,7 +12143,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="112" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
         <v>403</v>
       </c>
@@ -11965,7 +12193,7 @@
         <v>1268</v>
       </c>
     </row>
-    <row r="113" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
         <v>78</v>
       </c>
@@ -12015,7 +12243,7 @@
         <v>1271</v>
       </c>
     </row>
-    <row r="114" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
         <v>324</v>
       </c>
@@ -12068,7 +12296,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="115" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
         <v>406</v>
       </c>
@@ -12118,104 +12346,118 @@
         <v>1279</v>
       </c>
     </row>
-    <row r="116" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A116" t="s">
+    <row r="116" spans="1:25" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A116" s="13" t="s">
         <v>239</v>
       </c>
-      <c r="B116" t="s">
+      <c r="B116" s="13" t="s">
         <v>240</v>
       </c>
-      <c r="C116">
+      <c r="C116" s="13">
         <v>2023</v>
       </c>
-      <c r="D116" t="s">
+      <c r="D116" s="13" t="s">
         <v>241</v>
       </c>
-      <c r="E116" t="s">
+      <c r="E116" s="13" t="s">
         <v>193</v>
       </c>
-      <c r="G116" t="s">
+      <c r="G116" s="13" t="s">
         <v>467</v>
       </c>
-      <c r="J116" t="s">
+      <c r="J116" s="13" t="s">
         <v>511</v>
       </c>
-      <c r="L116" t="s">
+      <c r="L116" s="13" t="s">
         <v>511</v>
       </c>
-      <c r="O116" s="8" t="s">
+      <c r="N116"/>
+      <c r="O116" s="13" t="s">
         <v>1283</v>
       </c>
-      <c r="P116" t="s">
+      <c r="P116" s="13" t="s">
         <v>770</v>
       </c>
-      <c r="S116" t="s">
+      <c r="S116" s="13" t="s">
         <v>1242</v>
       </c>
-      <c r="T116" s="10" t="s">
+      <c r="T116" s="13" t="s">
         <v>1560</v>
       </c>
-      <c r="U116" t="s">
+      <c r="U116" s="13" t="s">
         <v>1550</v>
       </c>
-      <c r="V116" t="s">
+      <c r="V116" s="13" t="s">
         <v>1284</v>
       </c>
-      <c r="W116" t="s">
+      <c r="W116" s="13" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="117" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A117" t="s">
+      <c r="X116" s="15" t="s">
+        <v>1583</v>
+      </c>
+      <c r="Y116" s="15" t="s">
+        <v>1568</v>
+      </c>
+    </row>
+    <row r="117" spans="1:25" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A117" s="17" t="s">
         <v>80</v>
       </c>
-      <c r="B117" t="s">
+      <c r="B117" s="17" t="s">
         <v>81</v>
       </c>
-      <c r="C117">
+      <c r="C117" s="17">
         <v>2022</v>
       </c>
-      <c r="D117" t="s">
+      <c r="D117" s="17" t="s">
         <v>575</v>
       </c>
-      <c r="E117" t="s">
+      <c r="E117" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="G117" t="s">
+      <c r="G117" s="17" t="s">
         <v>467</v>
       </c>
-      <c r="I117" t="s">
+      <c r="I117" s="17" t="s">
         <v>1287</v>
       </c>
-      <c r="J117" t="s">
+      <c r="J117" s="17" t="s">
         <v>511</v>
       </c>
-      <c r="L117" t="s">
+      <c r="L117" s="17" t="s">
         <v>511</v>
       </c>
-      <c r="O117" s="8" t="s">
+      <c r="N117"/>
+      <c r="O117" s="17" t="s">
         <v>1285</v>
       </c>
-      <c r="P117" t="s">
+      <c r="P117" s="17" t="s">
         <v>703</v>
       </c>
-      <c r="S117" t="s">
+      <c r="S117" s="17" t="s">
         <v>1286</v>
       </c>
-      <c r="T117" s="10" t="s">
+      <c r="T117" s="17" t="s">
         <v>1554</v>
       </c>
-      <c r="U117" t="s">
+      <c r="U117" s="17" t="s">
         <v>1550</v>
       </c>
-      <c r="V117" t="s">
+      <c r="V117" s="17" t="s">
         <v>1288</v>
       </c>
-      <c r="W117" t="s">
+      <c r="W117" s="17" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="118" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X117" s="22" t="s">
+        <v>1584</v>
+      </c>
+      <c r="Y117" s="22" t="s">
+        <v>1568</v>
+      </c>
+    </row>
+    <row r="118" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
         <v>327</v>
       </c>
@@ -12271,7 +12513,7 @@
         <v>1291</v>
       </c>
     </row>
-    <row r="119" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
         <v>409</v>
       </c>
@@ -12327,7 +12569,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="120" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
         <v>412</v>
       </c>
@@ -12386,7 +12628,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="121" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
         <v>415</v>
       </c>
@@ -12442,7 +12684,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="122" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
         <v>242</v>
       </c>
@@ -12495,7 +12737,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="123" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
         <v>54</v>
       </c>
@@ -12545,7 +12787,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="124" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
         <v>245</v>
       </c>
@@ -12592,7 +12834,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="125" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
         <v>330</v>
       </c>
@@ -12654,57 +12896,64 @@
         <v>710</v>
       </c>
     </row>
-    <row r="126" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A126" t="s">
+    <row r="126" spans="1:25" s="19" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A126" s="19" t="s">
         <v>160</v>
       </c>
-      <c r="B126" t="s">
+      <c r="B126" s="19" t="s">
         <v>161</v>
       </c>
-      <c r="C126">
+      <c r="C126" s="19">
         <v>2020</v>
       </c>
-      <c r="D126" t="s">
+      <c r="D126" s="19" t="s">
         <v>577</v>
       </c>
-      <c r="E126" t="s">
+      <c r="E126" s="19" t="s">
         <v>155</v>
       </c>
-      <c r="G126" t="s">
+      <c r="G126" s="19" t="s">
         <v>488</v>
       </c>
-      <c r="J126" t="s">
+      <c r="J126" s="19" t="s">
         <v>511</v>
       </c>
-      <c r="L126" t="s">
+      <c r="L126" s="19" t="s">
         <v>451</v>
       </c>
-      <c r="M126" t="s">
+      <c r="M126" s="19" t="s">
         <v>511</v>
       </c>
-      <c r="O126" s="8" t="s">
+      <c r="N126"/>
+      <c r="O126" s="19" t="s">
         <v>714</v>
       </c>
-      <c r="P126" t="s">
+      <c r="P126" s="19" t="s">
         <v>715</v>
       </c>
-      <c r="Q126" t="s">
+      <c r="Q126" s="19" t="s">
         <v>716</v>
       </c>
-      <c r="S126" t="s">
+      <c r="S126" s="19" t="s">
         <v>717</v>
       </c>
-      <c r="T126" s="10" t="s">
+      <c r="T126" s="19" t="s">
         <v>1553</v>
       </c>
-      <c r="U126" t="s">
+      <c r="U126" s="19" t="s">
         <v>1551</v>
       </c>
-      <c r="V126" t="s">
+      <c r="V126" s="19" t="s">
         <v>718</v>
       </c>
-    </row>
-    <row r="127" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X126" s="21" t="s">
+        <v>1585</v>
+      </c>
+      <c r="Y126" s="21" t="s">
+        <v>1586</v>
+      </c>
+    </row>
+    <row r="127" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
         <v>125</v>
       </c>
@@ -12757,7 +13006,7 @@
         <v>1324</v>
       </c>
     </row>
-    <row r="128" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
         <v>333</v>
       </c>
@@ -12822,7 +13071,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="129" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
         <v>127</v>
       </c>
@@ -12878,7 +13127,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="130" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
         <v>129</v>
       </c>
@@ -12931,7 +13180,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="131" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
         <v>418</v>
       </c>
@@ -12981,7 +13230,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="132" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
         <v>421</v>
       </c>
@@ -13037,7 +13286,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="133" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
         <v>131</v>
       </c>
@@ -13087,7 +13336,7 @@
         <v>1352</v>
       </c>
     </row>
-    <row r="134" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
         <v>248</v>
       </c>
@@ -13143,7 +13392,7 @@
         <v>1354</v>
       </c>
     </row>
-    <row r="135" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
         <v>424</v>
       </c>
@@ -13190,7 +13439,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="136" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
         <v>251</v>
       </c>
@@ -13249,7 +13498,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="137" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
         <v>56</v>
       </c>
@@ -13299,7 +13548,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="138" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
         <v>181</v>
       </c>
@@ -13361,7 +13610,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="139" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
         <v>427</v>
       </c>
@@ -13408,57 +13657,64 @@
         <v>7</v>
       </c>
     </row>
-    <row r="140" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A140" t="s">
+    <row r="140" spans="1:25" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A140" s="13" t="s">
         <v>254</v>
       </c>
-      <c r="B140" t="s">
+      <c r="B140" s="13" t="s">
         <v>255</v>
       </c>
-      <c r="C140">
+      <c r="C140" s="13">
         <v>2022</v>
       </c>
-      <c r="D140" t="s">
+      <c r="D140" s="13" t="s">
         <v>256</v>
       </c>
-      <c r="E140" t="s">
+      <c r="E140" s="13" t="s">
         <v>193</v>
       </c>
-      <c r="G140" t="s">
+      <c r="G140" s="13" t="s">
         <v>466</v>
       </c>
-      <c r="J140" t="s">
+      <c r="J140" s="13" t="s">
         <v>511</v>
       </c>
-      <c r="L140" t="s">
+      <c r="L140" s="13" t="s">
         <v>511</v>
       </c>
-      <c r="O140" s="8" t="s">
+      <c r="N140"/>
+      <c r="O140" s="13" t="s">
         <v>1380</v>
       </c>
-      <c r="P140" t="s">
+      <c r="P140" s="13" t="s">
         <v>703</v>
       </c>
-      <c r="R140" t="s">
+      <c r="R140" s="13" t="s">
         <v>41</v>
       </c>
-      <c r="S140" t="s">
+      <c r="S140" s="13" t="s">
         <v>777</v>
       </c>
-      <c r="T140" s="10" t="s">
+      <c r="T140" s="13" t="s">
         <v>1558</v>
       </c>
-      <c r="U140" t="s">
+      <c r="U140" s="13" t="s">
         <v>1551</v>
       </c>
-      <c r="V140" t="s">
+      <c r="V140" s="13" t="s">
         <v>1384</v>
       </c>
-      <c r="W140" t="s">
+      <c r="W140" s="13" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="141" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X140" s="16" t="s">
+        <v>1587</v>
+      </c>
+      <c r="Y140" s="16" t="s">
+        <v>1568</v>
+      </c>
+    </row>
+    <row r="141" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
         <v>336</v>
       </c>
@@ -13514,7 +13770,7 @@
         <v>1383</v>
       </c>
     </row>
-    <row r="142" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
         <v>257</v>
       </c>
@@ -13573,63 +13829,70 @@
         <v>7</v>
       </c>
     </row>
-    <row r="143" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A143" t="s">
+    <row r="143" spans="1:25" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A143" s="17" t="s">
         <v>339</v>
       </c>
-      <c r="B143" t="s">
+      <c r="B143" s="17" t="s">
         <v>340</v>
       </c>
-      <c r="C143">
+      <c r="C143" s="17">
         <v>2003</v>
       </c>
-      <c r="D143" t="s">
+      <c r="D143" s="17" t="s">
         <v>341</v>
       </c>
-      <c r="E143" t="s">
+      <c r="E143" s="17" t="s">
         <v>278</v>
       </c>
-      <c r="G143" t="s">
+      <c r="G143" s="17" t="s">
         <v>487</v>
       </c>
-      <c r="I143" t="s">
+      <c r="I143" s="17" t="s">
         <v>1398</v>
       </c>
-      <c r="J143" t="s">
+      <c r="J143" s="17" t="s">
         <v>457</v>
       </c>
-      <c r="L143" t="s">
+      <c r="L143" s="17" t="s">
         <v>457</v>
       </c>
-      <c r="M143" t="s">
+      <c r="M143" s="17" t="s">
         <v>451</v>
       </c>
-      <c r="O143" s="8" t="s">
+      <c r="N143"/>
+      <c r="O143" s="17" t="s">
         <v>1395</v>
       </c>
-      <c r="P143" t="s">
+      <c r="P143" s="17" t="s">
         <v>622</v>
       </c>
-      <c r="Q143" t="s">
+      <c r="Q143" s="17" t="s">
         <v>1397</v>
       </c>
-      <c r="S143" t="s">
+      <c r="S143" s="17" t="s">
         <v>1394</v>
       </c>
-      <c r="T143" s="10" t="s">
+      <c r="T143" s="17" t="s">
         <v>1558</v>
       </c>
-      <c r="U143" t="s">
+      <c r="U143" s="17" t="s">
         <v>1551</v>
       </c>
-      <c r="V143" t="s">
+      <c r="V143" s="17" t="s">
         <v>1399</v>
       </c>
-      <c r="W143" t="s">
+      <c r="W143" s="17" t="s">
         <v>1396</v>
       </c>
-    </row>
-    <row r="144" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X143" s="18" t="s">
+        <v>1588</v>
+      </c>
+      <c r="Y143" s="18" t="s">
+        <v>1589</v>
+      </c>
+    </row>
+    <row r="144" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
         <v>260</v>
       </c>
@@ -13685,7 +13948,7 @@
         <v>723</v>
       </c>
     </row>
-    <row r="145" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
         <v>184</v>
       </c>
@@ -13744,7 +14007,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="146" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
         <v>133</v>
       </c>
@@ -13800,125 +14063,139 @@
         <v>7</v>
       </c>
     </row>
-    <row r="147" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A147" t="s">
+    <row r="147" spans="1:25" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A147" s="13" t="s">
         <v>342</v>
       </c>
-      <c r="B147" t="s">
+      <c r="B147" s="13" t="s">
         <v>343</v>
       </c>
-      <c r="C147">
+      <c r="C147" s="13">
         <v>2020</v>
       </c>
-      <c r="D147" t="s">
+      <c r="D147" s="13" t="s">
         <v>344</v>
       </c>
-      <c r="E147" t="s">
+      <c r="E147" s="13" t="s">
         <v>278</v>
       </c>
-      <c r="G147" t="s">
+      <c r="G147" s="13" t="s">
         <v>484</v>
       </c>
-      <c r="H147" t="s">
+      <c r="H147" s="13" t="s">
         <v>474</v>
       </c>
-      <c r="I147" t="s">
+      <c r="I147" s="13" t="s">
         <v>1414</v>
       </c>
-      <c r="J147" t="s">
+      <c r="J147" s="13" t="s">
         <v>453</v>
       </c>
-      <c r="K147" t="s">
+      <c r="K147" s="13" t="s">
         <v>461</v>
       </c>
-      <c r="L147" t="s">
+      <c r="L147" s="13" t="s">
         <v>453</v>
       </c>
-      <c r="M147" t="s">
+      <c r="M147" s="13" t="s">
         <v>455</v>
       </c>
-      <c r="O147" s="8" t="s">
+      <c r="N147"/>
+      <c r="O147" s="13" t="s">
         <v>1412</v>
       </c>
-      <c r="P147" t="s">
+      <c r="P147" s="13" t="s">
         <v>875</v>
       </c>
-      <c r="Q147" t="s">
+      <c r="Q147" s="13" t="s">
         <v>1413</v>
       </c>
-      <c r="S147" t="s">
+      <c r="S147" s="13" t="s">
         <v>1415</v>
       </c>
-      <c r="T147" s="10" t="s">
+      <c r="T147" s="13" t="s">
         <v>1558</v>
       </c>
-      <c r="U147" t="s">
+      <c r="U147" s="13" t="s">
         <v>1551</v>
       </c>
-      <c r="V147" t="s">
+      <c r="V147" s="13" t="s">
         <v>1417</v>
       </c>
-      <c r="W147" t="s">
+      <c r="W147" s="13" t="s">
         <v>1416</v>
       </c>
-    </row>
-    <row r="148" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A148" t="s">
+      <c r="X147" s="16" t="s">
+        <v>1590</v>
+      </c>
+      <c r="Y147" s="16" t="s">
+        <v>1568</v>
+      </c>
+    </row>
+    <row r="148" spans="1:25" s="19" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A148" s="19" t="s">
         <v>58</v>
       </c>
-      <c r="B148" t="s">
+      <c r="B148" s="19" t="s">
         <v>59</v>
       </c>
-      <c r="C148">
+      <c r="C148" s="19">
         <v>2022</v>
       </c>
-      <c r="D148" t="s">
+      <c r="D148" s="19" t="s">
         <v>584</v>
       </c>
-      <c r="E148" t="s">
+      <c r="E148" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="G148" t="s">
+      <c r="G148" s="19" t="s">
         <v>466</v>
       </c>
-      <c r="I148" t="s">
+      <c r="I148" s="19" t="s">
         <v>1421</v>
       </c>
-      <c r="J148" t="s">
+      <c r="J148" s="19" t="s">
         <v>509</v>
       </c>
-      <c r="L148" t="s">
+      <c r="L148" s="19" t="s">
         <v>451</v>
       </c>
-      <c r="M148" t="s">
+      <c r="M148" s="19" t="s">
         <v>509</v>
       </c>
-      <c r="O148" s="8" t="s">
+      <c r="N148"/>
+      <c r="O148" s="19" t="s">
         <v>1418</v>
       </c>
-      <c r="P148" t="s">
+      <c r="P148" s="19" t="s">
         <v>613</v>
       </c>
-      <c r="R148" t="s">
+      <c r="R148" s="19" t="s">
         <v>1419</v>
       </c>
-      <c r="S148" t="s">
+      <c r="S148" s="19" t="s">
         <v>732</v>
       </c>
-      <c r="T148" s="10" t="s">
+      <c r="T148" s="19" t="s">
         <v>1561</v>
       </c>
-      <c r="U148" t="s">
+      <c r="U148" s="19" t="s">
         <v>1551</v>
       </c>
-      <c r="V148" t="s">
+      <c r="V148" s="19" t="s">
         <v>1420</v>
       </c>
-      <c r="W148" t="s">
+      <c r="W148" s="19" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="149" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X148" s="20" t="s">
+        <v>1591</v>
+      </c>
+      <c r="Y148" s="20" t="s">
+        <v>1580</v>
+      </c>
+    </row>
+    <row r="149" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
         <v>135</v>
       </c>
@@ -13971,7 +14248,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="150" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
         <v>345</v>
       </c>
@@ -14027,7 +14304,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="151" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
         <v>430</v>
       </c>
@@ -14083,7 +14360,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="152" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
         <v>60</v>
       </c>
@@ -14136,7 +14413,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="153" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
         <v>82</v>
       </c>
@@ -14198,66 +14475,73 @@
         <v>7</v>
       </c>
     </row>
-    <row r="154" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A154" t="s">
+    <row r="154" spans="1:25" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A154" s="13" t="s">
         <v>433</v>
       </c>
-      <c r="B154" t="s">
+      <c r="B154" s="13" t="s">
         <v>434</v>
       </c>
-      <c r="C154">
+      <c r="C154" s="13">
         <v>2018</v>
       </c>
-      <c r="D154" t="s">
+      <c r="D154" s="13" t="s">
         <v>435</v>
       </c>
-      <c r="E154" t="s">
+      <c r="E154" s="13" t="s">
         <v>351</v>
       </c>
-      <c r="G154" t="s">
+      <c r="G154" s="13" t="s">
         <v>474</v>
       </c>
-      <c r="J154" t="s">
+      <c r="J154" s="13" t="s">
         <v>511</v>
       </c>
-      <c r="K154" t="s">
+      <c r="K154" s="13" t="s">
         <v>509</v>
       </c>
-      <c r="L154" t="s">
+      <c r="L154" s="13" t="s">
         <v>511</v>
       </c>
-      <c r="M154" t="s">
+      <c r="M154" s="13" t="s">
         <v>451</v>
       </c>
-      <c r="O154" s="8" t="s">
+      <c r="N154"/>
+      <c r="O154" s="13" t="s">
         <v>1448</v>
       </c>
-      <c r="P154" t="s">
+      <c r="P154" s="13" t="s">
         <v>622</v>
       </c>
-      <c r="Q154" t="s">
+      <c r="Q154" s="13" t="s">
         <v>1449</v>
       </c>
-      <c r="R154" t="s">
+      <c r="R154" s="13" t="s">
         <v>1450</v>
       </c>
-      <c r="S154" t="s">
+      <c r="S154" s="13" t="s">
         <v>1451</v>
       </c>
-      <c r="T154" s="10" t="s">
+      <c r="T154" s="13" t="s">
         <v>1562</v>
       </c>
-      <c r="U154" t="s">
+      <c r="U154" s="13" t="s">
         <v>1549</v>
       </c>
-      <c r="V154" t="s">
+      <c r="V154" s="13" t="s">
         <v>1452</v>
       </c>
-      <c r="W154" t="s">
+      <c r="W154" s="13" t="s">
         <v>1453</v>
       </c>
-    </row>
-    <row r="155" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X154" s="16" t="s">
+        <v>1592</v>
+      </c>
+      <c r="Y154" s="16" t="s">
+        <v>1568</v>
+      </c>
+    </row>
+    <row r="155" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
         <v>62</v>
       </c>
@@ -14310,7 +14594,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="156" spans="1:23" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:25" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
         <v>348</v>
       </c>
@@ -14375,7 +14659,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="157" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
         <v>162</v>
       </c>
@@ -14431,7 +14715,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="158" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
         <v>436</v>
       </c>
@@ -14487,7 +14771,7 @@
         <v>1468</v>
       </c>
     </row>
-    <row r="159" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
         <v>64</v>
       </c>
@@ -14537,7 +14821,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="160" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
         <v>164</v>
       </c>
@@ -14587,7 +14871,7 @@
         <v>1476</v>
       </c>
     </row>
-    <row r="161" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
         <v>439</v>
       </c>
@@ -14646,60 +14930,67 @@
         <v>1485</v>
       </c>
     </row>
-    <row r="162" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A162" t="s">
+    <row r="162" spans="1:25" s="19" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A162" s="19" t="s">
         <v>263</v>
       </c>
-      <c r="B162" t="s">
+      <c r="B162" s="19" t="s">
         <v>264</v>
       </c>
-      <c r="C162">
+      <c r="C162" s="19">
         <v>2015</v>
       </c>
-      <c r="D162" t="s">
+      <c r="D162" s="19" t="s">
         <v>265</v>
       </c>
-      <c r="E162" t="s">
+      <c r="E162" s="19" t="s">
         <v>193</v>
       </c>
-      <c r="F162" t="s">
+      <c r="F162" s="19" t="s">
         <v>519</v>
       </c>
-      <c r="G162" t="s">
+      <c r="G162" s="19" t="s">
         <v>467</v>
       </c>
-      <c r="J162" t="s">
+      <c r="J162" s="19" t="s">
         <v>509</v>
       </c>
-      <c r="L162" t="s">
+      <c r="L162" s="19" t="s">
         <v>451</v>
       </c>
-      <c r="O162" s="8" t="s">
+      <c r="N162"/>
+      <c r="O162" s="19" t="s">
         <v>728</v>
       </c>
-      <c r="P162" t="s">
+      <c r="P162" s="19" t="s">
         <v>731</v>
       </c>
-      <c r="Q162" t="s">
+      <c r="Q162" s="19" t="s">
         <v>729</v>
       </c>
-      <c r="R162" t="s">
+      <c r="R162" s="19" t="s">
         <v>730</v>
       </c>
-      <c r="S162" t="s">
+      <c r="S162" s="19" t="s">
         <v>732</v>
       </c>
-      <c r="T162" s="10" t="s">
+      <c r="T162" s="19" t="s">
         <v>1555</v>
       </c>
-      <c r="U162" t="s">
+      <c r="U162" s="19" t="s">
         <v>1551</v>
       </c>
-      <c r="V162" t="s">
+      <c r="V162" s="19" t="s">
         <v>733</v>
       </c>
-    </row>
-    <row r="163" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X162" s="20" t="s">
+        <v>1593</v>
+      </c>
+      <c r="Y162" s="20" t="s">
+        <v>1580</v>
+      </c>
+    </row>
+    <row r="163" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
         <v>187</v>
       </c>
@@ -14764,7 +15055,7 @@
         <v>1493</v>
       </c>
     </row>
-    <row r="164" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
         <v>442</v>
       </c>
@@ -14817,7 +15108,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="165" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
         <v>66</v>
       </c>
@@ -14870,60 +15161,67 @@
         <v>7</v>
       </c>
     </row>
-    <row r="166" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A166" t="s">
+    <row r="166" spans="1:25" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A166" s="17" t="s">
         <v>137</v>
       </c>
-      <c r="B166" t="s">
+      <c r="B166" s="17" t="s">
         <v>138</v>
       </c>
-      <c r="C166">
+      <c r="C166" s="17">
         <v>2008</v>
       </c>
-      <c r="D166" t="s">
+      <c r="D166" s="17" t="s">
         <v>593</v>
       </c>
-      <c r="E166" t="s">
+      <c r="E166" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="G166" t="s">
+      <c r="G166" s="17" t="s">
         <v>465</v>
       </c>
-      <c r="J166" t="s">
+      <c r="J166" s="17" t="s">
         <v>457</v>
       </c>
-      <c r="L166" t="s">
+      <c r="L166" s="17" t="s">
         <v>457</v>
       </c>
-      <c r="O166" s="8" t="s">
+      <c r="N166"/>
+      <c r="O166" s="17" t="s">
         <v>1505</v>
       </c>
-      <c r="P166" t="s">
+      <c r="P166" s="17" t="s">
         <v>622</v>
       </c>
-      <c r="Q166" t="s">
+      <c r="Q166" s="17" t="s">
         <v>880</v>
       </c>
-      <c r="R166" t="s">
+      <c r="R166" s="17" t="s">
         <v>1506</v>
       </c>
-      <c r="S166" t="s">
+      <c r="S166" s="17" t="s">
         <v>1507</v>
       </c>
-      <c r="T166" s="10" t="s">
+      <c r="T166" s="17" t="s">
         <v>1554</v>
       </c>
-      <c r="U166" t="s">
+      <c r="U166" s="17" t="s">
         <v>1550</v>
       </c>
-      <c r="V166" t="s">
+      <c r="V166" s="17" t="s">
         <v>1508</v>
       </c>
-      <c r="W166" t="s">
+      <c r="W166" s="17" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="167" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X166" s="18" t="s">
+        <v>1594</v>
+      </c>
+      <c r="Y166" s="18" t="s">
+        <v>1580</v>
+      </c>
+    </row>
+    <row r="167" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
         <v>269</v>
       </c>
@@ -14985,7 +15283,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="168" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
         <v>139</v>
       </c>
@@ -15041,63 +15339,70 @@
         <v>7</v>
       </c>
     </row>
-    <row r="169" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A169" t="s">
+    <row r="169" spans="1:25" s="19" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A169" s="19" t="s">
         <v>272</v>
       </c>
-      <c r="B169" t="s">
+      <c r="B169" s="19" t="s">
         <v>273</v>
       </c>
-      <c r="C169">
+      <c r="C169" s="19">
         <v>2020</v>
       </c>
-      <c r="D169" t="s">
+      <c r="D169" s="19" t="s">
         <v>274</v>
       </c>
-      <c r="E169" t="s">
+      <c r="E169" s="19" t="s">
         <v>193</v>
       </c>
-      <c r="G169" t="s">
+      <c r="G169" s="19" t="s">
         <v>466</v>
       </c>
-      <c r="I169" t="s">
+      <c r="I169" s="19" t="s">
         <v>1519</v>
       </c>
-      <c r="J169" t="s">
+      <c r="J169" s="19" t="s">
         <v>509</v>
       </c>
-      <c r="L169" t="s">
+      <c r="L169" s="19" t="s">
         <v>451</v>
       </c>
-      <c r="O169" s="8" t="s">
+      <c r="N169"/>
+      <c r="O169" s="19" t="s">
         <v>1520</v>
       </c>
-      <c r="P169" t="s">
+      <c r="P169" s="19" t="s">
         <v>613</v>
       </c>
-      <c r="Q169" t="s">
+      <c r="Q169" s="19" t="s">
         <v>1522</v>
       </c>
-      <c r="R169" t="s">
+      <c r="R169" s="19" t="s">
         <v>1521</v>
       </c>
-      <c r="S169" t="s">
+      <c r="S169" s="19" t="s">
         <v>1523</v>
       </c>
-      <c r="T169" s="10" t="s">
+      <c r="T169" s="19" t="s">
         <v>1561</v>
       </c>
-      <c r="U169" t="s">
+      <c r="U169" s="19" t="s">
         <v>1551</v>
       </c>
-      <c r="V169" t="s">
+      <c r="V169" s="19" t="s">
         <v>1524</v>
       </c>
-      <c r="W169" t="s">
+      <c r="W169" s="19" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="170" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X169" s="20" t="s">
+        <v>1595</v>
+      </c>
+      <c r="Y169" s="20" t="s">
+        <v>1580</v>
+      </c>
+    </row>
+    <row r="170" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
         <v>166</v>
       </c>
@@ -15150,7 +15455,7 @@
         <v>1529</v>
       </c>
     </row>
-    <row r="171" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
         <v>141</v>
       </c>
@@ -15205,6 +15510,13 @@
     </row>
   </sheetData>
   <autoFilter ref="A1:W171">
+    <filterColumn colId="20">
+      <filters>
+        <filter val="instrumental;relational"/>
+        <filter val="relational"/>
+        <filter val="relational;instrumental"/>
+      </filters>
+    </filterColumn>
     <sortState ref="A2:V171">
       <sortCondition ref="B1:B171"/>
     </sortState>

</xml_diff>

<commit_message>
manuscript ready?  figures updated?  ready for cover letter then submission?
</commit_message>
<xml_diff>
--- a/_data/screened_fulltext/ft_consolidated_coding.xlsx
+++ b/_data/screened_fulltext/ft_consolidated_coding.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10824"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ohara/github/sp1_systematic_map/_data/screened_fulltext/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\casey\Documents\github\sp1_systematic_map\_data\screened_fulltext\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1EAFC8FC-15A0-4A4B-AEAB-DD82F39D0795}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-36840" yWindow="-900" windowWidth="31360" windowHeight="15100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-36840" yWindow="-900" windowWidth="31365" windowHeight="15105"/>
   </bookViews>
   <sheets>
     <sheet name="ft_consolidated_revisit" sheetId="1" r:id="rId1"/>
@@ -24,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3026" uniqueCount="1600">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3045" uniqueCount="1611">
   <si>
     <t>title</t>
   </si>
@@ -4826,14 +4825,47 @@
     <t xml:space="preserve">We are expanding beyond values related to the natural world.  I would argue that slavery is a (negative) relationship between an enslaved person and their oppressive society.  </t>
   </si>
   <si>
-    <t>agree in retrospect - the sentiments may be attached to relational values but these sentiments are not necessarily expressed directly, merely associated with words from interview transcripts…</t>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>Justice is beyond instrumental; is it not a relationship between individuals and society?  Scroter (2020): "We here refer to justice as fundamental moral rights and  obligations, while equity comparatively evaluates relationships, including access and control among different societal groups regarding NCP and nature. Distributive equity and justice concerns the sense of a fair allocation, among individuals, groups or stakeholders, of positive and negative NCP resulting from management decisions and resulting distributive effects on people’s good quality of life" - in this case, distribution of tree canopy is a fair allocation of positive NCP</t>
+  </si>
+  <si>
+    <t>ok, agree with Rachelle in retrospect - the sentiments may be attached to relational values but these sentiments are not necessarily expressed directly, merely associated with words from interview transcripts…</t>
+  </si>
+  <si>
+    <t>ok, recoded - if going by their definition, they are focusing on accuracy of targeting toward a hypothetical policy, which indicates more instrumental, even if that *policy* is intended to reduce poverty</t>
+  </si>
+  <si>
+    <t>in addition to instrumental outcomes, they also study fairness "In addition, we assess the fairness of ML-based targeting with respect to several different demographic subgroups." (though they found their ML ESI did NOT improve fairness, it is still a method to assess a potential benefit!)</t>
+  </si>
+  <si>
+    <t>they may not measure the relational value, but they definitely link their outcome to it: "Evidence from several randomized control trials shows that this method of charity has large positive effects on multiple measures of recipients’ well-being.4"</t>
+  </si>
+  <si>
+    <t>manual add</t>
+  </si>
+  <si>
+    <t>Valuing Satellite Data for Harmful Algal Bloom Early Warning Systems</t>
+  </si>
+  <si>
+    <t>Newbold, Lindley, Albeke, Viers, Johnston</t>
+  </si>
+  <si>
+    <t>added per Yusuke recommendation Aug 2025</t>
+  </si>
+  <si>
+    <t>HAB warning system based on satellite imagery</t>
+  </si>
+  <si>
+    <t>newbold_valuingsatellitedataharmful_2022</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="23">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="23" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -5738,39 +5770,40 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <sheetPr filterMode="1"/>
-  <dimension ref="A1:Z171"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:Z172"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="P5" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="D151" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="Z126" sqref="Z126"/>
+      <selection pane="bottomRight" activeCell="D172" sqref="D172"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="25.5" customWidth="1"/>
-    <col min="2" max="2" width="9.83203125" customWidth="1"/>
-    <col min="3" max="4" width="9.1640625" customWidth="1"/>
-    <col min="5" max="5" width="7.33203125" customWidth="1"/>
-    <col min="6" max="6" width="9.1640625" customWidth="1"/>
-    <col min="7" max="7" width="17.83203125" customWidth="1"/>
-    <col min="8" max="8" width="20.5" customWidth="1"/>
-    <col min="9" max="9" width="18.83203125" customWidth="1"/>
-    <col min="10" max="13" width="6.5" customWidth="1"/>
-    <col min="14" max="14" width="12.33203125" hidden="1" customWidth="1"/>
-    <col min="15" max="15" width="12.33203125" style="7" customWidth="1"/>
-    <col min="16" max="20" width="12.33203125" customWidth="1"/>
-    <col min="21" max="21" width="13.5" customWidth="1"/>
-    <col min="22" max="22" width="12.33203125" customWidth="1"/>
-    <col min="23" max="23" width="16.1640625" customWidth="1"/>
-    <col min="24" max="24" width="28.5" customWidth="1"/>
-    <col min="25" max="25" width="16.5" customWidth="1"/>
+    <col min="1" max="1" width="25.42578125" customWidth="1"/>
+    <col min="2" max="2" width="9.85546875" customWidth="1"/>
+    <col min="3" max="4" width="9.140625" customWidth="1"/>
+    <col min="5" max="5" width="7.28515625" customWidth="1"/>
+    <col min="6" max="6" width="9.140625" customWidth="1"/>
+    <col min="7" max="7" width="17.85546875" customWidth="1"/>
+    <col min="8" max="8" width="20.42578125" customWidth="1"/>
+    <col min="9" max="9" width="18.85546875" hidden="1" customWidth="1"/>
+    <col min="10" max="13" width="6.42578125" customWidth="1"/>
+    <col min="14" max="14" width="12.28515625" hidden="1" customWidth="1"/>
+    <col min="15" max="15" width="12.28515625" style="7" hidden="1" customWidth="1"/>
+    <col min="16" max="18" width="12.28515625" hidden="1" customWidth="1"/>
+    <col min="19" max="20" width="12.28515625" customWidth="1"/>
+    <col min="21" max="21" width="13.42578125" customWidth="1"/>
+    <col min="22" max="22" width="12.28515625" hidden="1" customWidth="1"/>
+    <col min="23" max="23" width="16.140625" hidden="1" customWidth="1"/>
+    <col min="24" max="24" width="28.42578125" hidden="1" customWidth="1"/>
+    <col min="25" max="25" width="16.42578125" hidden="1" customWidth="1"/>
+    <col min="26" max="26" width="0" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" s="5" customFormat="1" ht="45.75" customHeight="1">
+    <row r="1" spans="1:26" s="5" customFormat="1" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -5850,7 +5883,7 @@
         <v>1596</v>
       </c>
     </row>
-    <row r="2" spans="1:26" hidden="1">
+    <row r="2" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>266</v>
       </c>
@@ -5909,7 +5942,7 @@
         <v>737</v>
       </c>
     </row>
-    <row r="3" spans="1:26" hidden="1">
+    <row r="3" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>86</v>
       </c>
@@ -5968,7 +6001,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:26" hidden="1">
+    <row r="4" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>84</v>
       </c>
@@ -6027,7 +6060,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:26" s="9" customFormat="1">
+    <row r="5" spans="1:26" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="9" t="s">
         <v>168</v>
       </c>
@@ -6095,7 +6128,7 @@
         <v>1568</v>
       </c>
     </row>
-    <row r="6" spans="1:26" hidden="1">
+    <row r="6" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>88</v>
       </c>
@@ -6151,7 +6184,7 @@
         <v>757</v>
       </c>
     </row>
-    <row r="7" spans="1:26" s="13" customFormat="1">
+    <row r="7" spans="1:26" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="13" t="s">
         <v>190</v>
       </c>
@@ -6217,7 +6250,7 @@
         <v>1597</v>
       </c>
     </row>
-    <row r="8" spans="1:26" hidden="1">
+    <row r="8" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>352</v>
       </c>
@@ -6279,7 +6312,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:26" hidden="1">
+    <row r="9" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>91</v>
       </c>
@@ -6338,7 +6371,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:26" hidden="1">
+    <row r="10" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>194</v>
       </c>
@@ -6403,7 +6436,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="11" spans="1:26" hidden="1">
+    <row r="11" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>355</v>
       </c>
@@ -6456,7 +6489,7 @@
         <v>786</v>
       </c>
     </row>
-    <row r="12" spans="1:26" hidden="1">
+    <row r="12" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>5</v>
       </c>
@@ -6512,7 +6545,7 @@
         <v>794</v>
       </c>
     </row>
-    <row r="13" spans="1:26" hidden="1">
+    <row r="13" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>358</v>
       </c>
@@ -6568,7 +6601,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="14" spans="1:26" hidden="1">
+    <row r="14" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>200</v>
       </c>
@@ -6636,7 +6669,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="15" spans="1:26" hidden="1">
+    <row r="15" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>197</v>
       </c>
@@ -6698,7 +6731,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="16" spans="1:26" hidden="1">
+    <row r="16" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>11</v>
       </c>
@@ -6754,7 +6787,7 @@
         <v>809</v>
       </c>
     </row>
-    <row r="17" spans="1:26" hidden="1">
+    <row r="17" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>9</v>
       </c>
@@ -6810,7 +6843,7 @@
         <v>806</v>
       </c>
     </row>
-    <row r="18" spans="1:26" hidden="1">
+    <row r="18" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>13</v>
       </c>
@@ -6866,7 +6899,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="19" spans="1:26" hidden="1">
+    <row r="19" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>93</v>
       </c>
@@ -6925,7 +6958,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="20" spans="1:26" hidden="1">
+    <row r="20" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>151</v>
       </c>
@@ -6981,7 +7014,7 @@
         <v>828</v>
       </c>
     </row>
-    <row r="21" spans="1:26" hidden="1">
+    <row r="21" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>361</v>
       </c>
@@ -7037,7 +7070,7 @@
         <v>832</v>
       </c>
     </row>
-    <row r="22" spans="1:26" hidden="1">
+    <row r="22" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>172</v>
       </c>
@@ -7096,7 +7129,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="23" spans="1:26" hidden="1">
+    <row r="23" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>275</v>
       </c>
@@ -7155,7 +7188,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="24" spans="1:26" hidden="1">
+    <row r="24" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>279</v>
       </c>
@@ -7208,7 +7241,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="25" spans="1:26" hidden="1">
+    <row r="25" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>15</v>
       </c>
@@ -7273,7 +7306,7 @@
         <v>854</v>
       </c>
     </row>
-    <row r="26" spans="1:26" hidden="1">
+    <row r="26" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>17</v>
       </c>
@@ -7341,7 +7374,7 @@
         <v>642</v>
       </c>
     </row>
-    <row r="27" spans="1:26" hidden="1">
+    <row r="27" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>19</v>
       </c>
@@ -7400,7 +7433,7 @@
         <v>864</v>
       </c>
     </row>
-    <row r="28" spans="1:26" hidden="1">
+    <row r="28" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>21</v>
       </c>
@@ -7459,7 +7492,7 @@
         <v>866</v>
       </c>
     </row>
-    <row r="29" spans="1:26" hidden="1">
+    <row r="29" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>282</v>
       </c>
@@ -7512,7 +7545,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="30" spans="1:26" s="15" customFormat="1">
+    <row r="30" spans="1:26" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A30" s="15" t="s">
         <v>364</v>
       </c>
@@ -7578,7 +7611,7 @@
         <v>1598</v>
       </c>
     </row>
-    <row r="31" spans="1:26" hidden="1">
+    <row r="31" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>23</v>
       </c>
@@ -7631,7 +7664,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="32" spans="1:26" hidden="1">
+    <row r="32" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>285</v>
       </c>
@@ -7687,7 +7720,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="33" spans="1:25" hidden="1">
+    <row r="33" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>95</v>
       </c>
@@ -7746,7 +7779,7 @@
         <v>893</v>
       </c>
     </row>
-    <row r="34" spans="1:25" hidden="1">
+    <row r="34" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>288</v>
       </c>
@@ -7802,7 +7835,7 @@
         <v>646</v>
       </c>
     </row>
-    <row r="35" spans="1:25" hidden="1">
+    <row r="35" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>97</v>
       </c>
@@ -7858,7 +7891,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="36" spans="1:25" hidden="1">
+    <row r="36" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>25</v>
       </c>
@@ -7911,7 +7944,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="37" spans="1:25" s="9" customFormat="1">
+    <row r="37" spans="1:25" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A37" s="9" t="s">
         <v>291</v>
       </c>
@@ -7973,7 +8006,7 @@
         <v>1574</v>
       </c>
     </row>
-    <row r="38" spans="1:25" hidden="1">
+    <row r="38" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>99</v>
       </c>
@@ -8032,7 +8065,7 @@
         <v>921</v>
       </c>
     </row>
-    <row r="39" spans="1:25" hidden="1">
+    <row r="39" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>203</v>
       </c>
@@ -8088,7 +8121,7 @@
         <v>925</v>
       </c>
     </row>
-    <row r="40" spans="1:25" hidden="1">
+    <row r="40" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>367</v>
       </c>
@@ -8144,7 +8177,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="41" spans="1:25" s="9" customFormat="1">
+    <row r="41" spans="1:25" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A41" s="9" t="s">
         <v>370</v>
       </c>
@@ -8216,7 +8249,7 @@
         <v>1576</v>
       </c>
     </row>
-    <row r="42" spans="1:25" hidden="1">
+    <row r="42" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>294</v>
       </c>
@@ -8272,7 +8305,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="43" spans="1:25" hidden="1">
+    <row r="43" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>29</v>
       </c>
@@ -8328,7 +8361,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="44" spans="1:25" hidden="1">
+    <row r="44" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>27</v>
       </c>
@@ -8381,7 +8414,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="45" spans="1:25" hidden="1">
+    <row r="45" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>101</v>
       </c>
@@ -8443,7 +8476,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="46" spans="1:25" hidden="1">
+    <row r="46" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>31</v>
       </c>
@@ -8502,7 +8535,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="47" spans="1:25" hidden="1">
+    <row r="47" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>33</v>
       </c>
@@ -8561,7 +8594,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="48" spans="1:25" hidden="1">
+    <row r="48" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>103</v>
       </c>
@@ -8617,7 +8650,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="49" spans="1:26" hidden="1">
+    <row r="49" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>373</v>
       </c>
@@ -8676,7 +8709,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="50" spans="1:26" hidden="1">
+    <row r="50" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>105</v>
       </c>
@@ -8735,7 +8768,7 @@
         <v>982</v>
       </c>
     </row>
-    <row r="51" spans="1:26" s="13" customFormat="1">
+    <row r="51" spans="1:26" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A51" s="13" t="s">
         <v>297</v>
       </c>
@@ -8801,10 +8834,10 @@
         <v>1570</v>
       </c>
       <c r="Z51" s="13" t="s">
-        <v>1599</v>
-      </c>
-    </row>
-    <row r="52" spans="1:26" hidden="1">
+        <v>1601</v>
+      </c>
+    </row>
+    <row r="52" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>35</v>
       </c>
@@ -8860,7 +8893,7 @@
         <v>993</v>
       </c>
     </row>
-    <row r="53" spans="1:26" hidden="1">
+    <row r="53" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>206</v>
       </c>
@@ -8907,7 +8940,7 @@
         <v>997</v>
       </c>
     </row>
-    <row r="54" spans="1:26" hidden="1">
+    <row r="54" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>156</v>
       </c>
@@ -8960,7 +8993,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="55" spans="1:26" s="9" customFormat="1">
+    <row r="55" spans="1:26" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A55" s="9" t="s">
         <v>175</v>
       </c>
@@ -9026,7 +9059,7 @@
         <v>1568</v>
       </c>
     </row>
-    <row r="56" spans="1:26" hidden="1">
+    <row r="56" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>209</v>
       </c>
@@ -9079,7 +9112,7 @@
         <v>1018</v>
       </c>
     </row>
-    <row r="57" spans="1:26" hidden="1">
+    <row r="57" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>212</v>
       </c>
@@ -9132,7 +9165,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="58" spans="1:26" hidden="1">
+    <row r="58" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>376</v>
       </c>
@@ -9188,7 +9221,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="59" spans="1:26" hidden="1">
+    <row r="59" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>379</v>
       </c>
@@ -9247,7 +9280,7 @@
         <v>1031</v>
       </c>
     </row>
-    <row r="60" spans="1:26" hidden="1">
+    <row r="60" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>300</v>
       </c>
@@ -9300,7 +9333,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="61" spans="1:26" hidden="1">
+    <row r="61" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>68</v>
       </c>
@@ -9362,7 +9395,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="62" spans="1:26" hidden="1">
+    <row r="62" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>303</v>
       </c>
@@ -9424,7 +9457,7 @@
         <v>1047</v>
       </c>
     </row>
-    <row r="63" spans="1:26" s="15" customFormat="1">
+    <row r="63" spans="1:26" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A63" s="15" t="s">
         <v>178</v>
       </c>
@@ -9492,8 +9525,11 @@
       <c r="Y63" s="16" t="s">
         <v>1580</v>
       </c>
-    </row>
-    <row r="64" spans="1:26" hidden="1">
+      <c r="Z63" s="15" t="s">
+        <v>1600</v>
+      </c>
+    </row>
+    <row r="64" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>37</v>
       </c>
@@ -9537,7 +9573,7 @@
         <v>627</v>
       </c>
     </row>
-    <row r="65" spans="1:25" hidden="1">
+    <row r="65" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>215</v>
       </c>
@@ -9590,7 +9626,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="66" spans="1:25" hidden="1">
+    <row r="66" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>153</v>
       </c>
@@ -9652,7 +9688,7 @@
         <v>663</v>
       </c>
     </row>
-    <row r="67" spans="1:25" s="9" customFormat="1">
+    <row r="67" spans="1:25" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A67" s="9" t="s">
         <v>382</v>
       </c>
@@ -9721,7 +9757,7 @@
         <v>1568</v>
       </c>
     </row>
-    <row r="68" spans="1:25" hidden="1">
+    <row r="68" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>107</v>
       </c>
@@ -9777,7 +9813,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="69" spans="1:25" hidden="1">
+    <row r="69" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>385</v>
       </c>
@@ -9833,7 +9869,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="70" spans="1:25" hidden="1">
+    <row r="70" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>109</v>
       </c>
@@ -9889,7 +9925,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="71" spans="1:25" hidden="1">
+    <row r="71" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>149</v>
       </c>
@@ -9945,7 +9981,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="72" spans="1:25" hidden="1">
+    <row r="72" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>39</v>
       </c>
@@ -9998,7 +10034,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="73" spans="1:25" hidden="1">
+    <row r="73" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>388</v>
       </c>
@@ -10051,7 +10087,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="74" spans="1:25" hidden="1">
+    <row r="74" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>143</v>
       </c>
@@ -10107,7 +10143,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="75" spans="1:25" hidden="1">
+    <row r="75" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>218</v>
       </c>
@@ -10163,7 +10199,7 @@
         <v>1103</v>
       </c>
     </row>
-    <row r="76" spans="1:25" hidden="1">
+    <row r="76" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>391</v>
       </c>
@@ -10219,7 +10255,7 @@
         <v>1106</v>
       </c>
     </row>
-    <row r="77" spans="1:25" hidden="1">
+    <row r="77" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>42</v>
       </c>
@@ -10272,7 +10308,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="78" spans="1:25" hidden="1">
+    <row r="78" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>394</v>
       </c>
@@ -10325,7 +10361,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="79" spans="1:25" hidden="1">
+    <row r="79" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>306</v>
       </c>
@@ -10375,7 +10411,7 @@
         <v>1124</v>
       </c>
     </row>
-    <row r="80" spans="1:25" hidden="1">
+    <row r="80" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>158</v>
       </c>
@@ -10434,7 +10470,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="81" spans="1:23" hidden="1">
+    <row r="81" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>221</v>
       </c>
@@ -10487,7 +10523,7 @@
         <v>1132</v>
       </c>
     </row>
-    <row r="82" spans="1:23" ht="409.6" hidden="1">
+    <row r="82" spans="1:23" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>309</v>
       </c>
@@ -10546,7 +10582,7 @@
         <v>1139</v>
       </c>
     </row>
-    <row r="83" spans="1:23" hidden="1">
+    <row r="83" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>224</v>
       </c>
@@ -10602,7 +10638,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="84" spans="1:23" hidden="1">
+    <row r="84" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>111</v>
       </c>
@@ -10655,7 +10691,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="85" spans="1:23" hidden="1">
+    <row r="85" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>147</v>
       </c>
@@ -10708,7 +10744,7 @@
         <v>1156</v>
       </c>
     </row>
-    <row r="86" spans="1:23" hidden="1">
+    <row r="86" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>70</v>
       </c>
@@ -10761,7 +10797,7 @@
         <v>1160</v>
       </c>
     </row>
-    <row r="87" spans="1:23" hidden="1">
+    <row r="87" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>227</v>
       </c>
@@ -10817,7 +10853,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="88" spans="1:23" hidden="1">
+    <row r="88" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>397</v>
       </c>
@@ -10870,7 +10906,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="89" spans="1:23" ht="409.6" hidden="1">
+    <row r="89" spans="1:23" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>44</v>
       </c>
@@ -10926,7 +10962,7 @@
         <v>1172</v>
       </c>
     </row>
-    <row r="90" spans="1:23" hidden="1">
+    <row r="90" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>46</v>
       </c>
@@ -10979,7 +11015,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="91" spans="1:23" hidden="1">
+    <row r="91" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>230</v>
       </c>
@@ -11032,7 +11068,7 @@
         <v>1180</v>
       </c>
     </row>
-    <row r="92" spans="1:23" hidden="1">
+    <row r="92" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>113</v>
       </c>
@@ -11085,7 +11121,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="93" spans="1:23" hidden="1">
+    <row r="93" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>72</v>
       </c>
@@ -11138,7 +11174,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="94" spans="1:23" ht="15" hidden="1" customHeight="1">
+    <row r="94" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>312</v>
       </c>
@@ -11197,7 +11233,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="95" spans="1:23" hidden="1">
+    <row r="95" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>233</v>
       </c>
@@ -11250,7 +11286,7 @@
         <v>1194</v>
       </c>
     </row>
-    <row r="96" spans="1:23" hidden="1">
+    <row r="96" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>400</v>
       </c>
@@ -11306,7 +11342,7 @@
         <v>1199</v>
       </c>
     </row>
-    <row r="97" spans="1:25" hidden="1">
+    <row r="97" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>315</v>
       </c>
@@ -11362,7 +11398,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="98" spans="1:25" s="9" customFormat="1">
+    <row r="98" spans="1:25" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A98" s="9" t="s">
         <v>145</v>
       </c>
@@ -11431,7 +11467,7 @@
         <v>1568</v>
       </c>
     </row>
-    <row r="99" spans="1:25" hidden="1">
+    <row r="99" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>115</v>
       </c>
@@ -11487,7 +11523,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="100" spans="1:25" ht="15" hidden="1" customHeight="1">
+    <row r="100" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>236</v>
       </c>
@@ -11540,7 +11576,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="101" spans="1:25" hidden="1">
+    <row r="101" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>117</v>
       </c>
@@ -11599,7 +11635,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="102" spans="1:25" ht="409.6" hidden="1">
+    <row r="102" spans="1:25" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>318</v>
       </c>
@@ -11658,7 +11694,7 @@
         <v>1230</v>
       </c>
     </row>
-    <row r="103" spans="1:25" hidden="1">
+    <row r="103" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>74</v>
       </c>
@@ -11720,7 +11756,7 @@
         <v>696</v>
       </c>
     </row>
-    <row r="104" spans="1:25" hidden="1">
+    <row r="104" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>48</v>
       </c>
@@ -11776,7 +11812,7 @@
         <v>700</v>
       </c>
     </row>
-    <row r="105" spans="1:25" hidden="1">
+    <row r="105" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
         <v>119</v>
       </c>
@@ -11835,7 +11871,7 @@
         <v>1239</v>
       </c>
     </row>
-    <row r="106" spans="1:25" hidden="1">
+    <row r="106" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
         <v>50</v>
       </c>
@@ -11885,7 +11921,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="107" spans="1:25" hidden="1">
+    <row r="107" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
         <v>321</v>
       </c>
@@ -11941,7 +11977,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="108" spans="1:25" hidden="1">
+    <row r="108" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
         <v>52</v>
       </c>
@@ -12003,7 +12039,7 @@
         <v>1249</v>
       </c>
     </row>
-    <row r="109" spans="1:25" hidden="1">
+    <row r="109" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
         <v>121</v>
       </c>
@@ -12053,7 +12089,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="110" spans="1:25" ht="15" hidden="1" customHeight="1">
+    <row r="110" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
         <v>76</v>
       </c>
@@ -12109,7 +12145,7 @@
         <v>1254</v>
       </c>
     </row>
-    <row r="111" spans="1:25" hidden="1">
+    <row r="111" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
         <v>123</v>
       </c>
@@ -12162,7 +12198,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="112" spans="1:25" hidden="1">
+    <row r="112" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
         <v>403</v>
       </c>
@@ -12212,7 +12248,7 @@
         <v>1268</v>
       </c>
     </row>
-    <row r="113" spans="1:25" hidden="1">
+    <row r="113" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
         <v>78</v>
       </c>
@@ -12262,7 +12298,7 @@
         <v>1271</v>
       </c>
     </row>
-    <row r="114" spans="1:25" hidden="1">
+    <row r="114" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
         <v>324</v>
       </c>
@@ -12315,7 +12351,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="115" spans="1:25" hidden="1">
+    <row r="115" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
         <v>406</v>
       </c>
@@ -12365,7 +12401,7 @@
         <v>1279</v>
       </c>
     </row>
-    <row r="116" spans="1:25" s="9" customFormat="1">
+    <row r="116" spans="1:26" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A116" s="9" t="s">
         <v>239</v>
       </c>
@@ -12419,7 +12455,7 @@
         <v>1568</v>
       </c>
     </row>
-    <row r="117" spans="1:25" s="13" customFormat="1">
+    <row r="117" spans="1:26" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A117" s="13" t="s">
         <v>80</v>
       </c>
@@ -12476,7 +12512,7 @@
         <v>1568</v>
       </c>
     </row>
-    <row r="118" spans="1:25" hidden="1">
+    <row r="118" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
         <v>327</v>
       </c>
@@ -12532,7 +12568,7 @@
         <v>1291</v>
       </c>
     </row>
-    <row r="119" spans="1:25" hidden="1">
+    <row r="119" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
         <v>409</v>
       </c>
@@ -12588,7 +12624,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="120" spans="1:25" hidden="1">
+    <row r="120" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
         <v>412</v>
       </c>
@@ -12647,7 +12683,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="121" spans="1:25" hidden="1">
+    <row r="121" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
         <v>415</v>
       </c>
@@ -12703,7 +12739,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="122" spans="1:25" hidden="1">
+    <row r="122" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
         <v>242</v>
       </c>
@@ -12756,7 +12792,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="123" spans="1:25" hidden="1">
+    <row r="123" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
         <v>54</v>
       </c>
@@ -12806,7 +12842,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="124" spans="1:25" hidden="1">
+    <row r="124" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
         <v>245</v>
       </c>
@@ -12853,7 +12889,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="125" spans="1:25" hidden="1">
+    <row r="125" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
         <v>330</v>
       </c>
@@ -12915,7 +12951,7 @@
         <v>710</v>
       </c>
     </row>
-    <row r="126" spans="1:25" s="15" customFormat="1">
+    <row r="126" spans="1:26" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A126" s="15" t="s">
         <v>160</v>
       </c>
@@ -12971,8 +13007,11 @@
       <c r="Y126" s="17" t="s">
         <v>1586</v>
       </c>
-    </row>
-    <row r="127" spans="1:25" hidden="1">
+      <c r="Z126" s="15" t="s">
+        <v>1599</v>
+      </c>
+    </row>
+    <row r="127" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
         <v>125</v>
       </c>
@@ -13025,7 +13064,7 @@
         <v>1324</v>
       </c>
     </row>
-    <row r="128" spans="1:25" hidden="1">
+    <row r="128" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
         <v>333</v>
       </c>
@@ -13090,7 +13129,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="129" spans="1:25" hidden="1">
+    <row r="129" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
         <v>127</v>
       </c>
@@ -13146,7 +13185,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="130" spans="1:25" hidden="1">
+    <row r="130" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
         <v>129</v>
       </c>
@@ -13199,7 +13238,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="131" spans="1:25" hidden="1">
+    <row r="131" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
         <v>418</v>
       </c>
@@ -13249,7 +13288,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="132" spans="1:25" hidden="1">
+    <row r="132" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
         <v>421</v>
       </c>
@@ -13305,7 +13344,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="133" spans="1:25" hidden="1">
+    <row r="133" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
         <v>131</v>
       </c>
@@ -13355,7 +13394,7 @@
         <v>1352</v>
       </c>
     </row>
-    <row r="134" spans="1:25" hidden="1">
+    <row r="134" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
         <v>248</v>
       </c>
@@ -13411,7 +13450,7 @@
         <v>1354</v>
       </c>
     </row>
-    <row r="135" spans="1:25" hidden="1">
+    <row r="135" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
         <v>424</v>
       </c>
@@ -13458,7 +13497,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="136" spans="1:25" hidden="1">
+    <row r="136" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
         <v>251</v>
       </c>
@@ -13517,7 +13556,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="137" spans="1:25" hidden="1">
+    <row r="137" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
         <v>56</v>
       </c>
@@ -13567,7 +13606,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="138" spans="1:25" hidden="1">
+    <row r="138" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
         <v>181</v>
       </c>
@@ -13629,7 +13668,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="139" spans="1:25" hidden="1">
+    <row r="139" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
         <v>427</v>
       </c>
@@ -13676,7 +13715,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="140" spans="1:25" s="9" customFormat="1">
+    <row r="140" spans="1:25" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A140" s="9" t="s">
         <v>254</v>
       </c>
@@ -13733,7 +13772,7 @@
         <v>1568</v>
       </c>
     </row>
-    <row r="141" spans="1:25" hidden="1">
+    <row r="141" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
         <v>336</v>
       </c>
@@ -13789,7 +13828,7 @@
         <v>1383</v>
       </c>
     </row>
-    <row r="142" spans="1:25" hidden="1">
+    <row r="142" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
         <v>257</v>
       </c>
@@ -13848,7 +13887,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="143" spans="1:25" s="13" customFormat="1">
+    <row r="143" spans="1:25" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A143" s="13" t="s">
         <v>339</v>
       </c>
@@ -13911,7 +13950,7 @@
         <v>1589</v>
       </c>
     </row>
-    <row r="144" spans="1:25" hidden="1">
+    <row r="144" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
         <v>260</v>
       </c>
@@ -13967,7 +14006,7 @@
         <v>723</v>
       </c>
     </row>
-    <row r="145" spans="1:25" hidden="1">
+    <row r="145" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
         <v>184</v>
       </c>
@@ -14026,7 +14065,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="146" spans="1:25" hidden="1">
+    <row r="146" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
         <v>133</v>
       </c>
@@ -14082,7 +14121,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="147" spans="1:25" s="9" customFormat="1">
+    <row r="147" spans="1:26" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A147" s="9" t="s">
         <v>342</v>
       </c>
@@ -14151,7 +14190,7 @@
         <v>1568</v>
       </c>
     </row>
-    <row r="148" spans="1:25" s="15" customFormat="1">
+    <row r="148" spans="1:26" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A148" s="15" t="s">
         <v>58</v>
       </c>
@@ -14213,8 +14252,11 @@
       <c r="Y148" s="16" t="s">
         <v>1580</v>
       </c>
-    </row>
-    <row r="149" spans="1:25" hidden="1">
+      <c r="Z148" s="15" t="s">
+        <v>1603</v>
+      </c>
+    </row>
+    <row r="149" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
         <v>135</v>
       </c>
@@ -14267,7 +14309,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="150" spans="1:25" hidden="1">
+    <row r="150" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
         <v>345</v>
       </c>
@@ -14323,7 +14365,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="151" spans="1:25" hidden="1">
+    <row r="151" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
         <v>430</v>
       </c>
@@ -14379,7 +14421,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="152" spans="1:25" hidden="1">
+    <row r="152" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
         <v>60</v>
       </c>
@@ -14432,7 +14474,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="153" spans="1:25" hidden="1">
+    <row r="153" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
         <v>82</v>
       </c>
@@ -14451,6 +14493,9 @@
       <c r="G153" t="s">
         <v>466</v>
       </c>
+      <c r="H153" t="s">
+        <v>470</v>
+      </c>
       <c r="I153" t="s">
         <v>1447</v>
       </c>
@@ -14494,7 +14539,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="154" spans="1:25" s="9" customFormat="1">
+    <row r="154" spans="1:26" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A154" s="9" t="s">
         <v>433</v>
       </c>
@@ -14560,7 +14605,7 @@
         <v>1568</v>
       </c>
     </row>
-    <row r="155" spans="1:25" hidden="1">
+    <row r="155" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
         <v>62</v>
       </c>
@@ -14613,7 +14658,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="156" spans="1:25" hidden="1">
+    <row r="156" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
         <v>348</v>
       </c>
@@ -14675,7 +14720,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="157" spans="1:25" hidden="1">
+    <row r="157" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
         <v>162</v>
       </c>
@@ -14731,7 +14776,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="158" spans="1:25" hidden="1">
+    <row r="158" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
         <v>436</v>
       </c>
@@ -14787,7 +14832,7 @@
         <v>1468</v>
       </c>
     </row>
-    <row r="159" spans="1:25" hidden="1">
+    <row r="159" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
         <v>64</v>
       </c>
@@ -14837,7 +14882,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="160" spans="1:25" hidden="1">
+    <row r="160" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
         <v>164</v>
       </c>
@@ -14887,7 +14932,7 @@
         <v>1476</v>
       </c>
     </row>
-    <row r="161" spans="1:25" hidden="1">
+    <row r="161" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
         <v>439</v>
       </c>
@@ -14946,7 +14991,7 @@
         <v>1485</v>
       </c>
     </row>
-    <row r="162" spans="1:25" s="15" customFormat="1">
+    <row r="162" spans="1:26" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A162" s="15" t="s">
         <v>263</v>
       </c>
@@ -15005,8 +15050,11 @@
       <c r="Y162" s="16" t="s">
         <v>1580</v>
       </c>
-    </row>
-    <row r="163" spans="1:25" hidden="1">
+      <c r="Z162" s="15" t="s">
+        <v>1604</v>
+      </c>
+    </row>
+    <row r="163" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
         <v>187</v>
       </c>
@@ -15071,7 +15119,7 @@
         <v>1493</v>
       </c>
     </row>
-    <row r="164" spans="1:25" hidden="1">
+    <row r="164" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
         <v>442</v>
       </c>
@@ -15124,7 +15172,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="165" spans="1:25" hidden="1">
+    <row r="165" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
         <v>66</v>
       </c>
@@ -15177,7 +15225,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="166" spans="1:25" s="13" customFormat="1">
+    <row r="166" spans="1:26" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A166" s="13" t="s">
         <v>137</v>
       </c>
@@ -15219,10 +15267,10 @@
         <v>1507</v>
       </c>
       <c r="T166" s="13" t="s">
-        <v>1554</v>
+        <v>627</v>
       </c>
       <c r="U166" s="13" t="s">
-        <v>1550</v>
+        <v>627</v>
       </c>
       <c r="V166" s="13" t="s">
         <v>1508</v>
@@ -15236,8 +15284,11 @@
       <c r="Y166" s="14" t="s">
         <v>1580</v>
       </c>
-    </row>
-    <row r="167" spans="1:25" hidden="1">
+      <c r="Z166" s="13" t="s">
+        <v>1597</v>
+      </c>
+    </row>
+    <row r="167" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
         <v>269</v>
       </c>
@@ -15299,7 +15350,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="168" spans="1:25" hidden="1">
+    <row r="168" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
         <v>139</v>
       </c>
@@ -15355,7 +15406,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="169" spans="1:25" s="15" customFormat="1">
+    <row r="169" spans="1:26" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A169" s="15" t="s">
         <v>272</v>
       </c>
@@ -15400,10 +15451,10 @@
         <v>1523</v>
       </c>
       <c r="T169" s="15" t="s">
-        <v>1561</v>
+        <v>627</v>
       </c>
       <c r="U169" s="15" t="s">
-        <v>1551</v>
+        <v>627</v>
       </c>
       <c r="V169" s="15" t="s">
         <v>1524</v>
@@ -15417,8 +15468,11 @@
       <c r="Y169" s="16" t="s">
         <v>1580</v>
       </c>
-    </row>
-    <row r="170" spans="1:25" hidden="1">
+      <c r="Z169" s="15" t="s">
+        <v>1602</v>
+      </c>
+    </row>
+    <row r="170" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
         <v>166</v>
       </c>
@@ -15471,7 +15525,7 @@
         <v>1529</v>
       </c>
     </row>
-    <row r="171" spans="1:25" hidden="1">
+    <row r="171" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
         <v>141</v>
       </c>
@@ -15524,20 +15578,54 @@
         <v>7</v>
       </c>
     </row>
+    <row r="172" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A172" t="s">
+        <v>1606</v>
+      </c>
+      <c r="B172" t="s">
+        <v>1607</v>
+      </c>
+      <c r="C172">
+        <v>2022</v>
+      </c>
+      <c r="D172" t="s">
+        <v>1610</v>
+      </c>
+      <c r="E172" t="s">
+        <v>1605</v>
+      </c>
+      <c r="F172" t="s">
+        <v>1608</v>
+      </c>
+      <c r="G172" t="s">
+        <v>466</v>
+      </c>
+      <c r="H172" t="s">
+        <v>502</v>
+      </c>
+      <c r="J172" t="s">
+        <v>461</v>
+      </c>
+      <c r="L172" t="s">
+        <v>455</v>
+      </c>
+      <c r="S172" t="s">
+        <v>1609</v>
+      </c>
+      <c r="T172" t="s">
+        <v>627</v>
+      </c>
+      <c r="U172" t="s">
+        <v>627</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:W171" xr:uid="{00000000-0009-0000-0000-000000000000}">
-    <filterColumn colId="20">
-      <filters>
-        <filter val="instrumental;relational"/>
-        <filter val="relational"/>
-        <filter val="relational;instrumental"/>
-      </filters>
-    </filterColumn>
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:V171">
+  <autoFilter ref="A1:W171">
+    <sortState ref="A2:V171">
       <sortCondition ref="B1:B171"/>
     </sortState>
   </autoFilter>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:Q209">
+  <sortState ref="A2:Q209">
     <sortCondition ref="B1"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -15545,19 +15633,19 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="3">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000000000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>lists!$E$2:$E$31</xm:f>
           </x14:formula1>
           <xm:sqref>G2:H171</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000001000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>lists!$B$2:$B$11</xm:f>
           </x14:formula1>
           <xm:sqref>L2:M171</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000002000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>lists!$A$2:$A$12</xm:f>
           </x14:formula1>
@@ -15570,24 +15658,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="18.5" defaultRowHeight="12"/>
+  <sheetFormatPr defaultColWidth="18.42578125" defaultRowHeight="12" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="14" style="1" customWidth="1"/>
-    <col min="2" max="2" width="22.83203125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="18.5" style="1"/>
-    <col min="4" max="4" width="30.5" style="1" customWidth="1"/>
-    <col min="5" max="5" width="28.1640625" style="1" customWidth="1"/>
-    <col min="6" max="16384" width="18.5" style="1"/>
+    <col min="2" max="2" width="22.85546875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="18.42578125" style="1"/>
+    <col min="4" max="4" width="30.42578125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="28.140625" style="1" customWidth="1"/>
+    <col min="6" max="16384" width="18.42578125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>493</v>
       </c>
@@ -15601,7 +15689,7 @@
         <v>449</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="13">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>453</v>
       </c>
@@ -15615,7 +15703,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="13">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>458</v>
       </c>
@@ -15627,7 +15715,7 @@
         <v>466</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="13">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>459</v>
       </c>
@@ -15639,7 +15727,7 @@
         <v>467</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="13">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>460</v>
       </c>
@@ -15651,7 +15739,7 @@
         <v>468</v>
       </c>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>461</v>
       </c>
@@ -15662,7 +15750,7 @@
         <v>507</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="13">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>462</v>
       </c>
@@ -15676,7 +15764,7 @@
         <v>469</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="13">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>463</v>
       </c>
@@ -15688,7 +15776,7 @@
         <v>470</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="13">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>457</v>
       </c>
@@ -15700,7 +15788,7 @@
         <v>501</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="13">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>464</v>
       </c>
@@ -15712,7 +15800,7 @@
         <v>502</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="13">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>509</v>
       </c>
@@ -15724,7 +15812,7 @@
         <v>471</v>
       </c>
     </row>
-    <row r="12" spans="1:5" ht="13">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>511</v>
       </c>
@@ -15735,13 +15823,13 @@
         <v>472</v>
       </c>
     </row>
-    <row r="13" spans="1:5" ht="13">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="D13" s="3"/>
       <c r="E13" s="3" t="s">
         <v>473</v>
       </c>
     </row>
-    <row r="14" spans="1:5" ht="13">
+    <row r="14" spans="1:5" ht="24" x14ac:dyDescent="0.2">
       <c r="D14" s="3" t="s">
         <v>497</v>
       </c>
@@ -15749,25 +15837,25 @@
         <v>474</v>
       </c>
     </row>
-    <row r="15" spans="1:5" ht="13">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="D15" s="3"/>
       <c r="E15" s="3" t="s">
         <v>475</v>
       </c>
     </row>
-    <row r="16" spans="1:5" ht="13">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="D16" s="3"/>
       <c r="E16" s="3" t="s">
         <v>476</v>
       </c>
     </row>
-    <row r="17" spans="4:5" ht="13">
+    <row r="17" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D17" s="3"/>
       <c r="E17" s="3" t="s">
         <v>477</v>
       </c>
     </row>
-    <row r="18" spans="4:5" ht="13">
+    <row r="18" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D18" s="3" t="s">
         <v>498</v>
       </c>
@@ -15775,13 +15863,13 @@
         <v>478</v>
       </c>
     </row>
-    <row r="19" spans="4:5" ht="13">
+    <row r="19" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D19" s="3"/>
       <c r="E19" s="3" t="s">
         <v>479</v>
       </c>
     </row>
-    <row r="20" spans="4:5" ht="13">
+    <row r="20" spans="4:5" ht="24" x14ac:dyDescent="0.2">
       <c r="D20" s="3" t="s">
         <v>499</v>
       </c>
@@ -15789,31 +15877,31 @@
         <v>480</v>
       </c>
     </row>
-    <row r="21" spans="4:5" ht="13">
+    <row r="21" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D21" s="3"/>
       <c r="E21" s="3" t="s">
         <v>481</v>
       </c>
     </row>
-    <row r="22" spans="4:5" ht="13">
+    <row r="22" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D22" s="3"/>
       <c r="E22" s="3" t="s">
         <v>482</v>
       </c>
     </row>
-    <row r="23" spans="4:5" ht="13">
+    <row r="23" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D23" s="3"/>
       <c r="E23" s="3" t="s">
         <v>483</v>
       </c>
     </row>
-    <row r="24" spans="4:5" ht="13">
+    <row r="24" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D24" s="3"/>
       <c r="E24" s="3" t="s">
         <v>484</v>
       </c>
     </row>
-    <row r="25" spans="4:5" ht="13">
+    <row r="25" spans="4:5" ht="24" x14ac:dyDescent="0.2">
       <c r="D25" s="3" t="s">
         <v>500</v>
       </c>
@@ -15821,37 +15909,37 @@
         <v>485</v>
       </c>
     </row>
-    <row r="26" spans="4:5" ht="13">
+    <row r="26" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D26" s="3"/>
       <c r="E26" s="3" t="s">
         <v>486</v>
       </c>
     </row>
-    <row r="27" spans="4:5" ht="13">
+    <row r="27" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D27" s="3"/>
       <c r="E27" s="3" t="s">
         <v>487</v>
       </c>
     </row>
-    <row r="28" spans="4:5" ht="26">
+    <row r="28" spans="4:5" ht="24" x14ac:dyDescent="0.2">
       <c r="D28" s="3"/>
       <c r="E28" s="3" t="s">
         <v>488</v>
       </c>
     </row>
-    <row r="29" spans="4:5" ht="13">
+    <row r="29" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D29" s="3"/>
       <c r="E29" s="3" t="s">
         <v>489</v>
       </c>
     </row>
-    <row r="30" spans="4:5" ht="13">
+    <row r="30" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D30" s="3"/>
       <c r="E30" s="3" t="s">
         <v>490</v>
       </c>
     </row>
-    <row r="31" spans="4:5" ht="13">
+    <row r="31" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D31" s="3"/>
       <c r="E31" s="3" t="s">
         <v>491</v>

</xml_diff>

<commit_message>
final updates for initial submission
</commit_message>
<xml_diff>
--- a/_data/screened_fulltext/ft_consolidated_coding.xlsx
+++ b/_data/screened_fulltext/ft_consolidated_coding.xlsx
@@ -16,7 +16,7 @@
     <sheet name="lists" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">ft_consolidated_revisit!$A$1:$W$171</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">ft_consolidated_revisit!$A$1:$W$172</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
 </workbook>
@@ -5771,13 +5771,14 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:Z172"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="D151" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="D116" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D172" sqref="D172"/>
+      <selection pane="bottomRight" activeCell="A77" sqref="A77"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5791,16 +5792,15 @@
     <col min="8" max="8" width="20.42578125" customWidth="1"/>
     <col min="9" max="9" width="18.85546875" hidden="1" customWidth="1"/>
     <col min="10" max="13" width="6.42578125" customWidth="1"/>
-    <col min="14" max="14" width="12.28515625" hidden="1" customWidth="1"/>
-    <col min="15" max="15" width="12.28515625" style="7" hidden="1" customWidth="1"/>
-    <col min="16" max="18" width="12.28515625" hidden="1" customWidth="1"/>
-    <col min="19" max="20" width="12.28515625" customWidth="1"/>
+    <col min="14" max="14" width="12.28515625" customWidth="1"/>
+    <col min="15" max="15" width="12.28515625" style="7" customWidth="1"/>
+    <col min="16" max="20" width="12.28515625" customWidth="1"/>
     <col min="21" max="21" width="13.42578125" customWidth="1"/>
-    <col min="22" max="22" width="12.28515625" hidden="1" customWidth="1"/>
-    <col min="23" max="23" width="16.140625" hidden="1" customWidth="1"/>
-    <col min="24" max="24" width="28.42578125" hidden="1" customWidth="1"/>
-    <col min="25" max="25" width="16.42578125" hidden="1" customWidth="1"/>
-    <col min="26" max="26" width="0" hidden="1" customWidth="1"/>
+    <col min="22" max="22" width="12.28515625" customWidth="1"/>
+    <col min="23" max="23" width="16.140625" customWidth="1"/>
+    <col min="24" max="24" width="28.42578125" customWidth="1"/>
+    <col min="25" max="25" width="16.42578125" customWidth="1"/>
+    <col min="26" max="26" width="8.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" s="5" customFormat="1" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -5942,7 +5942,7 @@
         <v>737</v>
       </c>
     </row>
-    <row r="3" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:26" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>86</v>
       </c>
@@ -6001,7 +6001,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:26" hidden="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>84</v>
       </c>
@@ -6128,7 +6128,7 @@
         <v>1568</v>
       </c>
     </row>
-    <row r="6" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:26" hidden="1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>88</v>
       </c>
@@ -6184,7 +6184,7 @@
         <v>757</v>
       </c>
     </row>
-    <row r="7" spans="1:26" s="13" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:26" s="13" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A7" s="13" t="s">
         <v>190</v>
       </c>
@@ -6312,7 +6312,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:26" hidden="1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>91</v>
       </c>
@@ -6436,7 +6436,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="11" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:26" hidden="1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>355</v>
       </c>
@@ -6545,7 +6545,7 @@
         <v>794</v>
       </c>
     </row>
-    <row r="13" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:26" hidden="1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>358</v>
       </c>
@@ -6601,7 +6601,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="14" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:26" hidden="1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>200</v>
       </c>
@@ -6669,7 +6669,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="15" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:26" hidden="1" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>197</v>
       </c>
@@ -6731,7 +6731,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="16" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:26" hidden="1" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>11</v>
       </c>
@@ -6787,7 +6787,7 @@
         <v>809</v>
       </c>
     </row>
-    <row r="17" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:26" hidden="1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>9</v>
       </c>
@@ -6899,7 +6899,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="19" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:26" hidden="1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>93</v>
       </c>
@@ -6958,7 +6958,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="20" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:26" hidden="1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>151</v>
       </c>
@@ -7070,7 +7070,7 @@
         <v>832</v>
       </c>
     </row>
-    <row r="22" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:26" hidden="1" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>172</v>
       </c>
@@ -7241,7 +7241,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="25" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:26" hidden="1" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>15</v>
       </c>
@@ -7306,7 +7306,7 @@
         <v>854</v>
       </c>
     </row>
-    <row r="26" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:26" hidden="1" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>17</v>
       </c>
@@ -7374,7 +7374,7 @@
         <v>642</v>
       </c>
     </row>
-    <row r="27" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:26" hidden="1" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>19</v>
       </c>
@@ -7433,7 +7433,7 @@
         <v>864</v>
       </c>
     </row>
-    <row r="28" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:26" hidden="1" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>21</v>
       </c>
@@ -7492,7 +7492,7 @@
         <v>866</v>
       </c>
     </row>
-    <row r="29" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:26" hidden="1" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>282</v>
       </c>
@@ -7611,7 +7611,7 @@
         <v>1598</v>
       </c>
     </row>
-    <row r="31" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:26" hidden="1" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>23</v>
       </c>
@@ -7664,7 +7664,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="32" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:26" hidden="1" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>285</v>
       </c>
@@ -7720,7 +7720,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="33" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>95</v>
       </c>
@@ -7835,7 +7835,7 @@
         <v>646</v>
       </c>
     </row>
-    <row r="35" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>97</v>
       </c>
@@ -8006,7 +8006,7 @@
         <v>1574</v>
       </c>
     </row>
-    <row r="38" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>99</v>
       </c>
@@ -8065,7 +8065,7 @@
         <v>921</v>
       </c>
     </row>
-    <row r="39" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>203</v>
       </c>
@@ -8121,7 +8121,7 @@
         <v>925</v>
       </c>
     </row>
-    <row r="40" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>367</v>
       </c>
@@ -8249,7 +8249,7 @@
         <v>1576</v>
       </c>
     </row>
-    <row r="42" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>294</v>
       </c>
@@ -8361,7 +8361,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="44" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>27</v>
       </c>
@@ -8414,7 +8414,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="45" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>101</v>
       </c>
@@ -8476,7 +8476,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="46" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>31</v>
       </c>
@@ -8535,7 +8535,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="47" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>33</v>
       </c>
@@ -8650,7 +8650,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="49" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:26" hidden="1" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>373</v>
       </c>
@@ -8709,7 +8709,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="50" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:26" hidden="1" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>105</v>
       </c>
@@ -8893,7 +8893,7 @@
         <v>993</v>
       </c>
     </row>
-    <row r="53" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:26" hidden="1" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>206</v>
       </c>
@@ -8940,7 +8940,7 @@
         <v>997</v>
       </c>
     </row>
-    <row r="54" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:26" hidden="1" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>156</v>
       </c>
@@ -9059,7 +9059,7 @@
         <v>1568</v>
       </c>
     </row>
-    <row r="56" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:26" hidden="1" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>209</v>
       </c>
@@ -9112,7 +9112,7 @@
         <v>1018</v>
       </c>
     </row>
-    <row r="57" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:26" hidden="1" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>212</v>
       </c>
@@ -9165,7 +9165,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="58" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:26" hidden="1" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>376</v>
       </c>
@@ -9280,7 +9280,7 @@
         <v>1031</v>
       </c>
     </row>
-    <row r="60" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:26" hidden="1" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>300</v>
       </c>
@@ -9333,7 +9333,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="61" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:26" hidden="1" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>68</v>
       </c>
@@ -9529,7 +9529,7 @@
         <v>1600</v>
       </c>
     </row>
-    <row r="64" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:26" hidden="1" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>37</v>
       </c>
@@ -9573,7 +9573,7 @@
         <v>627</v>
       </c>
     </row>
-    <row r="65" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>215</v>
       </c>
@@ -9626,7 +9626,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="66" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>153</v>
       </c>
@@ -9757,7 +9757,7 @@
         <v>1568</v>
       </c>
     </row>
-    <row r="68" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>107</v>
       </c>
@@ -9869,7 +9869,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="70" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>109</v>
       </c>
@@ -9925,7 +9925,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="71" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>149</v>
       </c>
@@ -9981,7 +9981,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="72" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>39</v>
       </c>
@@ -10087,7 +10087,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="74" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>143</v>
       </c>
@@ -10308,7 +10308,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="78" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>394</v>
       </c>
@@ -10361,7 +10361,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="79" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>306</v>
       </c>
@@ -10411,7 +10411,7 @@
         <v>1124</v>
       </c>
     </row>
-    <row r="80" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>158</v>
       </c>
@@ -10582,7 +10582,7 @@
         <v>1139</v>
       </c>
     </row>
-    <row r="83" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>224</v>
       </c>
@@ -10638,7 +10638,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="84" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>111</v>
       </c>
@@ -10691,7 +10691,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="85" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>147</v>
       </c>
@@ -10744,7 +10744,7 @@
         <v>1156</v>
       </c>
     </row>
-    <row r="86" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>70</v>
       </c>
@@ -10797,7 +10797,7 @@
         <v>1160</v>
       </c>
     </row>
-    <row r="87" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>227</v>
       </c>
@@ -10853,7 +10853,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="88" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>397</v>
       </c>
@@ -10906,7 +10906,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="89" spans="1:23" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:23" ht="409.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>44</v>
       </c>
@@ -10962,7 +10962,7 @@
         <v>1172</v>
       </c>
     </row>
-    <row r="90" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>46</v>
       </c>
@@ -11068,7 +11068,7 @@
         <v>1180</v>
       </c>
     </row>
-    <row r="92" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>113</v>
       </c>
@@ -11174,7 +11174,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="94" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:23" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>312</v>
       </c>
@@ -11233,7 +11233,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="95" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>233</v>
       </c>
@@ -11286,7 +11286,7 @@
         <v>1194</v>
       </c>
     </row>
-    <row r="96" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:23" hidden="1" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>400</v>
       </c>
@@ -11398,7 +11398,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="98" spans="1:25" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:25" s="9" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A98" s="9" t="s">
         <v>145</v>
       </c>
@@ -11467,7 +11467,7 @@
         <v>1568</v>
       </c>
     </row>
-    <row r="99" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>115</v>
       </c>
@@ -11523,7 +11523,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="100" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:25" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>236</v>
       </c>
@@ -11576,7 +11576,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="101" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>117</v>
       </c>
@@ -11694,7 +11694,7 @@
         <v>1230</v>
       </c>
     </row>
-    <row r="103" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>74</v>
       </c>
@@ -11756,7 +11756,7 @@
         <v>696</v>
       </c>
     </row>
-    <row r="104" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>48</v>
       </c>
@@ -11812,7 +11812,7 @@
         <v>700</v>
       </c>
     </row>
-    <row r="105" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
         <v>119</v>
       </c>
@@ -11871,7 +11871,7 @@
         <v>1239</v>
       </c>
     </row>
-    <row r="106" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
         <v>50</v>
       </c>
@@ -11921,7 +11921,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="107" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
         <v>321</v>
       </c>
@@ -11977,7 +11977,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="108" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
         <v>52</v>
       </c>
@@ -12039,7 +12039,7 @@
         <v>1249</v>
       </c>
     </row>
-    <row r="109" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
         <v>121</v>
       </c>
@@ -12089,7 +12089,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="110" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:25" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
         <v>76</v>
       </c>
@@ -12145,7 +12145,7 @@
         <v>1254</v>
       </c>
     </row>
-    <row r="111" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
         <v>123</v>
       </c>
@@ -12198,7 +12198,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="112" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
         <v>403</v>
       </c>
@@ -12298,7 +12298,7 @@
         <v>1271</v>
       </c>
     </row>
-    <row r="114" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:26" hidden="1" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
         <v>324</v>
       </c>
@@ -12351,7 +12351,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="115" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:26" hidden="1" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
         <v>406</v>
       </c>
@@ -12512,7 +12512,7 @@
         <v>1568</v>
       </c>
     </row>
-    <row r="118" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:26" hidden="1" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
         <v>327</v>
       </c>
@@ -12739,7 +12739,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="122" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:26" hidden="1" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
         <v>242</v>
       </c>
@@ -12842,7 +12842,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="124" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:26" hidden="1" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
         <v>245</v>
       </c>
@@ -13011,7 +13011,7 @@
         <v>1599</v>
       </c>
     </row>
-    <row r="127" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:26" hidden="1" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
         <v>125</v>
       </c>
@@ -13064,7 +13064,7 @@
         <v>1324</v>
       </c>
     </row>
-    <row r="128" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:26" hidden="1" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
         <v>333</v>
       </c>
@@ -13129,7 +13129,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="129" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
         <v>127</v>
       </c>
@@ -13185,7 +13185,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="130" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
         <v>129</v>
       </c>
@@ -13238,7 +13238,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="131" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
         <v>418</v>
       </c>
@@ -13344,7 +13344,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="133" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
         <v>131</v>
       </c>
@@ -13394,7 +13394,7 @@
         <v>1352</v>
       </c>
     </row>
-    <row r="134" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
         <v>248</v>
       </c>
@@ -13450,7 +13450,7 @@
         <v>1354</v>
       </c>
     </row>
-    <row r="135" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
         <v>424</v>
       </c>
@@ -13497,7 +13497,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="136" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
         <v>251</v>
       </c>
@@ -13556,7 +13556,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="137" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
         <v>56</v>
       </c>
@@ -13668,7 +13668,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="139" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
         <v>427</v>
       </c>
@@ -13828,7 +13828,7 @@
         <v>1383</v>
       </c>
     </row>
-    <row r="142" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
         <v>257</v>
       </c>
@@ -13887,7 +13887,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="143" spans="1:25" s="13" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:25" s="13" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A143" s="13" t="s">
         <v>339</v>
       </c>
@@ -13950,7 +13950,7 @@
         <v>1589</v>
       </c>
     </row>
-    <row r="144" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:25" hidden="1" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
         <v>260</v>
       </c>
@@ -14006,7 +14006,7 @@
         <v>723</v>
       </c>
     </row>
-    <row r="145" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:26" hidden="1" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
         <v>184</v>
       </c>
@@ -14065,7 +14065,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="146" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:26" hidden="1" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
         <v>133</v>
       </c>
@@ -14256,7 +14256,7 @@
         <v>1603</v>
       </c>
     </row>
-    <row r="149" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:26" hidden="1" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
         <v>135</v>
       </c>
@@ -14421,7 +14421,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="152" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:26" hidden="1" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
         <v>60</v>
       </c>
@@ -14539,7 +14539,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="154" spans="1:26" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:26" s="9" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A154" s="9" t="s">
         <v>433</v>
       </c>
@@ -14605,7 +14605,7 @@
         <v>1568</v>
       </c>
     </row>
-    <row r="155" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:26" hidden="1" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
         <v>62</v>
       </c>
@@ -14882,7 +14882,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="160" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:26" hidden="1" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
         <v>164</v>
       </c>
@@ -14932,7 +14932,7 @@
         <v>1476</v>
       </c>
     </row>
-    <row r="161" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:26" hidden="1" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
         <v>439</v>
       </c>
@@ -14991,7 +14991,7 @@
         <v>1485</v>
       </c>
     </row>
-    <row r="162" spans="1:26" s="15" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:26" s="15" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A162" s="15" t="s">
         <v>263</v>
       </c>
@@ -15054,7 +15054,7 @@
         <v>1604</v>
       </c>
     </row>
-    <row r="163" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:26" hidden="1" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
         <v>187</v>
       </c>
@@ -15172,7 +15172,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="165" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:26" hidden="1" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
         <v>66</v>
       </c>
@@ -15225,7 +15225,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="166" spans="1:26" s="13" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:26" s="13" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A166" s="13" t="s">
         <v>137</v>
       </c>
@@ -15288,7 +15288,7 @@
         <v>1597</v>
       </c>
     </row>
-    <row r="167" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:26" hidden="1" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
         <v>269</v>
       </c>
@@ -15350,7 +15350,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="168" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:26" hidden="1" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
         <v>139</v>
       </c>
@@ -15472,7 +15472,7 @@
         <v>1602</v>
       </c>
     </row>
-    <row r="170" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:26" hidden="1" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
         <v>166</v>
       </c>
@@ -15525,7 +15525,7 @@
         <v>1529</v>
       </c>
     </row>
-    <row r="171" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:26" hidden="1" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
         <v>141</v>
       </c>
@@ -15620,7 +15620,16 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:W171">
+  <autoFilter ref="A1:W172">
+    <filterColumn colId="2">
+      <filters>
+        <filter val="2019"/>
+        <filter val="2020"/>
+        <filter val="2021"/>
+        <filter val="2022"/>
+        <filter val="2023"/>
+      </filters>
+    </filterColumn>
     <sortState ref="A2:V171">
       <sortCondition ref="B1:B171"/>
     </sortState>

</xml_diff>